<commit_message>
running LSTM testing in parallel
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -25,9 +25,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t xml:space="preserve">window</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5, epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 500, batch size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing error </t>
+  </si>
+  <si>
+    <t xml:space="preserve">model fit time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 315.67 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training predict time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.57503 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing predict time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.080213 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training error eval time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.374 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testing error eval time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.098262 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compilation time </t>
   </si>
   <si>
     <t xml:space="preserve">epoch</t>
@@ -40,21 +85,6 @@
   </si>
   <si>
     <t xml:space="preserve">testing error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">model fit time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">training predict time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing predict time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">training error eval time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testing error eval time</t>
   </si>
   <si>
     <t xml:space="preserve">45</t>
@@ -82,9 +112,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -355,8 +386,12 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -364,7 +399,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6246,17 +6281,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>7.46179651998731E-005</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0.0407150174913511</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>316.879235744476</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6275,7 +6389,7 @@
   <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A253" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F297" activeCellId="0" sqref="F297"/>
+      <selection pane="topLeft" activeCell="D288" activeCellId="0" sqref="D288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6297,31 +6411,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16117,382 +16231,382 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="n">
+      <c r="C6" s="10"/>
+      <c r="D6" s="9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="9" t="n">
+        <v>250</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8" t="n">
-        <v>50</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8" t="n">
+      <c r="B8" s="17" t="n">
+        <v>3.58752902898499E-005</v>
+      </c>
+      <c r="C8" s="18" t="n">
+        <v>0.0130635215976293</v>
+      </c>
+      <c r="D8" s="19" t="n">
+        <v>1.82873157512579E-005</v>
+      </c>
+      <c r="E8" s="19" t="n">
+        <v>0.0276028922670915</v>
+      </c>
+      <c r="F8" s="17" t="n">
+        <v>5.92699062422513E-005</v>
+      </c>
+      <c r="G8" s="18" t="n">
+        <v>0.0105684386648203</v>
+      </c>
+      <c r="H8" s="19" t="n">
+        <v>7.21152814966765E-005</v>
+      </c>
+      <c r="I8" s="19" t="n">
+        <v>0.0390139155874581</v>
+      </c>
+      <c r="J8" s="17" t="n">
+        <v>0.000394138629702215</v>
+      </c>
+      <c r="K8" s="18" t="n">
+        <v>0.117094792603027</v>
+      </c>
+      <c r="L8" s="20" t="n">
+        <v>0.00011593728469645</v>
+      </c>
+      <c r="M8" s="21" t="n">
+        <v>0.0414687121440053</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="n">
         <v>100</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8" t="n">
+      <c r="B9" s="23" t="n">
+        <v>3.2691016816007E-006</v>
+      </c>
+      <c r="C9" s="24" t="n">
+        <v>0.000754228176129612</v>
+      </c>
+      <c r="D9" s="19" t="n">
+        <v>1.56051205621275E-005</v>
+      </c>
+      <c r="E9" s="19" t="n">
+        <v>0.000499874631743065</v>
+      </c>
+      <c r="F9" s="23" t="n">
+        <v>1.94098841162277E-005</v>
+      </c>
+      <c r="G9" s="24" t="n">
+        <v>0.00365694916376563</v>
+      </c>
+      <c r="H9" s="19" t="n">
+        <v>9.23603159455202E-005</v>
+      </c>
+      <c r="I9" s="19" t="n">
+        <v>0.0440800797792334</v>
+      </c>
+      <c r="J9" s="23" t="n">
+        <v>2.03450445336657E-005</v>
+      </c>
+      <c r="K9" s="24" t="n">
+        <v>0.0184236769399682</v>
+      </c>
+      <c r="L9" s="20" t="n">
+        <v>3.01978933678283E-005</v>
+      </c>
+      <c r="M9" s="25" t="n">
+        <v>0.013482961738168</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="n">
         <v>250</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="8" t="n">
+      <c r="B10" s="23" t="n">
+        <v>7.39015246330519E-006</v>
+      </c>
+      <c r="C10" s="24" t="n">
+        <v>0.000103601910841125</v>
+      </c>
+      <c r="D10" s="19" t="n">
+        <v>1.01029439510744E-005</v>
+      </c>
+      <c r="E10" s="19" t="n">
+        <v>0.00183707789433091</v>
+      </c>
+      <c r="F10" s="23" t="n">
+        <v>7.80557799891109E-006</v>
+      </c>
+      <c r="G10" s="24" t="n">
+        <v>0.000861489597280515</v>
+      </c>
+      <c r="H10" s="19" t="n">
+        <v>1.39827427512731E-005</v>
+      </c>
+      <c r="I10" s="19" t="n">
+        <v>0.00236455697234272</v>
+      </c>
+      <c r="J10" s="23" t="n">
+        <v>2.44172526510698E-005</v>
+      </c>
+      <c r="K10" s="24" t="n">
+        <v>0.00205907897283656</v>
+      </c>
+      <c r="L10" s="20" t="n">
+        <v>1.27397339631267E-005</v>
+      </c>
+      <c r="M10" s="25" t="n">
+        <v>0.00144516106952637</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="n">
         <v>500</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="B8" s="16" t="n">
-        <v>3.58752902898499E-005</v>
-      </c>
-      <c r="C8" s="17" t="n">
-        <v>0.0130635215976293</v>
-      </c>
-      <c r="D8" s="18" t="n">
-        <v>1.82873157512579E-005</v>
-      </c>
-      <c r="E8" s="18" t="n">
-        <v>0.0276028922670915</v>
-      </c>
-      <c r="F8" s="16" t="n">
-        <v>5.92699062422513E-005</v>
-      </c>
-      <c r="G8" s="17" t="n">
-        <v>0.0105684386648203</v>
-      </c>
-      <c r="H8" s="18" t="n">
-        <v>7.21152814966765E-005</v>
-      </c>
-      <c r="I8" s="18" t="n">
-        <v>0.0390139155874581</v>
-      </c>
-      <c r="J8" s="16" t="n">
-        <v>0.000394138629702215</v>
-      </c>
-      <c r="K8" s="17" t="n">
-        <v>0.117094792603027</v>
-      </c>
-      <c r="L8" s="19" t="n">
-        <v>0.00011593728469645</v>
-      </c>
-      <c r="M8" s="20" t="n">
-        <v>0.0414687121440053</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="n">
-        <v>100</v>
-      </c>
-      <c r="B9" s="22" t="n">
-        <v>3.2691016816007E-006</v>
-      </c>
-      <c r="C9" s="23" t="n">
-        <v>0.000754228176129612</v>
-      </c>
-      <c r="D9" s="18" t="n">
-        <v>1.56051205621275E-005</v>
-      </c>
-      <c r="E9" s="18" t="n">
-        <v>0.000499874631743065</v>
-      </c>
-      <c r="F9" s="22" t="n">
-        <v>1.94098841162277E-005</v>
-      </c>
-      <c r="G9" s="23" t="n">
-        <v>0.00365694916376563</v>
-      </c>
-      <c r="H9" s="18" t="n">
-        <v>9.23603159455202E-005</v>
-      </c>
-      <c r="I9" s="18" t="n">
-        <v>0.0440800797792334</v>
-      </c>
-      <c r="J9" s="22" t="n">
-        <v>2.03450445336657E-005</v>
-      </c>
-      <c r="K9" s="23" t="n">
-        <v>0.0184236769399682</v>
-      </c>
-      <c r="L9" s="19" t="n">
-        <v>3.01978933678283E-005</v>
-      </c>
-      <c r="M9" s="24" t="n">
-        <v>0.013482961738168</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="n">
-        <v>250</v>
-      </c>
-      <c r="B10" s="22" t="n">
-        <v>7.39015246330519E-006</v>
-      </c>
-      <c r="C10" s="23" t="n">
-        <v>0.000103601910841125</v>
-      </c>
-      <c r="D10" s="18" t="n">
-        <v>1.01029439510744E-005</v>
-      </c>
-      <c r="E10" s="18" t="n">
-        <v>0.00183707789433091</v>
-      </c>
-      <c r="F10" s="22" t="n">
-        <v>7.80557799891109E-006</v>
-      </c>
-      <c r="G10" s="23" t="n">
-        <v>0.000861489597280515</v>
-      </c>
-      <c r="H10" s="18" t="n">
-        <v>1.39827427512731E-005</v>
-      </c>
-      <c r="I10" s="18" t="n">
-        <v>0.00236455697234272</v>
-      </c>
-      <c r="J10" s="22" t="n">
-        <v>2.44172526510698E-005</v>
-      </c>
-      <c r="K10" s="23" t="n">
-        <v>0.00205907897283656</v>
-      </c>
-      <c r="L10" s="19" t="n">
-        <v>1.27397339631267E-005</v>
-      </c>
-      <c r="M10" s="24" t="n">
-        <v>0.00144516106952637</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
-        <v>500</v>
-      </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="23" t="n">
         <v>3.20869307476719E-006</v>
       </c>
-      <c r="C11" s="23" t="n">
+      <c r="C11" s="24" t="n">
         <v>0.0421378974908736</v>
       </c>
-      <c r="D11" s="18" t="n">
+      <c r="D11" s="19" t="n">
         <v>4.17980819639853E-006</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="19" t="n">
         <v>0.00042105101093757</v>
       </c>
-      <c r="F11" s="22" t="n">
+      <c r="F11" s="23" t="n">
         <v>5.89494798615797E-006</v>
       </c>
-      <c r="G11" s="23" t="n">
+      <c r="G11" s="24" t="n">
         <v>0.022097846016492</v>
       </c>
-      <c r="H11" s="18" t="n">
+      <c r="H11" s="19" t="n">
         <v>7.68050863963276E-006</v>
       </c>
-      <c r="I11" s="18" t="n">
+      <c r="I11" s="19" t="n">
         <v>0.000183722039095801</v>
       </c>
-      <c r="J11" s="22" t="n">
+      <c r="J11" s="23" t="n">
         <v>2.29452342860326E-005</v>
       </c>
-      <c r="K11" s="23" t="n">
+      <c r="K11" s="24" t="n">
         <v>0.00661509530930614</v>
       </c>
-      <c r="L11" s="19" t="n">
+      <c r="L11" s="20" t="n">
         <v>8.7818384365978E-006</v>
       </c>
-      <c r="M11" s="24" t="n">
+      <c r="M11" s="25" t="n">
         <v>0.014291122373341</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="n">
+      <c r="A12" s="22" t="n">
         <v>1000</v>
       </c>
-      <c r="B12" s="22" t="n">
+      <c r="B12" s="23" t="n">
         <v>6.30397683693763E-006</v>
       </c>
-      <c r="C12" s="23" t="n">
+      <c r="C12" s="24" t="n">
         <v>0.0657966584278266</v>
       </c>
-      <c r="D12" s="18" t="n">
+      <c r="D12" s="19" t="n">
         <v>4.58853535401996E-006</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="19" t="n">
         <v>0.000200816689121658</v>
       </c>
-      <c r="F12" s="22" t="n">
+      <c r="F12" s="23" t="n">
         <v>5.78562852636514E-006</v>
       </c>
-      <c r="G12" s="23" t="n">
+      <c r="G12" s="24" t="n">
         <v>0.000352585453400881</v>
       </c>
-      <c r="H12" s="18" t="n">
+      <c r="H12" s="19" t="n">
         <v>4.40366732763583E-006</v>
       </c>
-      <c r="I12" s="18" t="n">
+      <c r="I12" s="19" t="n">
         <v>0.000282026900133431</v>
       </c>
-      <c r="J12" s="22" t="n">
+      <c r="J12" s="23" t="n">
         <v>5.46095124019301E-006</v>
       </c>
-      <c r="K12" s="23" t="n">
+      <c r="K12" s="24" t="n">
         <v>0.00021223334112653</v>
       </c>
-      <c r="L12" s="19" t="n">
+      <c r="L12" s="20" t="n">
         <v>5.30855185703032E-006</v>
       </c>
-      <c r="M12" s="24" t="n">
+      <c r="M12" s="25" t="n">
         <v>0.0133688641623218</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="n">
+      <c r="A13" s="22" t="n">
         <v>2000</v>
       </c>
-      <c r="B13" s="25" t="n">
+      <c r="B13" s="26" t="n">
         <v>2.64641686266456E-006</v>
       </c>
-      <c r="C13" s="26" t="n">
+      <c r="C13" s="27" t="n">
         <v>0.108570956390905</v>
       </c>
-      <c r="D13" s="18" t="n">
+      <c r="D13" s="19" t="n">
         <v>2.86719382177899E-006</v>
       </c>
-      <c r="E13" s="18" t="n">
+      <c r="E13" s="19" t="n">
         <v>0.0177121966384384</v>
       </c>
-      <c r="F13" s="25" t="n">
+      <c r="F13" s="26" t="n">
         <v>5.22073468624526E-006</v>
       </c>
-      <c r="G13" s="26" t="n">
+      <c r="G13" s="27" t="n">
         <v>0.00392824935572987</v>
       </c>
-      <c r="H13" s="18" t="n">
+      <c r="H13" s="19" t="n">
         <v>1.11550614642507E-005</v>
       </c>
-      <c r="I13" s="18" t="n">
+      <c r="I13" s="19" t="n">
         <v>0.000420187558341592</v>
       </c>
-      <c r="J13" s="25" t="n">
+      <c r="J13" s="26" t="n">
         <v>8.34970908246678E-006</v>
       </c>
-      <c r="K13" s="26" t="n">
+      <c r="K13" s="27" t="n">
         <v>0.000814897227250397</v>
       </c>
-      <c r="L13" s="19" t="n">
+      <c r="L13" s="20" t="n">
         <v>6.04782318348127E-006</v>
       </c>
-      <c r="M13" s="27" t="n">
+      <c r="M13" s="28" t="n">
         <v>0.026289297434133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="29" t="n">
+      <c r="A14" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="30" t="n">
         <v>9.78227186818753E-006</v>
       </c>
-      <c r="C14" s="30" t="n">
+      <c r="C14" s="31" t="n">
         <v>0.0384044773323675</v>
       </c>
-      <c r="D14" s="29" t="n">
+      <c r="D14" s="30" t="n">
         <v>9.27181960610954E-006</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="31" t="n">
         <v>0.00804565152194385</v>
       </c>
-      <c r="F14" s="29" t="n">
+      <c r="F14" s="30" t="n">
         <v>1.72311132593597E-005</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="31" t="n">
         <v>0.0069109263752482</v>
       </c>
-      <c r="H14" s="29" t="n">
+      <c r="H14" s="30" t="n">
         <v>3.36162629374982E-005</v>
       </c>
-      <c r="I14" s="30" t="n">
+      <c r="I14" s="31" t="n">
         <v>0.0143907481394342</v>
       </c>
-      <c r="J14" s="29" t="n">
+      <c r="J14" s="30" t="n">
         <v>7.92761369159405E-005</v>
       </c>
-      <c r="K14" s="30" t="n">
+      <c r="K14" s="31" t="n">
         <v>0.0242032957322525</v>
       </c>
-      <c r="L14" s="31" t="n">
+      <c r="L14" s="32" t="n">
         <v>2.98355209174191E-005</v>
       </c>
-      <c r="M14" s="32" t="n">
+      <c r="M14" s="33" t="n">
         <v>0.0183910198202492</v>
       </c>
     </row>
@@ -16505,10 +16619,10 @@
       <c r="A20" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B20" s="33" t="n">
+      <c r="B20" s="34" t="n">
         <v>2.64602741007915E-006</v>
       </c>
-      <c r="C20" s="22" t="n">
+      <c r="C20" s="23" t="n">
         <v>8.45248971571096E-005</v>
       </c>
     </row>
@@ -16516,10 +16630,10 @@
       <c r="A21" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B21" s="18" t="n">
+      <c r="B21" s="19" t="n">
         <v>2.58307568920722E-006</v>
       </c>
-      <c r="C21" s="26" t="n">
+      <c r="C21" s="27" t="n">
         <v>7.58083330056681E-005</v>
       </c>
     </row>
@@ -16527,10 +16641,10 @@
       <c r="A22" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B22" s="33" t="n">
+      <c r="B22" s="34" t="n">
         <v>2.56160228536089E-006</v>
       </c>
-      <c r="C22" s="33" t="n">
+      <c r="C22" s="34" t="n">
         <v>7.68545666619592E-005</v>
       </c>
     </row>
@@ -16538,50 +16652,50 @@
       <c r="A23" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B23" s="25" t="n">
+      <c r="B23" s="26" t="n">
         <v>2.58417734445314E-006</v>
       </c>
-      <c r="C23" s="18" t="n">
+      <c r="C23" s="19" t="n">
         <v>0.000121594815380886</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="22" t="n">
+      <c r="B24" s="23" t="n">
         <v>3.03647753812124E-006</v>
       </c>
-      <c r="C24" s="18" t="n">
+      <c r="C24" s="19" t="n">
         <v>8.44823534778547E-005</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="22" t="n">
+      <c r="B25" s="23" t="n">
         <v>2.61434031870591E-006</v>
       </c>
-      <c r="C25" s="18" t="n">
+      <c r="C25" s="19" t="n">
         <v>8.1532351679863E-005</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="22" t="n">
+      <c r="B26" s="23" t="n">
         <v>2.76965992404646E-006</v>
       </c>
-      <c r="C26" s="33" t="n">
+      <c r="C26" s="34" t="n">
         <v>8.8773597318109E-005</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="22" t="n">
+      <c r="B27" s="23" t="n">
         <v>2.78905245566453E-006</v>
       </c>
-      <c r="C27" s="22" t="n">
+      <c r="C27" s="23" t="n">
         <v>0.000106031093266614</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="25" t="n">
+      <c r="B28" s="26" t="n">
         <v>2.64641686266456E-006</v>
       </c>
-      <c r="C28" s="18" t="n">
+      <c r="C28" s="19" t="n">
         <v>0.000200816689121658</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refined target distribution and transformation methodologies
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Findings" sheetId="1" state="visible" r:id="rId2"/>
@@ -9259,7 +9259,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9375,7 +9375,7 @@
   </sheetPr>
   <dimension ref="A1:G257"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J213" activeCellId="0" sqref="J213"/>
     </sheetView>
   </sheetViews>
@@ -15769,7 +15769,7 @@
   <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A247" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F283" activeCellId="0" sqref="F283"/>
+      <selection pane="topLeft" activeCell="F302" activeCellId="0" sqref="F302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -26789,8 +26789,8 @@
   </sheetPr>
   <dimension ref="A3:M28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updated documents on 4/4/2018
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Findings" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,11 +14,12 @@
     <sheet name="1 LSTM Data" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="2 LSTM Data" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Pivot Table (1 LSTM)" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Model Summary" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="70">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -191,6 +192,54 @@
   </si>
   <si>
     <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Algo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no PCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyperparameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lasso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 1day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 5day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 1day pct_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 5day pct_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XGBoost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 1day pct_change cls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 5day pct_change cls</t>
   </si>
 </sst>
 </file>
@@ -533,7 +582,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -788,6 +837,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="34" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -26789,8 +26846,8 @@
   </sheetPr>
   <dimension ref="A3:M28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27276,4 +27333,145 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.62"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="65" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new ways to display benchmark modeling results
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -14,12 +14,14 @@
     <sheet name="1 LSTM Data" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="2 LSTM Data" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Pivot Table (1 LSTM)" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="LSTM Model Summary" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Classification Model Summary" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Regression Model Summary" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="LSTM Model Summary" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="93">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -188,16 +190,46 @@
     <t xml:space="preserve">test error eval time</t>
   </si>
   <si>
-    <t xml:space="preserve">Construct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target</t>
+    <t xml:space="preserve">no PCA</t>
   </si>
   <si>
     <t xml:space="preserve">PCA</t>
   </si>
   <si>
-    <t xml:space="preserve">no PCA</t>
+    <t xml:space="preserve">No PCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual values, train</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actual values, test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 1day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 5day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 1day pct_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adj Close 5day pct_change cls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As % of target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_iter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
   </si>
   <si>
     <t xml:space="preserve">Hyperparameter</t>
@@ -210,9 +242,6 @@
   </si>
   <si>
     <t xml:space="preserve">10-1, no dropout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adj Close 1day</t>
   </si>
   <si>
     <t xml:space="preserve">adam</t>
@@ -251,16 +280,28 @@
     <t xml:space="preserve">1.8019 (79.18%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Adj Close 5day</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.0547 (2.40%)</t>
   </si>
   <si>
     <t xml:space="preserve">0.3450 (7.19%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Adj Close 1day pct_change</t>
+    <t xml:space="preserve">1.1332 (49.72%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3428 (7.15%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0298 (2137.13%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0475 (5748.59%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0296 (2125.28%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0151 (1829.25%)</t>
   </si>
   <si>
     <t xml:space="preserve">Adj Close 5day pct_change</t>
@@ -271,18 +312,17 @@
   <si>
     <t xml:space="preserve">Adj Close 1day pct_change cls</t>
   </si>
-  <si>
-    <t xml:space="preserve">Adj Close 5day pct_change cls</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -334,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -580,6 +620,27 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -624,7 +685,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -909,8 +970,52 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="25" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="35" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="36" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="37" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -28404,10 +28509,2618 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:A58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I98"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="32" t="n">
+        <v>1E-010</v>
+      </c>
+      <c r="B4" s="72" t="n">
+        <v>-0.00111293540284043</v>
+      </c>
+      <c r="C4" s="73" t="n">
+        <v>-0.00282414495713061</v>
+      </c>
+      <c r="D4" s="73" t="n">
+        <v>-0.000697946339227086</v>
+      </c>
+      <c r="E4" s="73" t="n">
+        <v>-0.00304118617429148</v>
+      </c>
+      <c r="F4" s="74" t="n">
+        <v>-0.00135596626242466</v>
+      </c>
+      <c r="G4" s="75" t="n">
+        <v>-0.00291327737615589</v>
+      </c>
+      <c r="H4" s="75" t="n">
+        <v>-0.000742094377226566</v>
+      </c>
+      <c r="I4" s="75" t="n">
+        <v>-0.00266934612194859</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="32" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="B5" s="76" t="n">
+        <v>-0.00111293371315058</v>
+      </c>
+      <c r="C5" s="76" t="n">
+        <v>-0.00282414319570515</v>
+      </c>
+      <c r="D5" s="76" t="n">
+        <v>-0.000697946354035176</v>
+      </c>
+      <c r="E5" s="76" t="n">
+        <v>-0.00304118618738589</v>
+      </c>
+      <c r="F5" s="77" t="n">
+        <v>-0.0013559640302148</v>
+      </c>
+      <c r="G5" s="77" t="n">
+        <v>-0.00291327494139364</v>
+      </c>
+      <c r="H5" s="77" t="n">
+        <v>-0.000742094205402627</v>
+      </c>
+      <c r="I5" s="77" t="n">
+        <v>-0.00266934514913159</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="32" t="n">
+        <v>1E-008</v>
+      </c>
+      <c r="B6" s="76" t="n">
+        <v>-0.00111291681821082</v>
+      </c>
+      <c r="C6" s="76" t="n">
+        <v>-0.00282412559097047</v>
+      </c>
+      <c r="D6" s="76" t="n">
+        <v>-0.000697946509613028</v>
+      </c>
+      <c r="E6" s="76" t="n">
+        <v>-0.00304118632476938</v>
+      </c>
+      <c r="F6" s="77" t="n">
+        <v>-0.00135594171035305</v>
+      </c>
+      <c r="G6" s="77" t="n">
+        <v>-0.00291325060517979</v>
+      </c>
+      <c r="H6" s="77" t="n">
+        <v>-0.000742092494733002</v>
+      </c>
+      <c r="I6" s="77" t="n">
+        <v>-0.00266933542928393</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="32" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="B7" s="76" t="n">
+        <v>-0.00111274884219232</v>
+      </c>
+      <c r="C7" s="76" t="n">
+        <v>-0.0028239506054595</v>
+      </c>
+      <c r="D7" s="76" t="n">
+        <v>-0.000697948815583526</v>
+      </c>
+      <c r="E7" s="76" t="n">
+        <v>-0.00304118834270706</v>
+      </c>
+      <c r="F7" s="77" t="n">
+        <v>-0.00135571798010367</v>
+      </c>
+      <c r="G7" s="77" t="n">
+        <v>-0.00291299676426354</v>
+      </c>
+      <c r="H7" s="77" t="n">
+        <v>-0.000742076142398709</v>
+      </c>
+      <c r="I7" s="77" t="n">
+        <v>-0.00266923909233181</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="32" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="B8" s="76" t="n">
+        <v>-0.00111108689110401</v>
+      </c>
+      <c r="C8" s="76" t="n">
+        <v>-0.00282225287629909</v>
+      </c>
+      <c r="D8" s="76" t="n">
+        <v>-0.000698037407777804</v>
+      </c>
+      <c r="E8" s="76" t="n">
+        <v>-0.00304125295274483</v>
+      </c>
+      <c r="F8" s="77" t="n">
+        <v>-0.00135357087357215</v>
+      </c>
+      <c r="G8" s="77" t="n">
+        <v>-0.00291096081902446</v>
+      </c>
+      <c r="H8" s="77" t="n">
+        <v>-0.000742027158295506</v>
+      </c>
+      <c r="I8" s="77" t="n">
+        <v>-0.0026684512193998</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="32" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="B9" s="76" t="n">
+        <v>-0.00109545216856461</v>
+      </c>
+      <c r="C9" s="76" t="n">
+        <v>-0.00280667914358119</v>
+      </c>
+      <c r="D9" s="76" t="n">
+        <v>-0.000699040313410207</v>
+      </c>
+      <c r="E9" s="76" t="n">
+        <v>-0.00304296287503557</v>
+      </c>
+      <c r="F9" s="77" t="n">
+        <v>-0.00133376043969365</v>
+      </c>
+      <c r="G9" s="77" t="n">
+        <v>-0.0028930388719619</v>
+      </c>
+      <c r="H9" s="77" t="n">
+        <v>-0.000742015114884388</v>
+      </c>
+      <c r="I9" s="77" t="n">
+        <v>-0.00266689726104487</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="32" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="B10" s="76" t="n">
+        <v>-0.000951001585219408</v>
+      </c>
+      <c r="C10" s="76" t="n">
+        <v>-0.00266549852838807</v>
+      </c>
+      <c r="D10" s="76" t="n">
+        <v>-0.000700097847035075</v>
+      </c>
+      <c r="E10" s="76" t="n">
+        <v>-0.00305321724402439</v>
+      </c>
+      <c r="F10" s="77" t="n">
+        <v>-0.00114910275528798</v>
+      </c>
+      <c r="G10" s="77" t="n">
+        <v>-0.00274525988528818</v>
+      </c>
+      <c r="H10" s="77" t="n">
+        <v>-0.000741866903437737</v>
+      </c>
+      <c r="I10" s="77" t="n">
+        <v>-0.00266680781006204</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="B11" s="76" t="n">
+        <v>-0.000420641696961403</v>
+      </c>
+      <c r="C11" s="76" t="n">
+        <v>-0.00214803263901152</v>
+      </c>
+      <c r="D11" s="76" t="n">
+        <v>-0.000702725810807464</v>
+      </c>
+      <c r="E11" s="76" t="n">
+        <v>-0.00306807339859227</v>
+      </c>
+      <c r="F11" s="77" t="n">
+        <v>-0.000531390052225809</v>
+      </c>
+      <c r="G11" s="77" t="n">
+        <v>-0.002253331687501</v>
+      </c>
+      <c r="H11" s="77" t="n">
+        <v>-0.000742084078181588</v>
+      </c>
+      <c r="I11" s="77" t="n">
+        <v>-0.00267147142199126</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B12" s="76" t="n">
+        <v>-0.000449769312716028</v>
+      </c>
+      <c r="C12" s="76" t="n">
+        <v>-0.00218689107338826</v>
+      </c>
+      <c r="D12" s="76" t="n">
+        <v>-0.000702725810807464</v>
+      </c>
+      <c r="E12" s="76" t="n">
+        <v>-0.00306964567825532</v>
+      </c>
+      <c r="F12" s="77" t="n">
+        <v>-0.000564639024443468</v>
+      </c>
+      <c r="G12" s="77" t="n">
+        <v>-0.00229396302026837</v>
+      </c>
+      <c r="H12" s="77" t="n">
+        <v>-0.000742084078181588</v>
+      </c>
+      <c r="I12" s="77" t="n">
+        <v>-0.00267163595460066</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B13" s="73" t="n">
+        <v>-0.00468758048692385</v>
+      </c>
+      <c r="C13" s="72" t="n">
+        <v>-0.00650323234156696</v>
+      </c>
+      <c r="D13" s="72" t="n">
+        <v>-0.000702725810807464</v>
+      </c>
+      <c r="E13" s="72" t="n">
+        <v>-0.00306964567825532</v>
+      </c>
+      <c r="F13" s="75" t="n">
+        <v>-0.00486270378259332</v>
+      </c>
+      <c r="G13" s="74" t="n">
+        <v>-0.00658565108550885</v>
+      </c>
+      <c r="H13" s="74" t="n">
+        <v>-0.000742084078181588</v>
+      </c>
+      <c r="I13" s="74" t="n">
+        <v>-0.00267163595460066</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="32" t="n">
+        <v>1E-010</v>
+      </c>
+      <c r="B18" s="79" t="n">
+        <f aca="false">B4/2.78594350245436</f>
+        <v>-0.00039948240223104</v>
+      </c>
+      <c r="C18" s="79" t="n">
+        <f aca="false">C4/2.78913990345228</f>
+        <v>-0.00101255048326368</v>
+      </c>
+      <c r="D18" s="79" t="n">
+        <f aca="false">D4/0.001137033158201</f>
+        <v>-0.613831121980091</v>
+      </c>
+      <c r="E18" s="79" t="n">
+        <f aca="false">E4/0.006986039944106</f>
+        <v>-0.435323330330694</v>
+      </c>
+      <c r="F18" s="79" t="n">
+        <f aca="false">F4/2.78594350245436</f>
+        <v>-0.000486717071336904</v>
+      </c>
+      <c r="G18" s="79" t="n">
+        <f aca="false">G4/2.78913990345228</f>
+        <v>-0.00104450743849384</v>
+      </c>
+      <c r="H18" s="79" t="n">
+        <f aca="false">H4/0.001137033158201</f>
+        <v>-0.65265851912419</v>
+      </c>
+      <c r="I18" s="79" t="n">
+        <f aca="false">I4/0.006986039944106</f>
+        <v>-0.382097174265467</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="32" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="B19" s="79" t="n">
+        <f aca="false">B5/2.78594350245436</f>
+        <v>-0.000399481795725616</v>
+      </c>
+      <c r="C19" s="79" t="n">
+        <f aca="false">C5/2.78913990345228</f>
+        <v>-0.0010125498517337</v>
+      </c>
+      <c r="D19" s="79" t="n">
+        <f aca="false">D5/0.001137033158201</f>
+        <v>-0.613831135003537</v>
+      </c>
+      <c r="E19" s="79" t="n">
+        <f aca="false">E5/0.006986039944106</f>
+        <v>-0.435323332205062</v>
+      </c>
+      <c r="F19" s="79" t="n">
+        <f aca="false">F5/2.78594350245436</f>
+        <v>-0.000486716270096728</v>
+      </c>
+      <c r="G19" s="79" t="n">
+        <f aca="false">G5/2.78913990345228</f>
+        <v>-0.00104450656555009</v>
+      </c>
+      <c r="H19" s="79" t="n">
+        <f aca="false">H5/0.001137033158201</f>
+        <v>-0.652658368008158</v>
+      </c>
+      <c r="I19" s="79" t="n">
+        <f aca="false">I5/0.006986039944106</f>
+        <v>-0.382097035013902</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="32" t="n">
+        <v>1E-008</v>
+      </c>
+      <c r="B20" s="79" t="n">
+        <f aca="false">B6/2.78594350245436</f>
+        <v>-0.000399475731374438</v>
+      </c>
+      <c r="C20" s="79" t="n">
+        <f aca="false">C6/2.78913990345228</f>
+        <v>-0.00101254353984714</v>
+      </c>
+      <c r="D20" s="79" t="n">
+        <f aca="false">D6/0.001137033158201</f>
+        <v>-0.613831271831431</v>
+      </c>
+      <c r="E20" s="79" t="n">
+        <f aca="false">E6/0.006986039944106</f>
+        <v>-0.435323351870493</v>
+      </c>
+      <c r="F20" s="79" t="n">
+        <f aca="false">F6/2.78594350245436</f>
+        <v>-0.00048670825849788</v>
+      </c>
+      <c r="G20" s="79" t="n">
+        <f aca="false">G6/2.78913990345228</f>
+        <v>-0.00104449784020296</v>
+      </c>
+      <c r="H20" s="79" t="n">
+        <f aca="false">H6/0.001137033158201</f>
+        <v>-0.65265686350531</v>
+      </c>
+      <c r="I20" s="79" t="n">
+        <f aca="false">I6/0.006986039944106</f>
+        <v>-0.382095643689526</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="32" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="B21" s="79" t="n">
+        <f aca="false">B7/2.78594350245436</f>
+        <v>-0.000399415437252053</v>
+      </c>
+      <c r="C21" s="79" t="n">
+        <f aca="false">C7/2.78913990345228</f>
+        <v>-0.00101248080168518</v>
+      </c>
+      <c r="D21" s="79" t="n">
+        <f aca="false">D7/0.001137033158201</f>
+        <v>-0.613833299890579</v>
+      </c>
+      <c r="E21" s="79" t="n">
+        <f aca="false">E7/0.006986039944106</f>
+        <v>-0.435323640723362</v>
+      </c>
+      <c r="F21" s="79" t="n">
+        <f aca="false">F7/2.78594350245436</f>
+        <v>-0.000486627951682908</v>
+      </c>
+      <c r="G21" s="79" t="n">
+        <f aca="false">G7/2.78913990345228</f>
+        <v>-0.00104440682973915</v>
+      </c>
+      <c r="H21" s="79" t="n">
+        <f aca="false">H7/0.001137033158201</f>
+        <v>-0.652642481924461</v>
+      </c>
+      <c r="I21" s="79" t="n">
+        <f aca="false">I7/0.006986039944106</f>
+        <v>-0.38208185376664</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="32" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="B22" s="79" t="n">
+        <f aca="false">B8/2.78594350245436</f>
+        <v>-0.000398818888511259</v>
+      </c>
+      <c r="C22" s="79" t="n">
+        <f aca="false">C8/2.78913990345228</f>
+        <v>-0.00101187210896299</v>
+      </c>
+      <c r="D22" s="79" t="n">
+        <f aca="false">D8/0.001137033158201</f>
+        <v>-0.613911215115512</v>
+      </c>
+      <c r="E22" s="79" t="n">
+        <f aca="false">E8/0.006986039944106</f>
+        <v>-0.435332889172882</v>
+      </c>
+      <c r="F22" s="79" t="n">
+        <f aca="false">F8/2.78594350245436</f>
+        <v>-0.000485857258906968</v>
+      </c>
+      <c r="G22" s="79" t="n">
+        <f aca="false">G8/2.78913990345228</f>
+        <v>-0.00104367687523362</v>
+      </c>
+      <c r="H22" s="79" t="n">
+        <f aca="false">H8/0.001137033158201</f>
+        <v>-0.652599401295854</v>
+      </c>
+      <c r="I22" s="79" t="n">
+        <f aca="false">I8/0.006986039944106</f>
+        <v>-0.381969075577806</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="32" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="B23" s="79" t="n">
+        <f aca="false">B9/2.78594350245436</f>
+        <v>-0.000393206885781976</v>
+      </c>
+      <c r="C23" s="79" t="n">
+        <f aca="false">C9/2.78913990345228</f>
+        <v>-0.0010062884045749</v>
+      </c>
+      <c r="D23" s="79" t="n">
+        <f aca="false">D9/0.001137033158201</f>
+        <v>-0.614793252393994</v>
+      </c>
+      <c r="E23" s="79" t="n">
+        <f aca="false">E9/0.006986039944106</f>
+        <v>-0.435577651914639</v>
+      </c>
+      <c r="F23" s="79" t="n">
+        <f aca="false">F9/2.78594350245436</f>
+        <v>-0.00047874640620624</v>
+      </c>
+      <c r="G23" s="79" t="n">
+        <f aca="false">G9/2.78913990345228</f>
+        <v>-0.00103725125741488</v>
+      </c>
+      <c r="H23" s="79" t="n">
+        <f aca="false">H9/0.001137033158201</f>
+        <v>-0.652588809334633</v>
+      </c>
+      <c r="I23" s="79" t="n">
+        <f aca="false">I9/0.006986039944106</f>
+        <v>-0.381746637921085</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="32" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="B24" s="79" t="n">
+        <f aca="false">B10/2.78594350245436</f>
+        <v>-0.000341357096574857</v>
+      </c>
+      <c r="C24" s="79" t="n">
+        <f aca="false">C10/2.78913990345228</f>
+        <v>-0.000955670429112871</v>
+      </c>
+      <c r="D24" s="79" t="n">
+        <f aca="false">D10/0.001137033158201</f>
+        <v>-0.615723333999126</v>
+      </c>
+      <c r="E24" s="79" t="n">
+        <f aca="false">E10/0.006986039944106</f>
+        <v>-0.437045489068572</v>
+      </c>
+      <c r="F24" s="79" t="n">
+        <f aca="false">F10/2.78594350245436</f>
+        <v>-0.000412464486187765</v>
+      </c>
+      <c r="G24" s="79" t="n">
+        <f aca="false">G10/2.78913990345228</f>
+        <v>-0.000984267544948252</v>
+      </c>
+      <c r="H24" s="79" t="n">
+        <f aca="false">H10/0.001137033158201</f>
+        <v>-0.652458460060663</v>
+      </c>
+      <c r="I24" s="79" t="n">
+        <f aca="false">I10/0.006986039944106</f>
+        <v>-0.381733833673822</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="B25" s="79" t="n">
+        <f aca="false">B11/2.78594350245436</f>
+        <v>-0.000150987159858348</v>
+      </c>
+      <c r="C25" s="79" t="n">
+        <f aca="false">C11/2.78913990345228</f>
+        <v>-0.000770141589653776</v>
+      </c>
+      <c r="D25" s="79" t="n">
+        <f aca="false">D11/0.001137033158201</f>
+        <v>-0.618034580380495</v>
+      </c>
+      <c r="E25" s="79" t="n">
+        <f aca="false">E11/0.006986039944106</f>
+        <v>-0.439172037826773</v>
+      </c>
+      <c r="F25" s="79" t="n">
+        <f aca="false">F11/2.78594350245436</f>
+        <v>-0.000190739708740563</v>
+      </c>
+      <c r="G25" s="79" t="n">
+        <f aca="false">G11/2.78913990345228</f>
+        <v>-0.000807894822598148</v>
+      </c>
+      <c r="H25" s="79" t="n">
+        <f aca="false">H11/0.001137033158201</f>
+        <v>-0.652649461301291</v>
+      </c>
+      <c r="I25" s="79" t="n">
+        <f aca="false">I11/0.006986039944106</f>
+        <v>-0.382401395263297</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B26" s="79" t="n">
+        <f aca="false">B12/2.78594350245436</f>
+        <v>-0.000161442366767234</v>
+      </c>
+      <c r="C26" s="79" t="n">
+        <f aca="false">C12/2.78913990345228</f>
+        <v>-0.000784073638859569</v>
+      </c>
+      <c r="D26" s="79" t="n">
+        <f aca="false">D12/0.001137033158201</f>
+        <v>-0.618034580380495</v>
+      </c>
+      <c r="E26" s="79" t="n">
+        <f aca="false">E12/0.006986039944106</f>
+        <v>-0.439397098043381</v>
+      </c>
+      <c r="F26" s="79" t="n">
+        <f aca="false">F12/2.78594350245436</f>
+        <v>-0.000202674255219473</v>
+      </c>
+      <c r="G26" s="79" t="n">
+        <f aca="false">G12/2.78913990345228</f>
+        <v>-0.000822462515210871</v>
+      </c>
+      <c r="H26" s="79" t="n">
+        <f aca="false">H12/0.001137033158201</f>
+        <v>-0.652649461301291</v>
+      </c>
+      <c r="I26" s="79" t="n">
+        <f aca="false">I12/0.006986039944106</f>
+        <v>-0.382424946890644</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B27" s="79" t="n">
+        <f aca="false">B13/2.78594350245436</f>
+        <v>-0.00168258275259142</v>
+      </c>
+      <c r="C27" s="79" t="n">
+        <f aca="false">C13/2.78913990345228</f>
+        <v>-0.00233162643921789</v>
+      </c>
+      <c r="D27" s="79" t="n">
+        <f aca="false">D13/0.001137033158201</f>
+        <v>-0.618034580380495</v>
+      </c>
+      <c r="E27" s="79" t="n">
+        <f aca="false">E13/0.006986039944106</f>
+        <v>-0.439397098043381</v>
+      </c>
+      <c r="F27" s="79" t="n">
+        <f aca="false">F13/2.78594350245436</f>
+        <v>-0.00174544235312359</v>
+      </c>
+      <c r="G27" s="79" t="n">
+        <f aca="false">G13/2.78913990345228</f>
+        <v>-0.00236117631724296</v>
+      </c>
+      <c r="H27" s="79" t="n">
+        <f aca="false">H13/0.001137033158201</f>
+        <v>-0.652649461301291</v>
+      </c>
+      <c r="I27" s="79" t="n">
+        <f aca="false">I13/0.006986039944106</f>
+        <v>-0.382424946890644</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="78"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" s="73" t="n">
+        <v>-0.00418950155250626</v>
+      </c>
+      <c r="C31" s="73" t="n">
+        <v>-0.00589857300792563</v>
+      </c>
+      <c r="D31" s="73" t="n">
+        <v>-0.000699821673541167</v>
+      </c>
+      <c r="E31" s="73" t="n">
+        <v>-0.00305221798475555</v>
+      </c>
+      <c r="F31" s="75" t="n">
+        <v>-0.00491784416144387</v>
+      </c>
+      <c r="G31" s="75" t="n">
+        <v>-0.00579954664786253</v>
+      </c>
+      <c r="H31" s="75" t="n">
+        <v>-0.000741851591458169</v>
+      </c>
+      <c r="I31" s="75" t="n">
+        <v>-0.00266995951679102</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="32" t="n">
+        <v>100</v>
+      </c>
+      <c r="B32" s="76" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C32" s="76" t="n">
+        <v>-0.00256726731164869</v>
+      </c>
+      <c r="D32" s="76" t="n">
+        <v>-0.000699794208077064</v>
+      </c>
+      <c r="E32" s="76" t="n">
+        <v>-0.00305112837241017</v>
+      </c>
+      <c r="F32" s="77" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G32" s="77" t="n">
+        <v>-0.00268912328761873</v>
+      </c>
+      <c r="H32" s="77" t="n">
+        <v>-0.00074196961743598</v>
+      </c>
+      <c r="I32" s="77" t="n">
+        <v>-0.0026687965932604</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B33" s="76" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C33" s="76" t="n">
+        <v>-0.00256700491974116</v>
+      </c>
+      <c r="D33" s="76" t="n">
+        <v>-0.000699761455773573</v>
+      </c>
+      <c r="E33" s="76" t="n">
+        <v>-0.00305073323066833</v>
+      </c>
+      <c r="F33" s="77" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G33" s="77" t="n">
+        <v>-0.00268896243097585</v>
+      </c>
+      <c r="H33" s="77" t="n">
+        <v>-0.000742167641530625</v>
+      </c>
+      <c r="I33" s="77" t="n">
+        <v>-0.0026687082011818</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B34" s="76" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C34" s="76" t="n">
+        <v>-0.00256694475062215</v>
+      </c>
+      <c r="D34" s="76" t="n">
+        <v>-0.000699719777918008</v>
+      </c>
+      <c r="E34" s="76" t="n">
+        <v>-0.00305069965316976</v>
+      </c>
+      <c r="F34" s="77" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G34" s="77" t="n">
+        <v>-0.00268902315871548</v>
+      </c>
+      <c r="H34" s="77" t="n">
+        <v>-0.000742201423760159</v>
+      </c>
+      <c r="I34" s="77" t="n">
+        <v>-0.00266903302312579</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="32" t="n">
+        <v>100000</v>
+      </c>
+      <c r="B35" s="76" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C35" s="76" t="n">
+        <v>-0.00256682666912852</v>
+      </c>
+      <c r="D35" s="76" t="n">
+        <v>-0.000699635575564522</v>
+      </c>
+      <c r="E35" s="76" t="n">
+        <v>-0.00305063541544027</v>
+      </c>
+      <c r="F35" s="77" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G35" s="77" t="n">
+        <v>-0.00268925408557493</v>
+      </c>
+      <c r="H35" s="77" t="n">
+        <v>-0.000742064946149555</v>
+      </c>
+      <c r="I35" s="77" t="n">
+        <v>-0.00266973552061847</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="32" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B36" s="76" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C36" s="76" t="n">
+        <v>-0.00256682450349221</v>
+      </c>
+      <c r="D36" s="76" t="n">
+        <v>-0.000699633011249336</v>
+      </c>
+      <c r="E36" s="76" t="n">
+        <v>-0.00305063337139949</v>
+      </c>
+      <c r="F36" s="77" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G36" s="77" t="n">
+        <v>-0.00268929696441721</v>
+      </c>
+      <c r="H36" s="77" t="n">
+        <v>-0.000742053910655911</v>
+      </c>
+      <c r="I36" s="77" t="n">
+        <v>-0.00266984146754958</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="32" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="B37" s="72" t="n">
+        <v>-0.000837907548335361</v>
+      </c>
+      <c r="C37" s="72" t="n">
+        <v>-0.00256682450349221</v>
+      </c>
+      <c r="D37" s="72" t="n">
+        <v>-0.000699633011249336</v>
+      </c>
+      <c r="E37" s="72" t="n">
+        <v>-0.00305063337139949</v>
+      </c>
+      <c r="F37" s="74" t="n">
+        <v>-0.000955880946032487</v>
+      </c>
+      <c r="G37" s="74" t="n">
+        <v>-0.00268929696441721</v>
+      </c>
+      <c r="H37" s="74" t="n">
+        <v>-0.000742053910655911</v>
+      </c>
+      <c r="I37" s="74" t="n">
+        <v>-0.00266984146754958</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H41" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I41" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="B42" s="79" t="n">
+        <f aca="false">B31/2.78594350245436</f>
+        <v>-0.00150379989716783</v>
+      </c>
+      <c r="C42" s="79" t="n">
+        <f aca="false">C31/2.78913990345228</f>
+        <v>-0.00211483583187226</v>
+      </c>
+      <c r="D42" s="79" t="n">
+        <f aca="false">D31/0.001137033158201</f>
+        <v>-0.615480444429972</v>
+      </c>
+      <c r="E42" s="79" t="n">
+        <f aca="false">E31/0.006986039944106</f>
+        <v>-0.4369024524875</v>
+      </c>
+      <c r="F42" s="79" t="n">
+        <f aca="false">F31/2.78594350245436</f>
+        <v>-0.00176523470670218</v>
+      </c>
+      <c r="G42" s="79" t="n">
+        <f aca="false">G31/2.78913990345228</f>
+        <v>-0.00207933156765786</v>
+      </c>
+      <c r="H42" s="79" t="n">
+        <f aca="false">H31/0.001137033158201</f>
+        <v>-0.652444993452889</v>
+      </c>
+      <c r="I42" s="79" t="n">
+        <f aca="false">I31/0.006986039944106</f>
+        <v>-0.38218497720495</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="32" t="n">
+        <v>100</v>
+      </c>
+      <c r="B43" s="79" t="n">
+        <f aca="false">B32/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C43" s="79" t="n">
+        <f aca="false">C32/2.78913990345228</f>
+        <v>-0.000920451250391218</v>
+      </c>
+      <c r="D43" s="79" t="n">
+        <f aca="false">D32/0.001137033158201</f>
+        <v>-0.615456289053408</v>
+      </c>
+      <c r="E43" s="79" t="n">
+        <f aca="false">E32/0.006986039944106</f>
+        <v>-0.436746482531115</v>
+      </c>
+      <c r="F43" s="79" t="n">
+        <f aca="false">F32/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G43" s="79" t="n">
+        <f aca="false">G32/2.78913990345228</f>
+        <v>-0.000964140695950838</v>
+      </c>
+      <c r="H43" s="79" t="n">
+        <f aca="false">H32/0.001137033158201</f>
+        <v>-0.652548795155557</v>
+      </c>
+      <c r="I43" s="79" t="n">
+        <f aca="false">I32/0.006986039944106</f>
+        <v>-0.382018513294075</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B44" s="79" t="n">
+        <f aca="false">B33/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C44" s="79" t="n">
+        <f aca="false">C33/2.78913990345228</f>
+        <v>-0.000920357174110853</v>
+      </c>
+      <c r="D44" s="79" t="n">
+        <f aca="false">D33/0.001137033158201</f>
+        <v>-0.615427483997676</v>
+      </c>
+      <c r="E44" s="79" t="n">
+        <f aca="false">E33/0.006986039944106</f>
+        <v>-0.436689920910369</v>
+      </c>
+      <c r="F44" s="79" t="n">
+        <f aca="false">F33/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G44" s="79" t="n">
+        <f aca="false">G33/2.78913990345228</f>
+        <v>-0.000964083023460949</v>
+      </c>
+      <c r="H44" s="79" t="n">
+        <f aca="false">H33/0.001137033158201</f>
+        <v>-0.652722953748221</v>
+      </c>
+      <c r="I44" s="79" t="n">
+        <f aca="false">I33/0.006986039944106</f>
+        <v>-0.382005860621129</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B45" s="79" t="n">
+        <f aca="false">B34/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C45" s="79" t="n">
+        <f aca="false">C34/2.78913990345228</f>
+        <v>-0.000920335601467998</v>
+      </c>
+      <c r="D45" s="79" t="n">
+        <f aca="false">D34/0.001137033158201</f>
+        <v>-0.615390829081094</v>
+      </c>
+      <c r="E45" s="79" t="n">
+        <f aca="false">E34/0.006986039944106</f>
+        <v>-0.436685114539544</v>
+      </c>
+      <c r="F45" s="79" t="n">
+        <f aca="false">F34/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G45" s="79" t="n">
+        <f aca="false">G34/2.78913990345228</f>
+        <v>-0.00096410479638799</v>
+      </c>
+      <c r="H45" s="79" t="n">
+        <f aca="false">H34/0.001137033158201</f>
+        <v>-0.652752664605191</v>
+      </c>
+      <c r="I45" s="79" t="n">
+        <f aca="false">I34/0.006986039944106</f>
+        <v>-0.382052356482388</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="32" t="n">
+        <v>100000</v>
+      </c>
+      <c r="B46" s="79" t="n">
+        <f aca="false">B35/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C46" s="79" t="n">
+        <f aca="false">C35/2.78913990345228</f>
+        <v>-0.000920293265300681</v>
+      </c>
+      <c r="D46" s="79" t="n">
+        <f aca="false">D35/0.001137033158201</f>
+        <v>-0.615316774641363</v>
+      </c>
+      <c r="E46" s="79" t="n">
+        <f aca="false">E35/0.006986039944106</f>
+        <v>-0.436675919383203</v>
+      </c>
+      <c r="F46" s="79" t="n">
+        <f aca="false">F35/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G46" s="79" t="n">
+        <f aca="false">G35/2.78913990345228</f>
+        <v>-0.000964187591395572</v>
+      </c>
+      <c r="H46" s="79" t="n">
+        <f aca="false">H35/0.001137033158201</f>
+        <v>-0.652632635026793</v>
+      </c>
+      <c r="I46" s="79" t="n">
+        <f aca="false">I35/0.006986039944106</f>
+        <v>-0.382152913807898</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="32" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B47" s="79" t="n">
+        <f aca="false">B36/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C47" s="79" t="n">
+        <f aca="false">C36/2.78913990345228</f>
+        <v>-0.000920292488847585</v>
+      </c>
+      <c r="D47" s="79" t="n">
+        <f aca="false">D36/0.001137033158201</f>
+        <v>-0.615314519372757</v>
+      </c>
+      <c r="E47" s="79" t="n">
+        <f aca="false">E36/0.006986039944106</f>
+        <v>-0.436675626793868</v>
+      </c>
+      <c r="F47" s="79" t="n">
+        <f aca="false">F36/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G47" s="79" t="n">
+        <f aca="false">G36/2.78913990345228</f>
+        <v>-0.000964202964895561</v>
+      </c>
+      <c r="H47" s="79" t="n">
+        <f aca="false">H36/0.001137033158201</f>
+        <v>-0.652622929510674</v>
+      </c>
+      <c r="I47" s="79" t="n">
+        <f aca="false">I36/0.006986039944106</f>
+        <v>-0.382168079328271</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="32" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="B48" s="79" t="n">
+        <f aca="false">B37/2.78594350245436</f>
+        <v>-0.000300762577416656</v>
+      </c>
+      <c r="C48" s="79" t="n">
+        <f aca="false">C37/2.78913990345228</f>
+        <v>-0.000920292488847585</v>
+      </c>
+      <c r="D48" s="79" t="n">
+        <f aca="false">D37/0.001137033158201</f>
+        <v>-0.615314519372757</v>
+      </c>
+      <c r="E48" s="79" t="n">
+        <f aca="false">E37/0.006986039944106</f>
+        <v>-0.436675626793868</v>
+      </c>
+      <c r="F48" s="79" t="n">
+        <f aca="false">F37/2.78594350245436</f>
+        <v>-0.000343108517882856</v>
+      </c>
+      <c r="G48" s="79" t="n">
+        <f aca="false">G37/2.78913990345228</f>
+        <v>-0.000964202964895561</v>
+      </c>
+      <c r="H48" s="79" t="n">
+        <f aca="false">H37/0.001137033158201</f>
+        <v>-0.652622929510674</v>
+      </c>
+      <c r="I48" s="79" t="n">
+        <f aca="false">I37/0.006986039944106</f>
+        <v>-0.382168079328271</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I53" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="32" t="n">
+        <v>1E-010</v>
+      </c>
+      <c r="B54" s="59" t="n">
+        <v>-0.000405996000266245</v>
+      </c>
+      <c r="C54" s="59" t="n">
+        <v>-0.00210695018623318</v>
+      </c>
+      <c r="D54" s="59" t="n">
+        <v>-0.000694249132928277</v>
+      </c>
+      <c r="E54" s="59" t="n">
+        <v>-0.00308672889512076</v>
+      </c>
+      <c r="F54" s="80" t="n">
+        <v>-0.000473225198945218</v>
+      </c>
+      <c r="G54" s="80" t="n">
+        <v>-0.00224827227833021</v>
+      </c>
+      <c r="H54" s="80" t="n">
+        <v>-0.000664809402421442</v>
+      </c>
+      <c r="I54" s="80" t="n">
+        <v>-0.00310177077550035</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="32" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="B55" s="61" t="n">
+        <v>-0.000405996000269856</v>
+      </c>
+      <c r="C55" s="61" t="n">
+        <v>-0.00210695018623432</v>
+      </c>
+      <c r="D55" s="61" t="n">
+        <v>-0.000694249132929411</v>
+      </c>
+      <c r="E55" s="61" t="n">
+        <v>-0.00308672889512208</v>
+      </c>
+      <c r="F55" s="81" t="n">
+        <v>-0.00047322521584036</v>
+      </c>
+      <c r="G55" s="81" t="n">
+        <v>-0.00224827242883179</v>
+      </c>
+      <c r="H55" s="81" t="n">
+        <v>-0.000664809302669281</v>
+      </c>
+      <c r="I55" s="81" t="n">
+        <v>-0.00310177069540761</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="32" t="n">
+        <v>1E-008</v>
+      </c>
+      <c r="B56" s="61" t="n">
+        <v>-0.000405996000543468</v>
+      </c>
+      <c r="C56" s="61" t="n">
+        <v>-0.00210695018634899</v>
+      </c>
+      <c r="D56" s="61" t="n">
+        <v>-0.000694249133042866</v>
+      </c>
+      <c r="E56" s="61" t="n">
+        <v>-0.0030867288952535</v>
+      </c>
+      <c r="F56" s="81" t="n">
+        <v>-0.000473225385076913</v>
+      </c>
+      <c r="G56" s="81" t="n">
+        <v>-0.00224827393304793</v>
+      </c>
+      <c r="H56" s="81" t="n">
+        <v>-0.000664808305233137</v>
+      </c>
+      <c r="I56" s="81" t="n">
+        <v>-0.00310176989481622</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="32" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="B57" s="61" t="n">
+        <v>-0.000405996027029902</v>
+      </c>
+      <c r="C57" s="61" t="n">
+        <v>-0.00210695019782497</v>
+      </c>
+      <c r="D57" s="61" t="n">
+        <v>-0.000694249144388348</v>
+      </c>
+      <c r="E57" s="61" t="n">
+        <v>-0.00308672890839525</v>
+      </c>
+      <c r="F57" s="81" t="n">
+        <v>-0.000473227105955835</v>
+      </c>
+      <c r="G57" s="81" t="n">
+        <v>-0.00224828877352045</v>
+      </c>
+      <c r="H57" s="81" t="n">
+        <v>-0.000664798338833684</v>
+      </c>
+      <c r="I57" s="81" t="n">
+        <v>-0.0031017619164212</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="32" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="B58" s="61" t="n">
+        <v>-0.000405998666913694</v>
+      </c>
+      <c r="C58" s="61" t="n">
+        <v>-0.00210695134437133</v>
+      </c>
+      <c r="D58" s="61" t="n">
+        <v>-0.000694250154098719</v>
+      </c>
+      <c r="E58" s="61" t="n">
+        <v>-0.00308673022251637</v>
+      </c>
+      <c r="F58" s="81" t="n">
+        <v>-0.000473247168444011</v>
+      </c>
+      <c r="G58" s="81" t="n">
+        <v>-0.00224844063761824</v>
+      </c>
+      <c r="H58" s="81" t="n">
+        <v>-0.000664708393184906</v>
+      </c>
+      <c r="I58" s="81" t="n">
+        <v>-0.00310168498553079</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="32" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="B59" s="61" t="n">
+        <v>-0.000406107426137982</v>
+      </c>
+      <c r="C59" s="61" t="n">
+        <v>-0.00210706597122042</v>
+      </c>
+      <c r="D59" s="61" t="n">
+        <v>-0.000694334349357489</v>
+      </c>
+      <c r="E59" s="61" t="n">
+        <v>-0.00308686164148339</v>
+      </c>
+      <c r="F59" s="81" t="n">
+        <v>-0.000473555016583991</v>
+      </c>
+      <c r="G59" s="81" t="n">
+        <v>-0.00225003374690476</v>
+      </c>
+      <c r="H59" s="81" t="n">
+        <v>-0.000663838893360779</v>
+      </c>
+      <c r="I59" s="81" t="n">
+        <v>-0.00310120378730034</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="32" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="B60" s="61" t="n">
+        <v>-0.000412733122966253</v>
+      </c>
+      <c r="C60" s="61" t="n">
+        <v>-0.00211764596185014</v>
+      </c>
+      <c r="D60" s="61" t="n">
+        <v>-0.000694815909750847</v>
+      </c>
+      <c r="E60" s="61" t="n">
+        <v>-0.00309531366537313</v>
+      </c>
+      <c r="F60" s="81" t="n">
+        <v>-0.000482141663327276</v>
+      </c>
+      <c r="G60" s="81" t="n">
+        <v>-0.00227361714250838</v>
+      </c>
+      <c r="H60" s="81" t="n">
+        <v>-0.000662048618980374</v>
+      </c>
+      <c r="I60" s="81" t="n">
+        <v>-0.00311204955332386</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="B61" s="61" t="n">
+        <v>-0.000559880029657381</v>
+      </c>
+      <c r="C61" s="61" t="n">
+        <v>-0.00233626147465881</v>
+      </c>
+      <c r="D61" s="61" t="n">
+        <v>-0.000695531714879928</v>
+      </c>
+      <c r="E61" s="61" t="n">
+        <v>-0.00310784073230535</v>
+      </c>
+      <c r="F61" s="81" t="n">
+        <v>-0.000626854569880979</v>
+      </c>
+      <c r="G61" s="81" t="n">
+        <v>-0.00259781641726194</v>
+      </c>
+      <c r="H61" s="81" t="n">
+        <v>-0.000661783668595696</v>
+      </c>
+      <c r="I61" s="81" t="n">
+        <v>-0.00312576526944782</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B62" s="61" t="n">
+        <v>-0.00146725153186042</v>
+      </c>
+      <c r="C62" s="61" t="n">
+        <v>-0.00318400565127745</v>
+      </c>
+      <c r="D62" s="61" t="n">
+        <v>-0.000695531714879928</v>
+      </c>
+      <c r="E62" s="61" t="n">
+        <v>-0.00310889176828074</v>
+      </c>
+      <c r="F62" s="81" t="n">
+        <v>-0.00152484853061883</v>
+      </c>
+      <c r="G62" s="81" t="n">
+        <v>-0.00343903530083687</v>
+      </c>
+      <c r="H62" s="81" t="n">
+        <v>-0.000661783668595696</v>
+      </c>
+      <c r="I62" s="81" t="n">
+        <v>-0.00312578159707235</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B63" s="62" t="n">
+        <v>-0.0158350869771286</v>
+      </c>
+      <c r="C63" s="62" t="n">
+        <v>-0.0174092615935918</v>
+      </c>
+      <c r="D63" s="62" t="n">
+        <v>-0.000695531714879928</v>
+      </c>
+      <c r="E63" s="62" t="n">
+        <v>-0.00310889176828074</v>
+      </c>
+      <c r="F63" s="82" t="n">
+        <v>-0.0158316400841852</v>
+      </c>
+      <c r="G63" s="82" t="n">
+        <v>-0.018051215658962</v>
+      </c>
+      <c r="H63" s="82" t="n">
+        <v>-0.000661783668595696</v>
+      </c>
+      <c r="I63" s="82" t="n">
+        <v>-0.00312578159707235</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D67" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E67" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G67" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H67" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I67" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="32" t="n">
+        <v>1E-010</v>
+      </c>
+      <c r="B68" s="79" t="n">
+        <f aca="false">B54/2.78301018765889</f>
+        <v>-0.000145883763583264</v>
+      </c>
+      <c r="C68" s="79" t="n">
+        <f aca="false">C54/2.78216724261881</f>
+        <v>-0.000757305367541435</v>
+      </c>
+      <c r="D68" s="79" t="n">
+        <f aca="false">D54/0.001115089567007</f>
+        <v>-0.622594949741754</v>
+      </c>
+      <c r="E68" s="79" t="n">
+        <f aca="false">E54/0.006561434337706</f>
+        <v>-0.470435081150251</v>
+      </c>
+      <c r="F68" s="79" t="n">
+        <f aca="false">F54/2.75877874258439</f>
+        <v>-0.000171534306699024</v>
+      </c>
+      <c r="G68" s="79" t="n">
+        <f aca="false">G54/2.77938916853549</f>
+        <v>-0.000808908771676211</v>
+      </c>
+      <c r="H68" s="79" t="n">
+        <f aca="false">H54/0.001996081508997</f>
+        <v>-0.333057242114075</v>
+      </c>
+      <c r="I68" s="79" t="n">
+        <f aca="false">I54/0.005768856219016</f>
+        <v>-0.537675174721103</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="32" t="n">
+        <v>1E-009</v>
+      </c>
+      <c r="B69" s="79" t="n">
+        <f aca="false">B55/2.78301018765889</f>
+        <v>-0.000145883763584562</v>
+      </c>
+      <c r="C69" s="79" t="n">
+        <f aca="false">C55/2.78216724261881</f>
+        <v>-0.000757305367541847</v>
+      </c>
+      <c r="D69" s="79" t="n">
+        <f aca="false">D55/0.001115089567007</f>
+        <v>-0.622594949742771</v>
+      </c>
+      <c r="E69" s="79" t="n">
+        <f aca="false">E55/0.006561434337706</f>
+        <v>-0.470435081150451</v>
+      </c>
+      <c r="F69" s="79" t="n">
+        <f aca="false">F55/2.75877874258439</f>
+        <v>-0.000171534312823162</v>
+      </c>
+      <c r="G69" s="79" t="n">
+        <f aca="false">G55/2.77938916853549</f>
+        <v>-0.000808908825825368</v>
+      </c>
+      <c r="H69" s="79" t="n">
+        <f aca="false">H55/0.001996081508997</f>
+        <v>-0.333057192140083</v>
+      </c>
+      <c r="I69" s="79" t="n">
+        <f aca="false">I55/0.005768856219016</f>
+        <v>-0.53767516083746</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="32" t="n">
+        <v>1E-008</v>
+      </c>
+      <c r="B70" s="79" t="n">
+        <f aca="false">B56/2.78301018765889</f>
+        <v>-0.000145883763682877</v>
+      </c>
+      <c r="C70" s="79" t="n">
+        <f aca="false">C56/2.78216724261881</f>
+        <v>-0.000757305367583061</v>
+      </c>
+      <c r="D70" s="79" t="n">
+        <f aca="false">D56/0.001115089567007</f>
+        <v>-0.622594949844516</v>
+      </c>
+      <c r="E70" s="79" t="n">
+        <f aca="false">E56/0.006561434337706</f>
+        <v>-0.47043508117048</v>
+      </c>
+      <c r="F70" s="79" t="n">
+        <f aca="false">F56/2.75877874258439</f>
+        <v>-0.000171534374167898</v>
+      </c>
+      <c r="G70" s="79" t="n">
+        <f aca="false">G56/2.77938916853549</f>
+        <v>-0.000808909367029227</v>
+      </c>
+      <c r="H70" s="79" t="n">
+        <f aca="false">H56/0.001996081508997</f>
+        <v>-0.333056692442982</v>
+      </c>
+      <c r="I70" s="79" t="n">
+        <f aca="false">I56/0.005768856219016</f>
+        <v>-0.537675022059276</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="32" t="n">
+        <v>1E-007</v>
+      </c>
+      <c r="B71" s="79" t="n">
+        <f aca="false">B57/2.78301018765889</f>
+        <v>-0.000145883773200066</v>
+      </c>
+      <c r="C71" s="79" t="n">
+        <f aca="false">C57/2.78216724261881</f>
+        <v>-0.000757305371707898</v>
+      </c>
+      <c r="D71" s="79" t="n">
+        <f aca="false">D57/0.001115089567007</f>
+        <v>-0.622594960019019</v>
+      </c>
+      <c r="E71" s="79" t="n">
+        <f aca="false">E57/0.006561434337706</f>
+        <v>-0.470435083173358</v>
+      </c>
+      <c r="F71" s="79" t="n">
+        <f aca="false">F57/2.75877874258439</f>
+        <v>-0.000171534997950768</v>
+      </c>
+      <c r="G71" s="79" t="n">
+        <f aca="false">G57/2.77938916853549</f>
+        <v>-0.0008089147065019</v>
+      </c>
+      <c r="H71" s="79" t="n">
+        <f aca="false">H57/0.001996081508997</f>
+        <v>-0.333051699460778</v>
+      </c>
+      <c r="I71" s="79" t="n">
+        <f aca="false">I57/0.005768856219016</f>
+        <v>-0.537673639047684</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="32" t="n">
+        <v>1E-006</v>
+      </c>
+      <c r="B72" s="79" t="n">
+        <f aca="false">B58/2.78301018765889</f>
+        <v>-0.000145884721771438</v>
+      </c>
+      <c r="C72" s="79" t="n">
+        <f aca="false">C58/2.78216724261881</f>
+        <v>-0.000757305783813375</v>
+      </c>
+      <c r="D72" s="79" t="n">
+        <f aca="false">D58/0.001115089567007</f>
+        <v>-0.622595865516121</v>
+      </c>
+      <c r="E72" s="79" t="n">
+        <f aca="false">E58/0.006561434337706</f>
+        <v>-0.470435283452908</v>
+      </c>
+      <c r="F72" s="79" t="n">
+        <f aca="false">F58/2.75877874258439</f>
+        <v>-0.000171542270186075</v>
+      </c>
+      <c r="G72" s="79" t="n">
+        <f aca="false">G58/2.77938916853549</f>
+        <v>-0.000808969345880765</v>
+      </c>
+      <c r="H72" s="79" t="n">
+        <f aca="false">H58/0.001996081508997</f>
+        <v>-0.333006638350611</v>
+      </c>
+      <c r="I72" s="79" t="n">
+        <f aca="false">I58/0.005768856219016</f>
+        <v>-0.537660303494242</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="32" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="B73" s="79" t="n">
+        <f aca="false">B59/2.78301018765889</f>
+        <v>-0.000145923801479004</v>
+      </c>
+      <c r="C73" s="79" t="n">
+        <f aca="false">C59/2.78216724261881</f>
+        <v>-0.000757346984373617</v>
+      </c>
+      <c r="D73" s="79" t="n">
+        <f aca="false">D59/0.001115089567007</f>
+        <v>-0.62267137089368</v>
+      </c>
+      <c r="E73" s="79" t="n">
+        <f aca="false">E59/0.006561434337706</f>
+        <v>-0.470455312452707</v>
+      </c>
+      <c r="F73" s="79" t="n">
+        <f aca="false">F59/2.75877874258439</f>
+        <v>-0.000171653858743442</v>
+      </c>
+      <c r="G73" s="79" t="n">
+        <f aca="false">G59/2.77938916853549</f>
+        <v>-0.000809542532717842</v>
+      </c>
+      <c r="H73" s="79" t="n">
+        <f aca="false">H59/0.001996081508997</f>
+        <v>-0.332571034984612</v>
+      </c>
+      <c r="I73" s="79" t="n">
+        <f aca="false">I59/0.005768856219016</f>
+        <v>-0.537576890385615</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="32" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="B74" s="79" t="n">
+        <f aca="false">B60/2.78301018765889</f>
+        <v>-0.000148304567764968</v>
+      </c>
+      <c r="C74" s="79" t="n">
+        <f aca="false">C60/2.78216724261881</f>
+        <v>-0.00076114977180769</v>
+      </c>
+      <c r="D74" s="79" t="n">
+        <f aca="false">D60/0.001115089567007</f>
+        <v>-0.623103228932359</v>
+      </c>
+      <c r="E74" s="79" t="n">
+        <f aca="false">E60/0.006561434337706</f>
+        <v>-0.471743449078743</v>
+      </c>
+      <c r="F74" s="79" t="n">
+        <f aca="false">F60/2.75877874258439</f>
+        <v>-0.000174766339860808</v>
+      </c>
+      <c r="G74" s="79" t="n">
+        <f aca="false">G60/2.77938916853549</f>
+        <v>-0.00081802763292281</v>
+      </c>
+      <c r="H74" s="79" t="n">
+        <f aca="false">H60/0.001996081508997</f>
+        <v>-0.331674140558039</v>
+      </c>
+      <c r="I74" s="79" t="n">
+        <f aca="false">I60/0.005768856219016</f>
+        <v>-0.539456945220016</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="32" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="B75" s="79" t="n">
+        <f aca="false">B61/2.78301018765889</f>
+        <v>-0.000201177858471428</v>
+      </c>
+      <c r="C75" s="79" t="n">
+        <f aca="false">C61/2.78216724261881</f>
+        <v>-0.000839727187809071</v>
+      </c>
+      <c r="D75" s="79" t="n">
+        <f aca="false">D61/0.001115089567007</f>
+        <v>-0.623745155061218</v>
+      </c>
+      <c r="E75" s="79" t="n">
+        <f aca="false">E61/0.006561434337706</f>
+        <v>-0.473652645496397</v>
+      </c>
+      <c r="F75" s="79" t="n">
+        <f aca="false">F61/2.75877874258439</f>
+        <v>-0.000227221763095706</v>
+      </c>
+      <c r="G75" s="79" t="n">
+        <f aca="false">G61/2.77938916853549</f>
+        <v>-0.000934671706528516</v>
+      </c>
+      <c r="H75" s="79" t="n">
+        <f aca="false">H61/0.001996081508997</f>
+        <v>-0.331541405304753</v>
+      </c>
+      <c r="I75" s="79" t="n">
+        <f aca="false">I61/0.005768856219016</f>
+        <v>-0.541834490369909</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="B76" s="79" t="n">
+        <f aca="false">B62/2.78301018765889</f>
+        <v>-0.000527217449065356</v>
+      </c>
+      <c r="C76" s="79" t="n">
+        <f aca="false">C62/2.78216724261881</f>
+        <v>-0.00114443359209434</v>
+      </c>
+      <c r="D76" s="79" t="n">
+        <f aca="false">D62/0.001115089567007</f>
+        <v>-0.623745155061218</v>
+      </c>
+      <c r="E76" s="79" t="n">
+        <f aca="false">E62/0.006561434337706</f>
+        <v>-0.473812829371034</v>
+      </c>
+      <c r="F76" s="79" t="n">
+        <f aca="false">F62/2.75877874258439</f>
+        <v>-0.000552725924366943</v>
+      </c>
+      <c r="G76" s="79" t="n">
+        <f aca="false">G62/2.77938916853549</f>
+        <v>-0.00123733492947623</v>
+      </c>
+      <c r="H76" s="79" t="n">
+        <f aca="false">H62/0.001996081508997</f>
+        <v>-0.331541405304753</v>
+      </c>
+      <c r="I76" s="79" t="n">
+        <f aca="false">I62/0.005768856219016</f>
+        <v>-0.541837320675245</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B77" s="79" t="n">
+        <f aca="false">B63/2.78301018765889</f>
+        <v>-0.00568991340647924</v>
+      </c>
+      <c r="C77" s="79" t="n">
+        <f aca="false">C63/2.78216724261881</f>
+        <v>-0.00625744611140081</v>
+      </c>
+      <c r="D77" s="79" t="n">
+        <f aca="false">D63/0.001115089567007</f>
+        <v>-0.623745155061218</v>
+      </c>
+      <c r="E77" s="79" t="n">
+        <f aca="false">E63/0.006561434337706</f>
+        <v>-0.473812829371034</v>
+      </c>
+      <c r="F77" s="79" t="n">
+        <f aca="false">F63/2.75877874258439</f>
+        <v>-0.00573864073976237</v>
+      </c>
+      <c r="G77" s="79" t="n">
+        <f aca="false">G63/2.77938916853549</f>
+        <v>-0.00649467007474649</v>
+      </c>
+      <c r="H77" s="79" t="n">
+        <f aca="false">H63/0.001996081508997</f>
+        <v>-0.331541405304753</v>
+      </c>
+      <c r="I77" s="79" t="n">
+        <f aca="false">I63/0.005768856219016</f>
+        <v>-0.541837320675245</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="78"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C80" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G80" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H80" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I80" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="B81" s="59" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C81" s="59" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D81" s="59" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E81" s="59" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F81" s="80" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G81" s="80" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H81" s="80" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I81" s="80" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="32" t="n">
+        <v>100</v>
+      </c>
+      <c r="B82" s="61" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C82" s="61" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D82" s="61" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E82" s="61" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F82" s="81" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G82" s="81" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H82" s="81" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I82" s="81" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B83" s="61" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C83" s="61" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D83" s="61" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E83" s="61" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F83" s="81" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G83" s="81" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H83" s="81" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I83" s="81" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B84" s="61" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C84" s="61" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D84" s="61" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E84" s="61" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F84" s="81" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G84" s="81" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H84" s="81" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I84" s="81" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="32" t="n">
+        <v>100000</v>
+      </c>
+      <c r="B85" s="61" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C85" s="61" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D85" s="61" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E85" s="61" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F85" s="81" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G85" s="81" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H85" s="81" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I85" s="81" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="32" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B86" s="61" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C86" s="61" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D86" s="61" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E86" s="61" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F86" s="81" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G86" s="81" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H86" s="81" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I86" s="81" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="32" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="B87" s="62" t="n">
+        <v>-0.00207110417827738</v>
+      </c>
+      <c r="C87" s="62" t="n">
+        <v>-0.00376889927536114</v>
+      </c>
+      <c r="D87" s="62" t="n">
+        <v>-0.000694699210113574</v>
+      </c>
+      <c r="E87" s="62" t="n">
+        <v>-0.00309414453921313</v>
+      </c>
+      <c r="F87" s="82" t="n">
+        <v>-0.00213051899388586</v>
+      </c>
+      <c r="G87" s="82" t="n">
+        <v>-0.00398532663178225</v>
+      </c>
+      <c r="H87" s="82" t="n">
+        <v>-0.000663517226047069</v>
+      </c>
+      <c r="I87" s="82" t="n">
+        <v>-0.00310993400718929</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="E91" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F91" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="G91" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="H91" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="I91" s="71" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="78" t="n">
+        <v>10</v>
+      </c>
+      <c r="B92" s="79" t="n">
+        <f aca="false">B81/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C92" s="79" t="n">
+        <f aca="false">C81/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D92" s="79" t="n">
+        <f aca="false">D81/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">E81/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F92" s="79" t="n">
+        <f aca="false">F81/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G92" s="79" t="n">
+        <f aca="false">G81/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H92" s="79" t="n">
+        <f aca="false">H81/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <f aca="false">I81/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="32" t="n">
+        <v>100</v>
+      </c>
+      <c r="B93" s="79" t="n">
+        <f aca="false">B82/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C93" s="79" t="n">
+        <f aca="false">C82/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D93" s="79" t="n">
+        <f aca="false">D82/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">E82/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F93" s="79" t="n">
+        <f aca="false">F82/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G93" s="79" t="n">
+        <f aca="false">G82/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H93" s="79" t="n">
+        <f aca="false">H82/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <f aca="false">I82/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B94" s="79" t="n">
+        <f aca="false">B83/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C94" s="79" t="n">
+        <f aca="false">C83/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D94" s="79" t="n">
+        <f aca="false">D83/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <f aca="false">E83/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F94" s="79" t="n">
+        <f aca="false">F83/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G94" s="79" t="n">
+        <f aca="false">G83/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H94" s="79" t="n">
+        <f aca="false">H83/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <f aca="false">I83/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="32" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B95" s="79" t="n">
+        <f aca="false">B84/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C95" s="79" t="n">
+        <f aca="false">C84/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D95" s="79" t="n">
+        <f aca="false">D84/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <f aca="false">E84/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F95" s="79" t="n">
+        <f aca="false">F84/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G95" s="79" t="n">
+        <f aca="false">G84/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H95" s="79" t="n">
+        <f aca="false">H84/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <f aca="false">I84/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="32" t="n">
+        <v>100000</v>
+      </c>
+      <c r="B96" s="79" t="n">
+        <f aca="false">B85/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C96" s="79" t="n">
+        <f aca="false">C85/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D96" s="79" t="n">
+        <f aca="false">D85/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <f aca="false">E85/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F96" s="79" t="n">
+        <f aca="false">F85/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G96" s="79" t="n">
+        <f aca="false">G85/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H96" s="79" t="n">
+        <f aca="false">H85/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I96" s="0" t="n">
+        <f aca="false">I85/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="32" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B97" s="79" t="n">
+        <f aca="false">B86/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C97" s="79" t="n">
+        <f aca="false">C86/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D97" s="79" t="n">
+        <f aca="false">D86/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <f aca="false">E86/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F97" s="79" t="n">
+        <f aca="false">F86/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G97" s="79" t="n">
+        <f aca="false">G86/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H97" s="79" t="n">
+        <f aca="false">H86/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I97" s="0" t="n">
+        <f aca="false">I86/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="32" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="B98" s="79" t="n">
+        <f aca="false">B87/2.78301018765889</f>
+        <v>-0.00074419568690822</v>
+      </c>
+      <c r="C98" s="79" t="n">
+        <f aca="false">C87/2.78216724261881</f>
+        <v>-0.00135466309056731</v>
+      </c>
+      <c r="D98" s="79" t="n">
+        <f aca="false">D87/0.001115089567007</f>
+        <v>-0.622998573987387</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <f aca="false">E87/0.006561434337706</f>
+        <v>-0.471565267586736</v>
+      </c>
+      <c r="F98" s="79" t="n">
+        <f aca="false">F87/2.75877874258439</f>
+        <v>-0.000772268888765619</v>
+      </c>
+      <c r="G98" s="79" t="n">
+        <f aca="false">G87/2.77938916853549</f>
+        <v>-0.00143388578933054</v>
+      </c>
+      <c r="H98" s="79" t="n">
+        <f aca="false">H87/0.001996081508997</f>
+        <v>-0.332409885596544</v>
+      </c>
+      <c r="I98" s="0" t="n">
+        <f aca="false">I87/0.005768856219016</f>
+        <v>-0.53909022674858</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28418,7 +31131,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="71" width="7.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="71" width="10.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="71" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="71" width="7.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="71" width="9.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="71" width="9.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="71" width="7.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="71" width="10.15"/>
@@ -28429,95 +31142,95 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73" t="s">
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73" t="s">
+      <c r="I2" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="73" t="s">
+      <c r="N2" s="84" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="72"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="74" t="s">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="83"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="74" t="s">
+      <c r="E3" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+    </row>
+    <row r="4" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="71" t="s">
         <v>58</v>
-      </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="74" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-    </row>
-    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="71" t="s">
-        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>26</v>
@@ -28529,21 +31242,21 @@
         <v>100</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G4" s="71" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H4" s="71" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="I4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="73"/>
+    <row r="5" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="84"/>
       <c r="B5" s="0"/>
       <c r="C5" s="71" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D5" s="71" t="n">
         <v>1000</v>
@@ -28552,20 +31265,20 @@
         <v>100</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G5" s="71" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H5" s="71" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="0"/>
       <c r="C6" s="71" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D6" s="71" t="n">
         <v>1000</v>
@@ -28574,20 +31287,20 @@
         <v>500</v>
       </c>
       <c r="F6" s="71" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G6" s="71" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="H6" s="71" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0"/>
       <c r="B7" s="0"/>
       <c r="C7" s="71" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D7" s="71" t="n">
         <v>1000</v>
@@ -28596,19 +31309,19 @@
         <v>100</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G7" s="71" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="H7" s="71" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="73"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="71" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>26</v>
@@ -28620,42 +31333,111 @@
         <v>100</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G8" s="71" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H8" s="71" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="73"/>
+      <c r="C9" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="71" t="n">
+        <v>500</v>
+      </c>
+      <c r="F9" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="84"/>
       <c r="B10" s="71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="71" t="n">
+        <v>100</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="37.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="84"/>
+      <c r="C11" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="71" t="n">
+        <v>100</v>
+      </c>
+      <c r="F11" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="84"/>
+      <c r="C12" s="71" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="71" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="72" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="71" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="71" t="s">
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="84"/>
+      <c r="C13" s="71" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="71" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="71" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="71" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing LSTM hyperparameter: number of neurons in the first layer
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Findings" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="105">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -361,7 +361,7 @@
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -389,6 +389,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1069,7 +1074,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -1100,10 +1105,10 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -1114,6 +1119,391 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$A$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>training error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$B$42:$H$42</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LSTM Model Summary'!$B$54:$H$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0457291</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0459124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0326236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0292324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0326041</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.030956</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0327057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$A$67</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>testing error</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$B$42:$H$42</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LSTM Model Summary'!$B$67:$H$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0168092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0154849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0145865</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0147008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0185102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0265924</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0150265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="48689626"/>
+        <c:axId val="83384776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="48689626"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="83384776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="83384776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="48689626"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>66960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>232200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>58680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6367680" y="9494640"/>
+        <a:ext cx="5762880" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28519,7 +28909,7 @@
   </sheetPr>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -29825,8 +30215,8 @@
   </sheetPr>
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32502,10 +32892,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32825,6 +33215,615 @@
         <v>54</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C42" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="D42" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="E42" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="F42" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="G42" s="74" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H42" s="74" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B43" s="74" t="n">
+        <v>0.02833</v>
+      </c>
+      <c r="C43" s="74" t="n">
+        <v>0.02814</v>
+      </c>
+      <c r="D43" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="E43" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="F43" s="74" t="n">
+        <v>0.036522</v>
+      </c>
+      <c r="G43" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="H43" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" s="74" t="n">
+        <v>0.080614</v>
+      </c>
+      <c r="C44" s="74" t="n">
+        <v>0.028199</v>
+      </c>
+      <c r="D44" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="E44" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="F44" s="74" t="n">
+        <v>0.02837</v>
+      </c>
+      <c r="G44" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="H44" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="74" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="C45" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="D45" s="74" t="n">
+        <v>0.028044</v>
+      </c>
+      <c r="E45" s="74" t="n">
+        <v>0.028215</v>
+      </c>
+      <c r="F45" s="74" t="n">
+        <v>0.036798</v>
+      </c>
+      <c r="G45" s="74" t="n">
+        <v>0.03302</v>
+      </c>
+      <c r="H45" s="74" t="n">
+        <v>0.036603</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="74" t="n">
+        <v>3</v>
+      </c>
+      <c r="B46" s="74" t="n">
+        <v>0.080458</v>
+      </c>
+      <c r="C46" s="74" t="n">
+        <v>0.028156</v>
+      </c>
+      <c r="D46" s="74" t="n">
+        <v>0.03354</v>
+      </c>
+      <c r="E46" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="F46" s="74" t="n">
+        <v>0.028123</v>
+      </c>
+      <c r="G46" s="74" t="n">
+        <v>0.032551</v>
+      </c>
+      <c r="H46" s="74" t="n">
+        <v>0.028249</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="74" t="n">
+        <v>4</v>
+      </c>
+      <c r="B47" s="74" t="n">
+        <v>0.029231</v>
+      </c>
+      <c r="C47" s="74" t="n">
+        <v>0.069067</v>
+      </c>
+      <c r="D47" s="74" t="n">
+        <v>0.0344</v>
+      </c>
+      <c r="E47" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="F47" s="74" t="n">
+        <v>0.036373</v>
+      </c>
+      <c r="G47" s="74" t="n">
+        <v>0.028156</v>
+      </c>
+      <c r="H47" s="74" t="n">
+        <v>0.035853</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B48" s="74" t="n">
+        <v>0.028125</v>
+      </c>
+      <c r="C48" s="74" t="n">
+        <v>0.028125</v>
+      </c>
+      <c r="D48" s="74" t="n">
+        <v>0.028119</v>
+      </c>
+      <c r="E48" s="74" t="n">
+        <v>0.038939</v>
+      </c>
+      <c r="F48" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="G48" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="H48" s="74" t="n">
+        <v>0.039457</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="74" t="n">
+        <v>6</v>
+      </c>
+      <c r="B49" s="74" t="n">
+        <v>0.028116</v>
+      </c>
+      <c r="C49" s="74" t="n">
+        <v>0.088619</v>
+      </c>
+      <c r="D49" s="74" t="n">
+        <v>0.028265</v>
+      </c>
+      <c r="E49" s="74" t="n">
+        <v>0.028215</v>
+      </c>
+      <c r="F49" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="G49" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="H49" s="74" t="n">
+        <v>0.028131</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="74" t="n">
+        <v>7</v>
+      </c>
+      <c r="B50" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="C50" s="74" t="n">
+        <v>0.10432</v>
+      </c>
+      <c r="D50" s="74" t="n">
+        <v>0.061364</v>
+      </c>
+      <c r="E50" s="74" t="n">
+        <v>0.028211</v>
+      </c>
+      <c r="F50" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="G50" s="74" t="n">
+        <v>0.042408</v>
+      </c>
+      <c r="H50" s="74" t="n">
+        <v>0.04624</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="74" t="n">
+        <v>8</v>
+      </c>
+      <c r="B51" s="74" t="n">
+        <v>0.098039</v>
+      </c>
+      <c r="C51" s="74" t="n">
+        <v>0.028246</v>
+      </c>
+      <c r="D51" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="E51" s="74" t="n">
+        <v>0.028084</v>
+      </c>
+      <c r="F51" s="74" t="n">
+        <v>0.044039</v>
+      </c>
+      <c r="G51" s="74" t="n">
+        <v>0.032711</v>
+      </c>
+      <c r="H51" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="74" t="n">
+        <v>9</v>
+      </c>
+      <c r="B52" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="C52" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="D52" s="74" t="n">
+        <v>0.028126</v>
+      </c>
+      <c r="E52" s="74" t="n">
+        <v>0.028156</v>
+      </c>
+      <c r="F52" s="74" t="n">
+        <v>0.031438</v>
+      </c>
+      <c r="G52" s="74" t="n">
+        <v>0.02821</v>
+      </c>
+      <c r="H52" s="74" t="n">
+        <v>0.028146</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="74" t="n">
+        <f aca="false">AVERAGE(B43:B52)</f>
+        <v>0.0457291</v>
+      </c>
+      <c r="C54" s="74" t="n">
+        <f aca="false">AVERAGE(C43:C52)</f>
+        <v>0.0459124</v>
+      </c>
+      <c r="D54" s="74" t="n">
+        <f aca="false">AVERAGE(D43:D52)</f>
+        <v>0.0326236</v>
+      </c>
+      <c r="E54" s="74" t="n">
+        <f aca="false">AVERAGE(E43:E52)</f>
+        <v>0.0292324</v>
+      </c>
+      <c r="F54" s="74" t="n">
+        <f aca="false">AVERAGE(F43:F52)</f>
+        <v>0.0326041</v>
+      </c>
+      <c r="G54" s="74" t="n">
+        <f aca="false">AVERAGE(G43:G52)</f>
+        <v>0.030956</v>
+      </c>
+      <c r="H54" s="74" t="n">
+        <f aca="false">AVERAGE(H43:H52)</f>
+        <v>0.0327057</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B56" s="74" t="n">
+        <v>0.014387</v>
+      </c>
+      <c r="C56" s="74" t="n">
+        <v>0.015725</v>
+      </c>
+      <c r="D56" s="74" t="n">
+        <v>0.014463</v>
+      </c>
+      <c r="E56" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="F56" s="74" t="n">
+        <v>0.014454</v>
+      </c>
+      <c r="G56" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H56" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" s="74" t="n">
+        <v>0.016235</v>
+      </c>
+      <c r="C57" s="74" t="n">
+        <v>0.014709</v>
+      </c>
+      <c r="D57" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="E57" s="74" t="n">
+        <v>0.014449</v>
+      </c>
+      <c r="F57" s="74" t="n">
+        <v>0.014527</v>
+      </c>
+      <c r="G57" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H57" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="74" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="C58" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="D58" s="74" t="n">
+        <v>0.014447</v>
+      </c>
+      <c r="E58" s="74" t="n">
+        <v>0.015715</v>
+      </c>
+      <c r="F58" s="74" t="n">
+        <v>0.014383</v>
+      </c>
+      <c r="G58" s="74" t="n">
+        <v>0.014451</v>
+      </c>
+      <c r="H58" s="74" t="n">
+        <v>0.014484</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="74" t="n">
+        <v>3</v>
+      </c>
+      <c r="B59" s="74" t="n">
+        <v>0.02234</v>
+      </c>
+      <c r="C59" s="74" t="n">
+        <v>0.016193</v>
+      </c>
+      <c r="D59" s="74" t="n">
+        <v>0.014435</v>
+      </c>
+      <c r="E59" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="F59" s="74" t="n">
+        <v>0.014443</v>
+      </c>
+      <c r="G59" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H59" s="74" t="n">
+        <v>0.019651</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="74" t="n">
+        <v>4</v>
+      </c>
+      <c r="B60" s="74" t="n">
+        <v>0.014414</v>
+      </c>
+      <c r="C60" s="74" t="n">
+        <v>0.014638</v>
+      </c>
+      <c r="D60" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="E60" s="74" t="n">
+        <v>0.014618</v>
+      </c>
+      <c r="F60" s="74" t="n">
+        <v>0.052725</v>
+      </c>
+      <c r="G60" s="74" t="n">
+        <v>0.014525</v>
+      </c>
+      <c r="H60" s="74" t="n">
+        <v>0.014637</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B61" s="74" t="n">
+        <v>0.022387</v>
+      </c>
+      <c r="C61" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="D61" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="E61" s="74" t="n">
+        <v>0.014522</v>
+      </c>
+      <c r="F61" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="G61" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H61" s="74" t="n">
+        <v>0.014515</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="74" t="n">
+        <v>6</v>
+      </c>
+      <c r="B62" s="74" t="n">
+        <v>0.014442</v>
+      </c>
+      <c r="C62" s="74" t="n">
+        <v>0.016691</v>
+      </c>
+      <c r="D62" s="74" t="n">
+        <v>0.014667</v>
+      </c>
+      <c r="E62" s="74" t="n">
+        <v>0.014718</v>
+      </c>
+      <c r="F62" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="G62" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H62" s="74" t="n">
+        <v>0.01446</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="74" t="n">
+        <v>7</v>
+      </c>
+      <c r="B63" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="C63" s="74" t="n">
+        <v>0.019091</v>
+      </c>
+      <c r="D63" s="74" t="n">
+        <v>0.015517</v>
+      </c>
+      <c r="E63" s="74" t="n">
+        <v>0.014727</v>
+      </c>
+      <c r="F63" s="74" t="n">
+        <v>0.014611</v>
+      </c>
+      <c r="G63" s="74" t="n">
+        <v>0.134489</v>
+      </c>
+      <c r="H63" s="74" t="n">
+        <v>0.014674</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="74" t="n">
+        <v>8</v>
+      </c>
+      <c r="B64" s="74" t="n">
+        <v>0.020567</v>
+      </c>
+      <c r="C64" s="74" t="n">
+        <v>0.014482</v>
+      </c>
+      <c r="D64" s="74" t="n">
+        <v>0.014503</v>
+      </c>
+      <c r="E64" s="74" t="n">
+        <v>0.014854</v>
+      </c>
+      <c r="F64" s="74" t="n">
+        <v>0.016596</v>
+      </c>
+      <c r="G64" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="H64" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="74" t="n">
+        <v>9</v>
+      </c>
+      <c r="B65" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="C65" s="74" t="n">
+        <v>0.01444</v>
+      </c>
+      <c r="D65" s="74" t="n">
+        <v>0.014513</v>
+      </c>
+      <c r="E65" s="74" t="n">
+        <v>0.014525</v>
+      </c>
+      <c r="F65" s="74" t="n">
+        <v>0.014483</v>
+      </c>
+      <c r="G65" s="74" t="n">
+        <v>0.015819</v>
+      </c>
+      <c r="H65" s="74" t="n">
+        <v>0.014524</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="74" t="n">
+        <f aca="false">AVERAGE(B56:B65)</f>
+        <v>0.0168092</v>
+      </c>
+      <c r="C67" s="74" t="n">
+        <f aca="false">AVERAGE(C56:C65)</f>
+        <v>0.0154849</v>
+      </c>
+      <c r="D67" s="74" t="n">
+        <f aca="false">AVERAGE(D56:D65)</f>
+        <v>0.0145865</v>
+      </c>
+      <c r="E67" s="74" t="n">
+        <f aca="false">AVERAGE(E56:E65)</f>
+        <v>0.0147008</v>
+      </c>
+      <c r="F67" s="74" t="n">
+        <f aca="false">AVERAGE(F56:F65)</f>
+        <v>0.0185102</v>
+      </c>
+      <c r="G67" s="74" t="n">
+        <f aca="false">AVERAGE(G56:G65)</f>
+        <v>0.0265924</v>
+      </c>
+      <c r="H67" s="74" t="n">
+        <f aca="false">AVERAGE(H56:H65)</f>
+        <v>0.0150265</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:A3"/>
@@ -32845,5 +33844,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
further testing one layer LSTM
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="107">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t xml:space="preserve">XGBoost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epochs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neuron</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1127,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1344,11 +1350,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="48689626"/>
-        <c:axId val="83384776"/>
+        <c:axId val="26040118"/>
+        <c:axId val="66009402"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48689626"/>
+        <c:axId val="26040118"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,14 +1389,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83384776"/>
+        <c:crossAx val="66009402"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83384776"/>
+        <c:axId val="66009402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,7 +1440,393 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48689626"/>
+        <c:crossAx val="26040118"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>train</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$B$74:$K$74</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LSTM Model Summary'!$B$90:$K$90</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.060303</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0519143333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0487313333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.061029</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0727306666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.074754</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0554596666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0829643333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.056543</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0558636666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>test</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$B$74:$K$74</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LSTM Model Summary'!$B$114:$K$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0150163333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.014533</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.014581</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0157726666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0359723333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.015442</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.017229</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0317283333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0327083333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0204486666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="76693369"/>
+        <c:axId val="89486080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="76693369"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="89486080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89486080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="76693369"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1498,6 +1890,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>462240</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>145080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>480600</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>51480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8251560" y="15837120"/>
+        <a:ext cx="5753160" cy="3240000"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -32892,10 +33314,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33824,6 +34246,1444 @@
         <v>0.0150265</v>
       </c>
     </row>
+    <row r="73" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="C74" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="D74" s="74" t="n">
+        <v>150</v>
+      </c>
+      <c r="E74" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="F74" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="G74" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="H74" s="74" t="n">
+        <v>350</v>
+      </c>
+      <c r="I74" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="J74" s="74" t="n">
+        <v>450</v>
+      </c>
+      <c r="K74" s="74" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B75" s="74" t="n">
+        <v>0.041825</v>
+      </c>
+      <c r="C75" s="74" t="n">
+        <v>0.066963</v>
+      </c>
+      <c r="D75" s="74" t="n">
+        <v>0.034672</v>
+      </c>
+      <c r="E75" s="74" t="n">
+        <v>0.060426</v>
+      </c>
+      <c r="F75" s="74" t="n">
+        <v>0.041484</v>
+      </c>
+      <c r="G75" s="74" t="n">
+        <v>0.128101</v>
+      </c>
+      <c r="H75" s="74" t="n">
+        <v>0.036792</v>
+      </c>
+      <c r="I75" s="74" t="n">
+        <v>0.106291</v>
+      </c>
+      <c r="J75" s="74" t="n">
+        <v>0.050515</v>
+      </c>
+      <c r="K75" s="74" t="n">
+        <v>0.07392</v>
+      </c>
+      <c r="L75" s="0"/>
+      <c r="M75" s="0"/>
+      <c r="N75" s="0"/>
+      <c r="O75" s="0"/>
+      <c r="P75" s="0"/>
+      <c r="Q75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="74" t="n">
+        <v>0.060234</v>
+      </c>
+      <c r="C76" s="74" t="n">
+        <v>0.051417</v>
+      </c>
+      <c r="D76" s="74" t="n">
+        <v>0.046023</v>
+      </c>
+      <c r="E76" s="74" t="n">
+        <v>0.07014</v>
+      </c>
+      <c r="F76" s="74" t="n">
+        <v>0.070388</v>
+      </c>
+      <c r="G76" s="74" t="n">
+        <v>0.059395</v>
+      </c>
+      <c r="H76" s="74" t="n">
+        <v>0.073575</v>
+      </c>
+      <c r="I76" s="74" t="n">
+        <v>0.054523</v>
+      </c>
+      <c r="J76" s="74" t="n">
+        <v>0.083121</v>
+      </c>
+      <c r="K76" s="74" t="n">
+        <v>0.03039</v>
+      </c>
+      <c r="L76" s="0"/>
+      <c r="M76" s="0"/>
+      <c r="N76" s="0"/>
+      <c r="O76" s="0"/>
+      <c r="P76" s="0"/>
+      <c r="Q76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="74" t="n">
+        <v>0.07885</v>
+      </c>
+      <c r="C77" s="74" t="n">
+        <v>0.037363</v>
+      </c>
+      <c r="D77" s="74" t="n">
+        <v>0.065499</v>
+      </c>
+      <c r="E77" s="74" t="n">
+        <v>0.052521</v>
+      </c>
+      <c r="F77" s="74" t="n">
+        <v>0.10632</v>
+      </c>
+      <c r="G77" s="74" t="n">
+        <v>0.036766</v>
+      </c>
+      <c r="H77" s="74" t="n">
+        <v>0.056012</v>
+      </c>
+      <c r="I77" s="74" t="n">
+        <v>0.088079</v>
+      </c>
+      <c r="J77" s="74" t="n">
+        <v>0.035993</v>
+      </c>
+      <c r="K77" s="74" t="n">
+        <v>0.063281</v>
+      </c>
+      <c r="L77" s="0"/>
+      <c r="M77" s="0"/>
+      <c r="N77" s="0"/>
+      <c r="O77" s="0"/>
+      <c r="P77" s="0"/>
+      <c r="Q77" s="0"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B78" s="74" t="n">
+        <v>0.041825</v>
+      </c>
+      <c r="C78" s="74" t="n">
+        <v>0.066963</v>
+      </c>
+      <c r="D78" s="74" t="n">
+        <v>0.034672</v>
+      </c>
+      <c r="E78" s="74" t="n">
+        <v>0.060426</v>
+      </c>
+      <c r="F78" s="74" t="n">
+        <v>0.041484</v>
+      </c>
+      <c r="G78" s="74" t="n">
+        <v>0.128101</v>
+      </c>
+      <c r="H78" s="74" t="n">
+        <v>0.036792</v>
+      </c>
+      <c r="I78" s="74" t="n">
+        <v>0.106291</v>
+      </c>
+      <c r="J78" s="74" t="n">
+        <v>0.050515</v>
+      </c>
+      <c r="K78" s="74" t="n">
+        <v>0.07392</v>
+      </c>
+      <c r="L78" s="0"/>
+      <c r="M78" s="0"/>
+      <c r="N78" s="0"/>
+      <c r="O78" s="0"/>
+      <c r="P78" s="0"/>
+      <c r="Q78" s="0"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="74" t="n">
+        <v>0.060234</v>
+      </c>
+      <c r="C79" s="74" t="n">
+        <v>0.051417</v>
+      </c>
+      <c r="D79" s="74" t="n">
+        <v>0.046023</v>
+      </c>
+      <c r="E79" s="74" t="n">
+        <v>0.07014</v>
+      </c>
+      <c r="F79" s="74" t="n">
+        <v>0.070388</v>
+      </c>
+      <c r="G79" s="74" t="n">
+        <v>0.059395</v>
+      </c>
+      <c r="H79" s="74" t="n">
+        <v>0.073575</v>
+      </c>
+      <c r="I79" s="74" t="n">
+        <v>0.054523</v>
+      </c>
+      <c r="J79" s="74" t="n">
+        <v>0.083121</v>
+      </c>
+      <c r="K79" s="74" t="n">
+        <v>0.03039</v>
+      </c>
+      <c r="L79" s="0"/>
+      <c r="M79" s="0"/>
+      <c r="N79" s="0"/>
+      <c r="O79" s="0"/>
+      <c r="P79" s="0"/>
+      <c r="Q79" s="0"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="74" t="n">
+        <v>0.07885</v>
+      </c>
+      <c r="C80" s="74" t="n">
+        <v>0.037363</v>
+      </c>
+      <c r="D80" s="74" t="n">
+        <v>0.065499</v>
+      </c>
+      <c r="E80" s="74" t="n">
+        <v>0.052521</v>
+      </c>
+      <c r="F80" s="74" t="n">
+        <v>0.10632</v>
+      </c>
+      <c r="G80" s="74" t="n">
+        <v>0.036766</v>
+      </c>
+      <c r="H80" s="74" t="n">
+        <v>0.056012</v>
+      </c>
+      <c r="I80" s="74" t="n">
+        <v>0.088079</v>
+      </c>
+      <c r="J80" s="74" t="n">
+        <v>0.035993</v>
+      </c>
+      <c r="K80" s="74" t="n">
+        <v>0.063281</v>
+      </c>
+      <c r="L80" s="0"/>
+      <c r="M80" s="0"/>
+      <c r="N80" s="0"/>
+      <c r="O80" s="0"/>
+      <c r="P80" s="0"/>
+      <c r="Q80" s="0"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B81" s="74" t="n">
+        <v>0.041825</v>
+      </c>
+      <c r="C81" s="74" t="n">
+        <v>0.066963</v>
+      </c>
+      <c r="D81" s="74" t="n">
+        <v>0.034672</v>
+      </c>
+      <c r="E81" s="74" t="n">
+        <v>0.060426</v>
+      </c>
+      <c r="F81" s="74" t="n">
+        <v>0.041484</v>
+      </c>
+      <c r="G81" s="74" t="n">
+        <v>0.128101</v>
+      </c>
+      <c r="H81" s="74" t="n">
+        <v>0.036792</v>
+      </c>
+      <c r="I81" s="74" t="n">
+        <v>0.106291</v>
+      </c>
+      <c r="J81" s="74" t="n">
+        <v>0.050515</v>
+      </c>
+      <c r="K81" s="74" t="n">
+        <v>0.07392</v>
+      </c>
+      <c r="L81" s="0"/>
+      <c r="M81" s="0"/>
+      <c r="N81" s="0"/>
+      <c r="O81" s="0"/>
+      <c r="P81" s="0"/>
+      <c r="Q81" s="0"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="74" t="n">
+        <v>0.060234</v>
+      </c>
+      <c r="C82" s="74" t="n">
+        <v>0.051417</v>
+      </c>
+      <c r="D82" s="74" t="n">
+        <v>0.046023</v>
+      </c>
+      <c r="E82" s="74" t="n">
+        <v>0.07014</v>
+      </c>
+      <c r="F82" s="74" t="n">
+        <v>0.070388</v>
+      </c>
+      <c r="G82" s="74" t="n">
+        <v>0.059395</v>
+      </c>
+      <c r="H82" s="74" t="n">
+        <v>0.073575</v>
+      </c>
+      <c r="I82" s="74" t="n">
+        <v>0.054523</v>
+      </c>
+      <c r="J82" s="74" t="n">
+        <v>0.083121</v>
+      </c>
+      <c r="K82" s="74" t="n">
+        <v>0.03039</v>
+      </c>
+      <c r="L82" s="0"/>
+      <c r="M82" s="0"/>
+      <c r="N82" s="0"/>
+      <c r="O82" s="0"/>
+      <c r="P82" s="0"/>
+      <c r="Q82" s="0"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="74" t="n">
+        <v>0.07885</v>
+      </c>
+      <c r="C83" s="74" t="n">
+        <v>0.037363</v>
+      </c>
+      <c r="D83" s="74" t="n">
+        <v>0.065499</v>
+      </c>
+      <c r="E83" s="74" t="n">
+        <v>0.052521</v>
+      </c>
+      <c r="F83" s="74" t="n">
+        <v>0.10632</v>
+      </c>
+      <c r="G83" s="74" t="n">
+        <v>0.036766</v>
+      </c>
+      <c r="H83" s="74" t="n">
+        <v>0.056012</v>
+      </c>
+      <c r="I83" s="74" t="n">
+        <v>0.088079</v>
+      </c>
+      <c r="J83" s="74" t="n">
+        <v>0.035993</v>
+      </c>
+      <c r="K83" s="74" t="n">
+        <v>0.063281</v>
+      </c>
+      <c r="L83" s="0"/>
+      <c r="M83" s="0"/>
+      <c r="N83" s="0"/>
+      <c r="O83" s="0"/>
+      <c r="P83" s="0"/>
+      <c r="Q83" s="0"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="74" t="n">
+        <v>20</v>
+      </c>
+      <c r="B84" s="74" t="n">
+        <v>0.041825</v>
+      </c>
+      <c r="C84" s="74" t="n">
+        <v>0.066963</v>
+      </c>
+      <c r="D84" s="74" t="n">
+        <v>0.034672</v>
+      </c>
+      <c r="E84" s="74" t="n">
+        <v>0.060426</v>
+      </c>
+      <c r="F84" s="74" t="n">
+        <v>0.041484</v>
+      </c>
+      <c r="G84" s="74" t="n">
+        <v>0.128101</v>
+      </c>
+      <c r="H84" s="74" t="n">
+        <v>0.036792</v>
+      </c>
+      <c r="I84" s="74" t="n">
+        <v>0.106291</v>
+      </c>
+      <c r="J84" s="74" t="n">
+        <v>0.050515</v>
+      </c>
+      <c r="K84" s="74" t="n">
+        <v>0.07392</v>
+      </c>
+      <c r="L84" s="0"/>
+      <c r="M84" s="0"/>
+      <c r="N84" s="0"/>
+      <c r="O84" s="0"/>
+      <c r="P84" s="0"/>
+      <c r="Q84" s="0"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="74" t="n">
+        <v>0.060234</v>
+      </c>
+      <c r="C85" s="74" t="n">
+        <v>0.051417</v>
+      </c>
+      <c r="D85" s="74" t="n">
+        <v>0.046023</v>
+      </c>
+      <c r="E85" s="74" t="n">
+        <v>0.07014</v>
+      </c>
+      <c r="F85" s="74" t="n">
+        <v>0.070388</v>
+      </c>
+      <c r="G85" s="74" t="n">
+        <v>0.059395</v>
+      </c>
+      <c r="H85" s="74" t="n">
+        <v>0.073575</v>
+      </c>
+      <c r="I85" s="74" t="n">
+        <v>0.054523</v>
+      </c>
+      <c r="J85" s="74" t="n">
+        <v>0.083121</v>
+      </c>
+      <c r="K85" s="74" t="n">
+        <v>0.03039</v>
+      </c>
+      <c r="L85" s="0"/>
+      <c r="M85" s="0"/>
+      <c r="N85" s="0"/>
+      <c r="O85" s="0"/>
+      <c r="P85" s="0"/>
+      <c r="Q85" s="0"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="74" t="n">
+        <v>0.07885</v>
+      </c>
+      <c r="C86" s="74" t="n">
+        <v>0.037363</v>
+      </c>
+      <c r="D86" s="74" t="n">
+        <v>0.065499</v>
+      </c>
+      <c r="E86" s="74" t="n">
+        <v>0.052521</v>
+      </c>
+      <c r="F86" s="74" t="n">
+        <v>0.10632</v>
+      </c>
+      <c r="G86" s="74" t="n">
+        <v>0.036766</v>
+      </c>
+      <c r="H86" s="74" t="n">
+        <v>0.056012</v>
+      </c>
+      <c r="I86" s="74" t="n">
+        <v>0.088079</v>
+      </c>
+      <c r="J86" s="74" t="n">
+        <v>0.035993</v>
+      </c>
+      <c r="K86" s="74" t="n">
+        <v>0.063281</v>
+      </c>
+      <c r="L86" s="0"/>
+      <c r="M86" s="0"/>
+      <c r="N86" s="0"/>
+      <c r="O86" s="0"/>
+      <c r="P86" s="0"/>
+      <c r="Q86" s="0"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0"/>
+      <c r="B87" s="0"/>
+      <c r="C87" s="0"/>
+      <c r="D87" s="0"/>
+      <c r="E87" s="0"/>
+      <c r="F87" s="0"/>
+      <c r="G87" s="0"/>
+      <c r="H87" s="0"/>
+      <c r="I87" s="0"/>
+      <c r="J87" s="0"/>
+      <c r="L87" s="0"/>
+      <c r="M87" s="0"/>
+      <c r="N87" s="0"/>
+      <c r="O87" s="0"/>
+      <c r="P87" s="0"/>
+      <c r="Q87" s="0"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0"/>
+      <c r="B88" s="0"/>
+      <c r="C88" s="0"/>
+      <c r="D88" s="0"/>
+      <c r="E88" s="0"/>
+      <c r="F88" s="0"/>
+      <c r="G88" s="0"/>
+      <c r="H88" s="0"/>
+      <c r="I88" s="0"/>
+      <c r="J88" s="0"/>
+      <c r="L88" s="0"/>
+      <c r="M88" s="0"/>
+      <c r="N88" s="0"/>
+      <c r="O88" s="0"/>
+      <c r="P88" s="0"/>
+      <c r="Q88" s="0"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0"/>
+      <c r="B89" s="0"/>
+      <c r="C89" s="0"/>
+      <c r="D89" s="0"/>
+      <c r="E89" s="0"/>
+      <c r="F89" s="0"/>
+      <c r="G89" s="0"/>
+      <c r="H89" s="0"/>
+      <c r="I89" s="0"/>
+      <c r="J89" s="0"/>
+      <c r="L89" s="0"/>
+      <c r="M89" s="0"/>
+      <c r="N89" s="0"/>
+      <c r="O89" s="0"/>
+      <c r="P89" s="0"/>
+      <c r="Q89" s="0"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0"/>
+      <c r="B90" s="0" t="n">
+        <f aca="false">AVERAGE(B75:B77)</f>
+        <v>0.060303</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <f aca="false">AVERAGE(C75:C77)</f>
+        <v>0.0519143333333333</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <f aca="false">AVERAGE(D75:D77)</f>
+        <v>0.0487313333333333</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <f aca="false">AVERAGE(E75:E77)</f>
+        <v>0.061029</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <f aca="false">AVERAGE(F75:F77)</f>
+        <v>0.0727306666666667</v>
+      </c>
+      <c r="G90" s="0" t="n">
+        <f aca="false">AVERAGE(G75:G77)</f>
+        <v>0.074754</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <f aca="false">AVERAGE(H75:H77)</f>
+        <v>0.0554596666666667</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <f aca="false">AVERAGE(I75:I77)</f>
+        <v>0.0829643333333333</v>
+      </c>
+      <c r="J90" s="0" t="n">
+        <f aca="false">AVERAGE(J75:J77)</f>
+        <v>0.056543</v>
+      </c>
+      <c r="K90" s="0" t="n">
+        <f aca="false">AVERAGE(K75:K77)</f>
+        <v>0.0558636666666667</v>
+      </c>
+      <c r="L90" s="0"/>
+      <c r="M90" s="0"/>
+      <c r="N90" s="0"/>
+      <c r="O90" s="0"/>
+      <c r="P90" s="0"/>
+      <c r="Q90" s="0"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0"/>
+      <c r="B91" s="0" t="n">
+        <f aca="false">AVERAGE(B78:B80)</f>
+        <v>0.060303</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <f aca="false">AVERAGE(C78:C80)</f>
+        <v>0.0519143333333333</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <f aca="false">AVERAGE(D78:D80)</f>
+        <v>0.0487313333333333</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <f aca="false">AVERAGE(E78:E80)</f>
+        <v>0.061029</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <f aca="false">AVERAGE(F78:F80)</f>
+        <v>0.0727306666666667</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <f aca="false">AVERAGE(G78:G80)</f>
+        <v>0.074754</v>
+      </c>
+      <c r="H91" s="0" t="n">
+        <f aca="false">AVERAGE(H78:H80)</f>
+        <v>0.0554596666666667</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <f aca="false">AVERAGE(I78:I80)</f>
+        <v>0.0829643333333333</v>
+      </c>
+      <c r="J91" s="0" t="n">
+        <f aca="false">AVERAGE(J78:J80)</f>
+        <v>0.056543</v>
+      </c>
+      <c r="K91" s="0" t="n">
+        <f aca="false">AVERAGE(K78:K80)</f>
+        <v>0.0558636666666667</v>
+      </c>
+      <c r="L91" s="0"/>
+      <c r="M91" s="0"/>
+      <c r="N91" s="0"/>
+      <c r="O91" s="0"/>
+      <c r="P91" s="0"/>
+      <c r="Q91" s="0"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0"/>
+      <c r="B92" s="0" t="n">
+        <f aca="false">AVERAGE(B81:B83)</f>
+        <v>0.060303</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <f aca="false">AVERAGE(C81:C83)</f>
+        <v>0.0519143333333333</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <f aca="false">AVERAGE(D81:D83)</f>
+        <v>0.0487313333333333</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <f aca="false">AVERAGE(E81:E83)</f>
+        <v>0.061029</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <f aca="false">AVERAGE(F81:F83)</f>
+        <v>0.0727306666666667</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <f aca="false">AVERAGE(G81:G83)</f>
+        <v>0.074754</v>
+      </c>
+      <c r="H92" s="0" t="n">
+        <f aca="false">AVERAGE(H81:H83)</f>
+        <v>0.0554596666666667</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <f aca="false">AVERAGE(I81:I83)</f>
+        <v>0.0829643333333333</v>
+      </c>
+      <c r="J92" s="0" t="n">
+        <f aca="false">AVERAGE(J81:J83)</f>
+        <v>0.056543</v>
+      </c>
+      <c r="K92" s="0" t="n">
+        <f aca="false">AVERAGE(K81:K83)</f>
+        <v>0.0558636666666667</v>
+      </c>
+      <c r="L92" s="0"/>
+      <c r="M92" s="0"/>
+      <c r="N92" s="0"/>
+      <c r="O92" s="0"/>
+      <c r="P92" s="0"/>
+      <c r="Q92" s="0"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0"/>
+      <c r="B93" s="0" t="n">
+        <f aca="false">AVERAGE(B84:B86)</f>
+        <v>0.060303</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <f aca="false">AVERAGE(C84:C86)</f>
+        <v>0.0519143333333333</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <f aca="false">AVERAGE(D84:D86)</f>
+        <v>0.0487313333333333</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <f aca="false">AVERAGE(E84:E86)</f>
+        <v>0.061029</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <f aca="false">AVERAGE(F84:F86)</f>
+        <v>0.0727306666666667</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <f aca="false">AVERAGE(G84:G86)</f>
+        <v>0.074754</v>
+      </c>
+      <c r="H93" s="0" t="n">
+        <f aca="false">AVERAGE(H84:H86)</f>
+        <v>0.0554596666666667</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <f aca="false">AVERAGE(I84:I86)</f>
+        <v>0.0829643333333333</v>
+      </c>
+      <c r="J93" s="0" t="n">
+        <f aca="false">AVERAGE(J84:J86)</f>
+        <v>0.056543</v>
+      </c>
+      <c r="K93" s="0" t="n">
+        <f aca="false">AVERAGE(K84:K86)</f>
+        <v>0.0558636666666667</v>
+      </c>
+      <c r="L93" s="0"/>
+      <c r="M93" s="0"/>
+      <c r="N93" s="0"/>
+      <c r="O93" s="0"/>
+      <c r="P93" s="0"/>
+      <c r="Q93" s="0"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F94" s="0"/>
+      <c r="G94" s="0"/>
+      <c r="H94" s="0"/>
+      <c r="I94" s="0"/>
+      <c r="J94" s="0"/>
+      <c r="K94" s="0"/>
+      <c r="L94" s="0"/>
+      <c r="M94" s="0"/>
+      <c r="N94" s="0"/>
+      <c r="O94" s="0"/>
+      <c r="P94" s="0"/>
+      <c r="Q94" s="0"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F95" s="0"/>
+      <c r="G95" s="0"/>
+      <c r="H95" s="0"/>
+      <c r="I95" s="0"/>
+      <c r="J95" s="0"/>
+      <c r="K95" s="0"/>
+      <c r="L95" s="0"/>
+      <c r="M95" s="0"/>
+      <c r="N95" s="0"/>
+      <c r="O95" s="0"/>
+      <c r="P95" s="0"/>
+      <c r="Q95" s="0"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="74" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="C98" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="D98" s="74" t="n">
+        <v>150</v>
+      </c>
+      <c r="E98" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="F98" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="G98" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="H98" s="74" t="n">
+        <v>350</v>
+      </c>
+      <c r="I98" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="J98" s="74" t="n">
+        <v>450</v>
+      </c>
+      <c r="K98" s="74" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B99" s="74" t="n">
+        <v>0.01454</v>
+      </c>
+      <c r="C99" s="74" t="n">
+        <v>0.014449</v>
+      </c>
+      <c r="D99" s="74" t="n">
+        <v>0.014696</v>
+      </c>
+      <c r="E99" s="74" t="n">
+        <v>0.016965</v>
+      </c>
+      <c r="F99" s="74" t="n">
+        <v>0.074963</v>
+      </c>
+      <c r="G99" s="74" t="n">
+        <v>0.016488</v>
+      </c>
+      <c r="H99" s="74" t="n">
+        <v>0.014524</v>
+      </c>
+      <c r="I99" s="74" t="n">
+        <v>0.065197</v>
+      </c>
+      <c r="J99" s="74" t="n">
+        <v>0.014612</v>
+      </c>
+      <c r="K99" s="74" t="n">
+        <v>0.030353</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="74" t="n">
+        <v>0.015427</v>
+      </c>
+      <c r="C100" s="74" t="n">
+        <v>0.014667</v>
+      </c>
+      <c r="D100" s="74" t="n">
+        <v>0.014655</v>
+      </c>
+      <c r="E100" s="74" t="n">
+        <v>0.015793</v>
+      </c>
+      <c r="F100" s="74" t="n">
+        <v>0.014604</v>
+      </c>
+      <c r="G100" s="74" t="n">
+        <v>0.015309</v>
+      </c>
+      <c r="H100" s="74" t="n">
+        <v>0.022296</v>
+      </c>
+      <c r="I100" s="74" t="n">
+        <v>0.014665</v>
+      </c>
+      <c r="J100" s="74" t="n">
+        <v>0.068903</v>
+      </c>
+      <c r="K100" s="74" t="n">
+        <v>0.014517</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="74" t="n">
+        <v>0.015082</v>
+      </c>
+      <c r="C101" s="74" t="n">
+        <v>0.014483</v>
+      </c>
+      <c r="D101" s="74" t="n">
+        <v>0.014392</v>
+      </c>
+      <c r="E101" s="74" t="n">
+        <v>0.01456</v>
+      </c>
+      <c r="F101" s="74" t="n">
+        <v>0.01835</v>
+      </c>
+      <c r="G101" s="74" t="n">
+        <v>0.014529</v>
+      </c>
+      <c r="H101" s="74" t="n">
+        <v>0.014867</v>
+      </c>
+      <c r="I101" s="74" t="n">
+        <v>0.015323</v>
+      </c>
+      <c r="J101" s="74" t="n">
+        <v>0.01461</v>
+      </c>
+      <c r="K101" s="74" t="n">
+        <v>0.016476</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B102" s="74" t="n">
+        <v>0.01454</v>
+      </c>
+      <c r="C102" s="74" t="n">
+        <v>0.014449</v>
+      </c>
+      <c r="D102" s="74" t="n">
+        <v>0.014696</v>
+      </c>
+      <c r="E102" s="74" t="n">
+        <v>0.016965</v>
+      </c>
+      <c r="F102" s="74" t="n">
+        <v>0.074963</v>
+      </c>
+      <c r="G102" s="74" t="n">
+        <v>0.016488</v>
+      </c>
+      <c r="H102" s="74" t="n">
+        <v>0.014524</v>
+      </c>
+      <c r="I102" s="74" t="n">
+        <v>0.065197</v>
+      </c>
+      <c r="J102" s="74" t="n">
+        <v>0.014612</v>
+      </c>
+      <c r="K102" s="74" t="n">
+        <v>0.030353</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="74" t="n">
+        <v>0.015427</v>
+      </c>
+      <c r="C103" s="74" t="n">
+        <v>0.014667</v>
+      </c>
+      <c r="D103" s="74" t="n">
+        <v>0.014655</v>
+      </c>
+      <c r="E103" s="74" t="n">
+        <v>0.015793</v>
+      </c>
+      <c r="F103" s="74" t="n">
+        <v>0.014604</v>
+      </c>
+      <c r="G103" s="74" t="n">
+        <v>0.015309</v>
+      </c>
+      <c r="H103" s="74" t="n">
+        <v>0.022296</v>
+      </c>
+      <c r="I103" s="74" t="n">
+        <v>0.014665</v>
+      </c>
+      <c r="J103" s="74" t="n">
+        <v>0.068903</v>
+      </c>
+      <c r="K103" s="74" t="n">
+        <v>0.014517</v>
+      </c>
+      <c r="L103" s="0"/>
+      <c r="M103" s="0"/>
+      <c r="N103" s="0"/>
+      <c r="O103" s="0"/>
+      <c r="P103" s="0"/>
+      <c r="Q103" s="0"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="74" t="n">
+        <v>0.015082</v>
+      </c>
+      <c r="C104" s="74" t="n">
+        <v>0.014483</v>
+      </c>
+      <c r="D104" s="74" t="n">
+        <v>0.014392</v>
+      </c>
+      <c r="E104" s="74" t="n">
+        <v>0.01456</v>
+      </c>
+      <c r="F104" s="74" t="n">
+        <v>0.01835</v>
+      </c>
+      <c r="G104" s="74" t="n">
+        <v>0.014529</v>
+      </c>
+      <c r="H104" s="74" t="n">
+        <v>0.014867</v>
+      </c>
+      <c r="I104" s="74" t="n">
+        <v>0.015323</v>
+      </c>
+      <c r="J104" s="74" t="n">
+        <v>0.01461</v>
+      </c>
+      <c r="K104" s="74" t="n">
+        <v>0.016476</v>
+      </c>
+      <c r="L104" s="0"/>
+      <c r="M104" s="0"/>
+      <c r="N104" s="0"/>
+      <c r="O104" s="0"/>
+      <c r="P104" s="0"/>
+      <c r="Q104" s="0"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B105" s="74" t="n">
+        <v>0.01454</v>
+      </c>
+      <c r="C105" s="74" t="n">
+        <v>0.014449</v>
+      </c>
+      <c r="D105" s="74" t="n">
+        <v>0.014696</v>
+      </c>
+      <c r="E105" s="74" t="n">
+        <v>0.016965</v>
+      </c>
+      <c r="F105" s="74" t="n">
+        <v>0.074963</v>
+      </c>
+      <c r="G105" s="74" t="n">
+        <v>0.016488</v>
+      </c>
+      <c r="H105" s="74" t="n">
+        <v>0.014524</v>
+      </c>
+      <c r="I105" s="74" t="n">
+        <v>0.065197</v>
+      </c>
+      <c r="J105" s="74" t="n">
+        <v>0.014612</v>
+      </c>
+      <c r="K105" s="74" t="n">
+        <v>0.030353</v>
+      </c>
+      <c r="L105" s="0"/>
+      <c r="M105" s="0"/>
+      <c r="N105" s="0"/>
+      <c r="O105" s="0"/>
+      <c r="P105" s="0"/>
+      <c r="Q105" s="0"/>
+    </row>
+    <row r="106" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="74" t="n">
+        <v>0.015427</v>
+      </c>
+      <c r="C106" s="74" t="n">
+        <v>0.014667</v>
+      </c>
+      <c r="D106" s="74" t="n">
+        <v>0.014655</v>
+      </c>
+      <c r="E106" s="74" t="n">
+        <v>0.015793</v>
+      </c>
+      <c r="F106" s="74" t="n">
+        <v>0.014604</v>
+      </c>
+      <c r="G106" s="74" t="n">
+        <v>0.015309</v>
+      </c>
+      <c r="H106" s="74" t="n">
+        <v>0.022296</v>
+      </c>
+      <c r="I106" s="74" t="n">
+        <v>0.014665</v>
+      </c>
+      <c r="J106" s="74" t="n">
+        <v>0.068903</v>
+      </c>
+      <c r="K106" s="74" t="n">
+        <v>0.014517</v>
+      </c>
+      <c r="L106" s="0"/>
+      <c r="M106" s="0"/>
+      <c r="N106" s="0"/>
+      <c r="O106" s="0"/>
+      <c r="P106" s="0"/>
+      <c r="Q106" s="0"/>
+    </row>
+    <row r="107" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="74" t="n">
+        <v>0.015082</v>
+      </c>
+      <c r="C107" s="74" t="n">
+        <v>0.014483</v>
+      </c>
+      <c r="D107" s="74" t="n">
+        <v>0.014392</v>
+      </c>
+      <c r="E107" s="74" t="n">
+        <v>0.01456</v>
+      </c>
+      <c r="F107" s="74" t="n">
+        <v>0.01835</v>
+      </c>
+      <c r="G107" s="74" t="n">
+        <v>0.014529</v>
+      </c>
+      <c r="H107" s="74" t="n">
+        <v>0.014867</v>
+      </c>
+      <c r="I107" s="74" t="n">
+        <v>0.015323</v>
+      </c>
+      <c r="J107" s="74" t="n">
+        <v>0.01461</v>
+      </c>
+      <c r="K107" s="74" t="n">
+        <v>0.016476</v>
+      </c>
+      <c r="L107" s="0"/>
+      <c r="M107" s="0"/>
+      <c r="N107" s="0"/>
+      <c r="O107" s="0"/>
+      <c r="P107" s="0"/>
+      <c r="Q107" s="0"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="74" t="n">
+        <v>20</v>
+      </c>
+      <c r="B108" s="74" t="n">
+        <v>0.01454</v>
+      </c>
+      <c r="C108" s="74" t="n">
+        <v>0.014449</v>
+      </c>
+      <c r="D108" s="74" t="n">
+        <v>0.014696</v>
+      </c>
+      <c r="E108" s="74" t="n">
+        <v>0.016965</v>
+      </c>
+      <c r="F108" s="74" t="n">
+        <v>0.074963</v>
+      </c>
+      <c r="G108" s="74" t="n">
+        <v>0.016488</v>
+      </c>
+      <c r="H108" s="74" t="n">
+        <v>0.014524</v>
+      </c>
+      <c r="I108" s="74" t="n">
+        <v>0.065197</v>
+      </c>
+      <c r="J108" s="74" t="n">
+        <v>0.014612</v>
+      </c>
+      <c r="K108" s="74" t="n">
+        <v>0.030353</v>
+      </c>
+      <c r="L108" s="0"/>
+      <c r="M108" s="0"/>
+      <c r="N108" s="0"/>
+      <c r="O108" s="0"/>
+      <c r="P108" s="0"/>
+      <c r="Q108" s="0"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="74" t="n">
+        <v>0.015427</v>
+      </c>
+      <c r="C109" s="74" t="n">
+        <v>0.014667</v>
+      </c>
+      <c r="D109" s="74" t="n">
+        <v>0.014655</v>
+      </c>
+      <c r="E109" s="74" t="n">
+        <v>0.015793</v>
+      </c>
+      <c r="F109" s="74" t="n">
+        <v>0.014604</v>
+      </c>
+      <c r="G109" s="74" t="n">
+        <v>0.015309</v>
+      </c>
+      <c r="H109" s="74" t="n">
+        <v>0.022296</v>
+      </c>
+      <c r="I109" s="74" t="n">
+        <v>0.014665</v>
+      </c>
+      <c r="J109" s="74" t="n">
+        <v>0.068903</v>
+      </c>
+      <c r="K109" s="74" t="n">
+        <v>0.014517</v>
+      </c>
+      <c r="L109" s="0"/>
+      <c r="M109" s="0"/>
+      <c r="N109" s="0"/>
+      <c r="O109" s="0"/>
+      <c r="P109" s="0"/>
+      <c r="Q109" s="0"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="74" t="n">
+        <v>0.015082</v>
+      </c>
+      <c r="C110" s="74" t="n">
+        <v>0.014483</v>
+      </c>
+      <c r="D110" s="74" t="n">
+        <v>0.014392</v>
+      </c>
+      <c r="E110" s="74" t="n">
+        <v>0.01456</v>
+      </c>
+      <c r="F110" s="74" t="n">
+        <v>0.01835</v>
+      </c>
+      <c r="G110" s="74" t="n">
+        <v>0.014529</v>
+      </c>
+      <c r="H110" s="74" t="n">
+        <v>0.014867</v>
+      </c>
+      <c r="I110" s="74" t="n">
+        <v>0.015323</v>
+      </c>
+      <c r="J110" s="74" t="n">
+        <v>0.01461</v>
+      </c>
+      <c r="K110" s="74" t="n">
+        <v>0.016476</v>
+      </c>
+      <c r="L110" s="0"/>
+      <c r="M110" s="0"/>
+      <c r="N110" s="0"/>
+      <c r="O110" s="0"/>
+      <c r="P110" s="0"/>
+      <c r="Q110" s="0"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="0" t="n">
+        <f aca="false">AVERAGE(B99:B101)</f>
+        <v>0.0150163333333333</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <f aca="false">AVERAGE(C99:C101)</f>
+        <v>0.014533</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <f aca="false">AVERAGE(D99:D101)</f>
+        <v>0.014581</v>
+      </c>
+      <c r="E114" s="0" t="n">
+        <f aca="false">AVERAGE(E99:E101)</f>
+        <v>0.0157726666666667</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <f aca="false">AVERAGE(F99:F101)</f>
+        <v>0.0359723333333333</v>
+      </c>
+      <c r="G114" s="0" t="n">
+        <f aca="false">AVERAGE(G99:G101)</f>
+        <v>0.015442</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <f aca="false">AVERAGE(H99:H101)</f>
+        <v>0.017229</v>
+      </c>
+      <c r="I114" s="0" t="n">
+        <f aca="false">AVERAGE(I99:I101)</f>
+        <v>0.0317283333333333</v>
+      </c>
+      <c r="J114" s="0" t="n">
+        <f aca="false">AVERAGE(J99:J101)</f>
+        <v>0.0327083333333333</v>
+      </c>
+      <c r="K114" s="0" t="n">
+        <f aca="false">AVERAGE(K99:K101)</f>
+        <v>0.0204486666666667</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B115" s="0" t="n">
+        <f aca="false">AVERAGE(B102:B104)</f>
+        <v>0.0150163333333333</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <f aca="false">AVERAGE(C102:C104)</f>
+        <v>0.014533</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <f aca="false">AVERAGE(D102:D104)</f>
+        <v>0.014581</v>
+      </c>
+      <c r="E115" s="0" t="n">
+        <f aca="false">AVERAGE(E102:E104)</f>
+        <v>0.0157726666666667</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <f aca="false">AVERAGE(F102:F104)</f>
+        <v>0.0359723333333333</v>
+      </c>
+      <c r="G115" s="0" t="n">
+        <f aca="false">AVERAGE(G102:G104)</f>
+        <v>0.015442</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <f aca="false">AVERAGE(H102:H104)</f>
+        <v>0.017229</v>
+      </c>
+      <c r="I115" s="0" t="n">
+        <f aca="false">AVERAGE(I102:I104)</f>
+        <v>0.0317283333333333</v>
+      </c>
+      <c r="J115" s="0" t="n">
+        <f aca="false">AVERAGE(J102:J104)</f>
+        <v>0.0327083333333333</v>
+      </c>
+      <c r="K115" s="0" t="n">
+        <f aca="false">AVERAGE(K102:K104)</f>
+        <v>0.0204486666666667</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="0" t="n">
+        <f aca="false">AVERAGE(B105:B107)</f>
+        <v>0.0150163333333333</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <f aca="false">AVERAGE(C105:C107)</f>
+        <v>0.014533</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <f aca="false">AVERAGE(D105:D107)</f>
+        <v>0.014581</v>
+      </c>
+      <c r="E116" s="0" t="n">
+        <f aca="false">AVERAGE(E105:E107)</f>
+        <v>0.0157726666666667</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <f aca="false">AVERAGE(F105:F107)</f>
+        <v>0.0359723333333333</v>
+      </c>
+      <c r="G116" s="0" t="n">
+        <f aca="false">AVERAGE(G105:G107)</f>
+        <v>0.015442</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <f aca="false">AVERAGE(H105:H107)</f>
+        <v>0.017229</v>
+      </c>
+      <c r="I116" s="0" t="n">
+        <f aca="false">AVERAGE(I105:I107)</f>
+        <v>0.0317283333333333</v>
+      </c>
+      <c r="J116" s="0" t="n">
+        <f aca="false">AVERAGE(J105:J107)</f>
+        <v>0.0327083333333333</v>
+      </c>
+      <c r="K116" s="0" t="n">
+        <f aca="false">AVERAGE(K105:K107)</f>
+        <v>0.0204486666666667</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="n">
+        <f aca="false">AVERAGE(B108:B110)</f>
+        <v>0.0150163333333333</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <f aca="false">AVERAGE(C108:C110)</f>
+        <v>0.014533</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <f aca="false">AVERAGE(D108:D110)</f>
+        <v>0.014581</v>
+      </c>
+      <c r="E117" s="0" t="n">
+        <f aca="false">AVERAGE(E108:E110)</f>
+        <v>0.0157726666666667</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <f aca="false">AVERAGE(F108:F110)</f>
+        <v>0.0359723333333333</v>
+      </c>
+      <c r="G117" s="0" t="n">
+        <f aca="false">AVERAGE(G108:G110)</f>
+        <v>0.015442</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <f aca="false">AVERAGE(H108:H110)</f>
+        <v>0.017229</v>
+      </c>
+      <c r="I117" s="0" t="n">
+        <f aca="false">AVERAGE(I108:I110)</f>
+        <v>0.0317283333333333</v>
+      </c>
+      <c r="J117" s="0" t="n">
+        <f aca="false">AVERAGE(J108:J110)</f>
+        <v>0.0327083333333333</v>
+      </c>
+      <c r="K117" s="0" t="n">
+        <f aca="false">AVERAGE(K108:K110)</f>
+        <v>0.0204486666666667</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:A3"/>

</xml_diff>

<commit_message>
troubleshooting reason for LSTM producing the same error for different batch sizes
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -1127,7 +1127,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1350,11 +1350,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="26040118"/>
-        <c:axId val="66009402"/>
+        <c:axId val="48706031"/>
+        <c:axId val="52946531"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26040118"/>
+        <c:axId val="48706031"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,14 +1389,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66009402"/>
+        <c:crossAx val="52946531"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66009402"/>
+        <c:axId val="52946531"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26040118"/>
+        <c:crossAx val="48706031"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1477,7 +1477,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1736,11 +1736,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="76693369"/>
-        <c:axId val="89486080"/>
+        <c:axId val="64482331"/>
+        <c:axId val="56333786"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76693369"/>
+        <c:axId val="64482331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,14 +1775,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89486080"/>
+        <c:crossAx val="56333786"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89486080"/>
+        <c:axId val="56333786"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1826,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76693369"/>
+        <c:crossAx val="64482331"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -33317,7 +33317,7 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="topLeft" activeCell="O42" activeCellId="0" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
experimenting with 2 layer LSTM
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="121">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -353,6 +353,48 @@
   </si>
   <si>
     <t xml:space="preserve">neuron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">batch_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me: 150, dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ype: float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150-250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150-250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-150-50</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1169,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1350,11 +1392,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="48706031"/>
-        <c:axId val="52946531"/>
+        <c:axId val="64610594"/>
+        <c:axId val="60325443"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="48706031"/>
+        <c:axId val="64610594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,14 +1431,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52946531"/>
+        <c:crossAx val="60325443"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52946531"/>
+        <c:axId val="60325443"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1440,7 +1482,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48706031"/>
+        <c:crossAx val="64610594"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1477,7 +1519,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1736,11 +1778,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="64482331"/>
-        <c:axId val="56333786"/>
+        <c:axId val="94589059"/>
+        <c:axId val="78047122"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64482331"/>
+        <c:axId val="94589059"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,14 +1817,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56333786"/>
+        <c:crossAx val="78047122"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56333786"/>
+        <c:axId val="78047122"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1868,242 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64482331"/>
+        <c:crossAx val="94589059"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>train</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>train</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'LSTM Model Summary'!$C$123:$G$123</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'LSTM Model Summary'!$C$133:$G$133</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0356666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0356666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0356666666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0356666666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0356666666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="40697322"/>
+        <c:axId val="56849403"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="40697322"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="56849403"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56849403"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="40697322"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1920,6 +2197,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>60840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="782280" y="16871760"/>
+        <a:ext cx="5759640" cy="3239640"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -33314,10 +33621,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q117"/>
+  <dimension ref="A1:Q187"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O42" activeCellId="0" sqref="O42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35684,6 +35991,886 @@
         <v>0.0204486666666667</v>
       </c>
     </row>
+    <row r="122" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C122" s="74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C123" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="D123" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="E123" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="F123" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="G123" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="H123" s="0"/>
+      <c r="I123" s="0"/>
+      <c r="J123" s="0"/>
+      <c r="K123" s="0"/>
+      <c r="L123" s="0"/>
+    </row>
+    <row r="124" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C124" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="D124" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="E124" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="F124" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="G124" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="H124" s="0"/>
+      <c r="I124" s="0"/>
+      <c r="J124" s="0"/>
+      <c r="K124" s="0"/>
+      <c r="L124" s="0"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C125" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="D125" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="E125" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="F125" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="G125" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="H125" s="0"/>
+      <c r="I125" s="0"/>
+      <c r="J125" s="0"/>
+      <c r="K125" s="0"/>
+      <c r="L125" s="0"/>
+    </row>
+    <row r="126" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C126" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="D126" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="E126" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="F126" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="G126" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="H126" s="0"/>
+      <c r="I126" s="0"/>
+      <c r="J126" s="0"/>
+      <c r="K126" s="0"/>
+      <c r="L126" s="0"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C127" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="D127" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="E127" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="F127" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="G127" s="74" t="n">
+        <v>0.04253</v>
+      </c>
+      <c r="H127" s="0"/>
+      <c r="I127" s="0"/>
+      <c r="J127" s="0"/>
+      <c r="K127" s="0"/>
+      <c r="L127" s="0"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C128" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="D128" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="E128" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="F128" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="G128" s="74" t="n">
+        <v>0.036234</v>
+      </c>
+      <c r="H128" s="0"/>
+      <c r="I128" s="0"/>
+      <c r="J128" s="0"/>
+      <c r="K128" s="0"/>
+      <c r="L128" s="0"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C129" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="D129" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="E129" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="F129" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="G129" s="74" t="n">
+        <v>0.028236</v>
+      </c>
+      <c r="H129" s="0"/>
+      <c r="I129" s="0"/>
+      <c r="J129" s="0"/>
+      <c r="K129" s="0"/>
+      <c r="L129" s="0"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H130" s="0"/>
+      <c r="I130" s="0"/>
+      <c r="J130" s="0"/>
+      <c r="K130" s="0"/>
+      <c r="L130" s="0"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H131" s="0"/>
+      <c r="I131" s="0"/>
+      <c r="J131" s="0"/>
+      <c r="K131" s="0"/>
+      <c r="L131" s="0"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H132" s="0"/>
+      <c r="I132" s="0"/>
+      <c r="J132" s="0"/>
+      <c r="K132" s="0"/>
+      <c r="L132" s="0"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C133" s="0" t="n">
+        <f aca="false">AVERAGE(C124:C126)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <f aca="false">AVERAGE(D124:D126)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="E133" s="0" t="n">
+        <f aca="false">AVERAGE(E124:E126)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <f aca="false">AVERAGE(F124:F126)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <f aca="false">AVERAGE(G124:G126)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="H133" s="0"/>
+      <c r="I133" s="0"/>
+      <c r="J133" s="0"/>
+      <c r="K133" s="0"/>
+      <c r="L133" s="0"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C134" s="0" t="n">
+        <f aca="false">AVERAGE(C127:C129)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <f aca="false">AVERAGE(D127:D129)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="E134" s="0" t="n">
+        <f aca="false">AVERAGE(E127:E129)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <f aca="false">AVERAGE(F127:F129)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="G134" s="0" t="n">
+        <f aca="false">AVERAGE(G127:G129)</f>
+        <v>0.0356666666666667</v>
+      </c>
+      <c r="H134" s="0"/>
+      <c r="I134" s="0"/>
+      <c r="J134" s="0"/>
+      <c r="K134" s="0"/>
+      <c r="L134" s="0"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H135" s="0"/>
+      <c r="I135" s="0"/>
+      <c r="J135" s="0"/>
+      <c r="K135" s="0"/>
+      <c r="L135" s="0"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H136" s="0"/>
+      <c r="I136" s="0"/>
+      <c r="J136" s="0"/>
+      <c r="K136" s="0"/>
+      <c r="L136" s="0"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H137" s="0"/>
+      <c r="I137" s="0"/>
+      <c r="J137" s="0"/>
+      <c r="K137" s="0"/>
+      <c r="L137" s="0"/>
+    </row>
+    <row r="138" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C138" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="H138" s="0"/>
+      <c r="I138" s="0"/>
+      <c r="J138" s="0"/>
+      <c r="K138" s="0"/>
+      <c r="L138" s="0"/>
+    </row>
+    <row r="139" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B139" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C139" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="D139" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="E139" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="F139" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="G139" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="H139" s="0"/>
+      <c r="I139" s="0"/>
+      <c r="J139" s="0"/>
+      <c r="K139" s="0"/>
+      <c r="L139" s="0"/>
+    </row>
+    <row r="140" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B140" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C140" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="D140" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="E140" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="F140" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="G140" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="H140" s="0"/>
+      <c r="I140" s="0"/>
+      <c r="J140" s="0"/>
+      <c r="K140" s="0"/>
+      <c r="L140" s="0"/>
+    </row>
+    <row r="141" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C141" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="D141" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="E141" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="F141" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="G141" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="H141" s="0"/>
+      <c r="I141" s="0"/>
+      <c r="J141" s="0"/>
+      <c r="K141" s="0"/>
+      <c r="L141" s="0"/>
+    </row>
+    <row r="142" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C142" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="D142" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="E142" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="F142" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="G142" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="H142" s="0"/>
+      <c r="I142" s="0"/>
+      <c r="J142" s="0"/>
+      <c r="K142" s="0"/>
+      <c r="L142" s="0"/>
+    </row>
+    <row r="143" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C143" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="D143" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="E143" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="F143" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="G143" s="74" t="n">
+        <v>0.014728</v>
+      </c>
+      <c r="H143" s="0"/>
+      <c r="I143" s="0"/>
+      <c r="J143" s="0"/>
+      <c r="K143" s="0"/>
+      <c r="L143" s="0"/>
+    </row>
+    <row r="144" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C144" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="D144" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="E144" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="F144" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="G144" s="74" t="n">
+        <v>0.014417</v>
+      </c>
+      <c r="H144" s="0"/>
+      <c r="I144" s="0"/>
+      <c r="J144" s="0"/>
+      <c r="K144" s="0"/>
+      <c r="L144" s="0"/>
+    </row>
+    <row r="145" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C145" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="D145" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="E145" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="F145" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="G145" s="74" t="n">
+        <v>0.014683</v>
+      </c>
+      <c r="H145" s="0"/>
+      <c r="I145" s="0"/>
+      <c r="J145" s="0"/>
+      <c r="K145" s="0"/>
+      <c r="L145" s="0"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H146" s="0"/>
+      <c r="I146" s="0"/>
+      <c r="J146" s="0"/>
+      <c r="K146" s="0"/>
+      <c r="L146" s="0"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H147" s="0"/>
+      <c r="I147" s="0"/>
+      <c r="J147" s="0"/>
+      <c r="K147" s="0"/>
+      <c r="L147" s="0"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H148" s="0"/>
+      <c r="I148" s="0"/>
+      <c r="J148" s="0"/>
+      <c r="K148" s="0"/>
+      <c r="L148" s="0"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C149" s="0" t="n">
+        <f aca="false">AVERAGE(C140:C142)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <f aca="false">AVERAGE(D140:D142)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="E149" s="0" t="n">
+        <f aca="false">AVERAGE(E140:E142)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <f aca="false">AVERAGE(F140:F142)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <f aca="false">AVERAGE(G140:G142)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="H149" s="0"/>
+      <c r="I149" s="0"/>
+      <c r="J149" s="0"/>
+      <c r="K149" s="0"/>
+      <c r="L149" s="0"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C150" s="0" t="n">
+        <f aca="false">AVERAGE(C143:C145)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <f aca="false">AVERAGE(D143:D145)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="E150" s="0" t="n">
+        <f aca="false">AVERAGE(E143:E145)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <f aca="false">AVERAGE(F143:F145)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <f aca="false">AVERAGE(G143:G145)</f>
+        <v>0.0146093333333333</v>
+      </c>
+      <c r="H150" s="0"/>
+      <c r="I150" s="0"/>
+      <c r="J150" s="0"/>
+      <c r="K150" s="0"/>
+      <c r="L150" s="0"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G151" s="0"/>
+      <c r="H151" s="0"/>
+      <c r="I151" s="0"/>
+      <c r="J151" s="0"/>
+      <c r="K151" s="0"/>
+      <c r="L151" s="0"/>
+    </row>
+    <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I157" s="74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B158" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="H158" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="I158" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="J158" s="74" t="n">
+        <v>50</v>
+      </c>
+      <c r="K158" s="74" t="n">
+        <v>100</v>
+      </c>
+      <c r="L158" s="74" t="n">
+        <v>250</v>
+      </c>
+      <c r="M158" s="74" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B159" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+      <c r="H159" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="I159" s="74" t="n">
+        <v>0.027493</v>
+      </c>
+      <c r="J159" s="74" t="n">
+        <v>0.027493</v>
+      </c>
+      <c r="K159" s="74" t="n">
+        <v>0.027493</v>
+      </c>
+      <c r="L159" s="74" t="n">
+        <v>0.027493</v>
+      </c>
+      <c r="M159" s="74" t="n">
+        <v>0.027493</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B160" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C160" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D160" s="74" t="n">
+        <v>64</v>
+      </c>
+      <c r="H160" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="I160" s="74" t="n">
+        <v>0.015811</v>
+      </c>
+      <c r="J160" s="74" t="n">
+        <v>0.015811</v>
+      </c>
+      <c r="K160" s="74" t="n">
+        <v>0.015811</v>
+      </c>
+      <c r="L160" s="74" t="n">
+        <v>0.015811</v>
+      </c>
+      <c r="M160" s="74" t="n">
+        <v>0.015811</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="74" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B161" s="74" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B162" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+      <c r="H162" s="0"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B163" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C163" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D163" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="74" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B164" s="74" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B165" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B166" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C166" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D166" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B167" s="74" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B168" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B169" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C169" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D169" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B170" s="74" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B171" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B172" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C172" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D172" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="74" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B173" s="74" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B174" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B175" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C175" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D175" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="74" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B176" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B177" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B178" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C178" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D178" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B179" s="74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B180" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B181" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C181" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D181" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="74" t="n">
+        <v>-5</v>
+      </c>
+      <c r="B182" s="74" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B183" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B184" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C184" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D184" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B185" s="74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="74" t="n">
+        <v>0</v>
+      </c>
+      <c r="B186" s="74" t="n">
+        <v>0.02903</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B187" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="C187" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="D187" s="74" t="n">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:A3"/>

</xml_diff>

<commit_message>
more results for optimizing 2 layer LSTM
</commit_message>
<xml_diff>
--- a/Model Results.xlsx
+++ b/Model Results.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="120">
   <si>
     <t xml:space="preserve">for finding prices 5 days (1 week) out:</t>
   </si>
@@ -387,16 +387,13 @@
     <t xml:space="preserve">Average - test error</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">500</t>
   </si>
   <si>
-    <t xml:space="preserve">250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Average - train error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Average - test error</t>
+    <t xml:space="preserve">400</t>
   </si>
 </sst>
 </file>
@@ -473,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="43">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -747,6 +744,34 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -791,7 +816,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="145">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1240,10 +1265,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1304,7 +1325,75 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="22" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="37" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="36" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="37" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="19" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="27" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="39" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="19" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="40" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="42" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="39" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1386,7 +1475,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1622,11 +1711,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="32699431"/>
-        <c:axId val="18304384"/>
+        <c:axId val="45859400"/>
+        <c:axId val="65435284"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32699431"/>
+        <c:axId val="45859400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,14 +1750,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18304384"/>
+        <c:crossAx val="65435284"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18304384"/>
+        <c:axId val="65435284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1712,7 +1801,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32699431"/>
+        <c:crossAx val="45859400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1757,7 +1846,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2029,11 +2118,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="27869205"/>
-        <c:axId val="65600726"/>
+        <c:axId val="58370709"/>
+        <c:axId val="25808834"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27869205"/>
+        <c:axId val="58370709"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2068,14 +2157,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65600726"/>
+        <c:crossAx val="25808834"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65600726"/>
+        <c:axId val="25808834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2119,7 +2208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27869205"/>
+        <c:crossAx val="58370709"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2164,7 +2253,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2376,11 +2465,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="29092161"/>
-        <c:axId val="9501576"/>
+        <c:axId val="3029186"/>
+        <c:axId val="14987403"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="29092161"/>
+        <c:axId val="3029186"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2415,14 +2504,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9501576"/>
+        <c:crossAx val="14987403"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9501576"/>
+        <c:axId val="14987403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,7 +2555,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29092161"/>
+        <c:crossAx val="3029186"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5285,205 +5374,205 @@
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="81">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A109:F190" sheet="LSTM Model Summary"/>
+    <worksheetSource ref="A192:F273" sheet="LSTM Model Summary"/>
   </cacheSource>
   <cacheFields count="6">
     <cacheField name="Layer 1" numFmtId="0">
       <sharedItems count="3" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
         <n v="5"/>
-        <n v="100"/>
-        <n v="200"/>
+        <n v="10"/>
+        <n v="15"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Layer 2" numFmtId="0">
       <sharedItems count="3" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
         <n v="5"/>
-        <n v="100"/>
-        <n v="200"/>
+        <n v="10"/>
+        <n v="15"/>
       </sharedItems>
     </cacheField>
     <cacheField name="epochs" numFmtId="0">
       <sharedItems count="3" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="50"/>
-        <n v="150"/>
-        <n v="250"/>
+        <n v="200"/>
+        <n v="300"/>
+        <n v="400"/>
       </sharedItems>
     </cacheField>
     <cacheField name="batch_size" numFmtId="0">
       <sharedItems count="3" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="100"/>
-        <n v="250"/>
+        <n v="400"/>
         <n v="500"/>
+        <n v="600"/>
       </sharedItems>
     </cacheField>
     <cacheField name="train error" numFmtId="0">
       <sharedItems count="81" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="0.0272065054889437"/>
-        <n v="0.0272209969858319"/>
-        <n v="0.0272214129949313"/>
-        <n v="0.0272302600978663"/>
-        <n v="0.0272335154469437"/>
-        <n v="0.0272350196025248"/>
-        <n v="0.0272354505464678"/>
-        <n v="0.0272355064953294"/>
-        <n v="0.0272377569689874"/>
-        <n v="0.0272515089731327"/>
-        <n v="0.0272585240704172"/>
-        <n v="0.0272635930501846"/>
-        <n v="0.0272640409606607"/>
-        <n v="0.0272691545365854"/>
-        <n v="0.0272693830605323"/>
-        <n v="0.0272703426992574"/>
-        <n v="0.0272709646264066"/>
-        <n v="0.0272755466267592"/>
-        <n v="0.0272779181318615"/>
-        <n v="0.0272792315428739"/>
-        <n v="0.0272809202528401"/>
-        <n v="0.027285534352261"/>
-        <n v="0.0272934618492123"/>
-        <n v="0.0272969396953199"/>
-        <n v="0.0272984651174741"/>
-        <n v="0.0272990046718147"/>
-        <n v="0.0273185415282283"/>
-        <n v="0.0273219236613738"/>
-        <n v="0.0273256610855934"/>
-        <n v="0.0273351927256876"/>
-        <n v="0.0273392195604861"/>
-        <n v="0.0273445572916669"/>
-        <n v="0.0273478868832364"/>
-        <n v="0.0273544537518659"/>
-        <n v="0.0273552685972334"/>
-        <n v="0.0273646832369971"/>
-        <n v="0.027365722909352"/>
-        <n v="0.0274061332919906"/>
-        <n v="0.0274238627310136"/>
-        <n v="0.0274521532417963"/>
-        <n v="0.0274522227695689"/>
-        <n v="0.0274707288594973"/>
-        <n v="0.0275419643225268"/>
-        <n v="0.0276106720643442"/>
-        <n v="0.0277128449782957"/>
-        <n v="0.0277528204062096"/>
-        <n v="0.0277767351864871"/>
-        <n v="0.0277913201424675"/>
-        <n v="0.02779894416183"/>
-        <n v="0.0278017895927491"/>
-        <n v="0.0278061539955832"/>
-        <n v="0.0278522589432458"/>
-        <n v="0.0279028740207298"/>
-        <n v="0.0279145247398856"/>
-        <n v="0.0279901559930906"/>
-        <n v="0.0280065928181823"/>
-        <n v="0.0280360952073744"/>
-        <n v="0.0280480463435267"/>
-        <n v="0.0280533702114766"/>
-        <n v="0.0281789483566831"/>
-        <n v="0.0282824168626586"/>
-        <n v="0.0284972134708762"/>
-        <n v="0.0285073804287791"/>
-        <n v="0.0294055325152909"/>
-        <n v="0.0295773775351717"/>
-        <n v="0.0296352590972941"/>
-        <n v="0.0303005333844776"/>
-        <n v="0.0311630932233325"/>
-        <n v="0.0312970137295476"/>
-        <n v="0.0317331008866493"/>
-        <n v="0.0317971412355243"/>
-        <n v="0.0320739926975223"/>
-        <n v="0.0358210581354495"/>
-        <n v="0.0368397698884037"/>
-        <n v="0.0389497513644492"/>
-        <n v="0.039335213352485"/>
-        <n v="0.0449479188326848"/>
-        <n v="0.0455083275254972"/>
-        <n v="0.0533123980500741"/>
-        <n v="0.0633155538847759"/>
-        <n v="0.0736203524780101"/>
+        <n v="0.0271518106329575"/>
+        <n v="0.0272125604602303"/>
+        <n v="0.0272158467188324"/>
+        <n v="0.0272165003166818"/>
+        <n v="0.0272176386166153"/>
+        <n v="0.0272529773626372"/>
+        <n v="0.0272586871352166"/>
+        <n v="0.0272646346878384"/>
+        <n v="0.0272657333347741"/>
+        <n v="0.0272665363842072"/>
+        <n v="0.027295362988569"/>
+        <n v="0.0273043879412292"/>
+        <n v="0.0273051667088274"/>
+        <n v="0.0273053628853176"/>
+        <n v="0.0273060852930813"/>
+        <n v="0.0273089049360908"/>
+        <n v="0.0273247498138547"/>
+        <n v="0.027356920053565"/>
+        <n v="0.0273683398064657"/>
+        <n v="0.0273701311001188"/>
+        <n v="0.0273786645058657"/>
+        <n v="0.0273790312592369"/>
+        <n v="0.027487302185228"/>
+        <n v="0.0276663858624463"/>
+        <n v="0.0276757637049803"/>
+        <n v="0.0276779780809594"/>
+        <n v="0.0276824073742217"/>
+        <n v="0.0276900660968758"/>
+        <n v="0.027690100844877"/>
+        <n v="0.0276915940591702"/>
+        <n v="0.0276937340335798"/>
+        <n v="0.0276964748558608"/>
+        <n v="0.0277019951349735"/>
+        <n v="0.0277024746583089"/>
+        <n v="0.0277175303354732"/>
+        <n v="0.0277268761976726"/>
+        <n v="0.0277320560480617"/>
+        <n v="0.0277333989059793"/>
+        <n v="0.027733973046727"/>
+        <n v="0.0277366060793134"/>
+        <n v="0.0277371586088751"/>
+        <n v="0.0277425010147322"/>
+        <n v="0.0277505237748832"/>
+        <n v="0.0277514009752104"/>
+        <n v="0.0277531030510179"/>
+        <n v="0.0277550542727464"/>
+        <n v="0.0277553616674744"/>
+        <n v="0.0277603267167707"/>
+        <n v="0.0277606145767714"/>
+        <n v="0.0277668783301186"/>
+        <n v="0.0277700110639005"/>
+        <n v="0.027770511232103"/>
+        <n v="0.0277726083903836"/>
+        <n v="0.0277747590940481"/>
+        <n v="0.0277761435152246"/>
+        <n v="0.0277773462332775"/>
+        <n v="0.0277810733875579"/>
+        <n v="0.0277828978231535"/>
+        <n v="0.0277831732658871"/>
+        <n v="0.0277932846262325"/>
+        <n v="0.0277943996366322"/>
+        <n v="0.0277981288577423"/>
+        <n v="0.0277981416468563"/>
+        <n v="0.0278023212572681"/>
+        <n v="0.0278027096699477"/>
+        <n v="0.0278050211434735"/>
+        <n v="0.0278074471434338"/>
+        <n v="0.0278078167612897"/>
+        <n v="0.0278093531209519"/>
+        <n v="0.0278153513650753"/>
+        <n v="0.0278248932349117"/>
+        <n v="0.0278287982505812"/>
+        <n v="0.0278709661161988"/>
+        <n v="0.0278794815104737"/>
+        <n v="0.027893601286958"/>
+        <n v="0.0279109589248243"/>
+        <n v="0.0279257951748146"/>
+        <n v="0.0279948252467428"/>
+        <n v="0.0280526200881892"/>
+        <n v="0.028720556953706"/>
+        <n v="0.0296861445609495"/>
       </sharedItems>
     </cacheField>
     <cacheField name="test error" numFmtId="0">
       <sharedItems count="81" containsMixedTypes="0" containsSemiMixedTypes="0" containsString="0" containsNumber="1">
-        <n v="0.0124289011974595"/>
-        <n v="0.0124849115003355"/>
-        <n v="0.0124893038665277"/>
-        <n v="0.0124893482068401"/>
-        <n v="0.0125226079926572"/>
-        <n v="0.0125342325096674"/>
-        <n v="0.0125371525608608"/>
-        <n v="0.0125466987406911"/>
-        <n v="0.0125516333272871"/>
-        <n v="0.0125668499049907"/>
-        <n v="0.012576419198419"/>
-        <n v="0.0125902147946494"/>
-        <n v="0.0125940674975925"/>
-        <n v="0.0126022494267417"/>
-        <n v="0.0126208281203498"/>
-        <n v="0.0126879370834801"/>
-        <n v="0.0126976508511742"/>
-        <n v="0.012704343593809"/>
-        <n v="0.0127060594733748"/>
-        <n v="0.0128022346260483"/>
-        <n v="0.0128215332591325"/>
-        <n v="0.0129453730286626"/>
-        <n v="0.0130040030099412"/>
-        <n v="0.0130388105008857"/>
-        <n v="0.0132260054284554"/>
-        <n v="0.0140127349216021"/>
-        <n v="0.0142552893773083"/>
-        <n v="0.0142561479292723"/>
-        <n v="0.0142718014607585"/>
-        <n v="0.0142976608267818"/>
-        <n v="0.0143103628031221"/>
-        <n v="0.0143417168203758"/>
-        <n v="0.0143473320382373"/>
-        <n v="0.0143809121504855"/>
-        <n v="0.0144017721844569"/>
-        <n v="0.0144129311382408"/>
-        <n v="0.0144264254293205"/>
-        <n v="0.0144317038335937"/>
-        <n v="0.0144336986530901"/>
-        <n v="0.0144427742917483"/>
-        <n v="0.0144429518942074"/>
-        <n v="0.0144458748802765"/>
-        <n v="0.0144523326816405"/>
-        <n v="0.0144770802544975"/>
-        <n v="0.0144846701105474"/>
-        <n v="0.0145201279170436"/>
-        <n v="0.014524229174075"/>
-        <n v="0.0145253688546531"/>
-        <n v="0.0145475792778464"/>
-        <n v="0.0145485020633269"/>
-        <n v="0.0145663361034824"/>
-        <n v="0.014569540254397"/>
-        <n v="0.0145712736989678"/>
-        <n v="0.0145926921310113"/>
-        <n v="0.0146181219473787"/>
-        <n v="0.0146699658078308"/>
-        <n v="0.0146723626248758"/>
-        <n v="0.0147291317437829"/>
-        <n v="0.0147531827919433"/>
-        <n v="0.0147662520806502"/>
-        <n v="0.0147721191544922"/>
-        <n v="0.0147795307790086"/>
-        <n v="0.0147809306140652"/>
-        <n v="0.0149150972334863"/>
-        <n v="0.0150418928181687"/>
-        <n v="0.0150433709789416"/>
-        <n v="0.0151766220967037"/>
-        <n v="0.0154341458448654"/>
-        <n v="0.015543903177036"/>
-        <n v="0.0157658943901425"/>
-        <n v="0.0159273510067355"/>
-        <n v="0.0161769522485603"/>
-        <n v="0.0162157743406281"/>
-        <n v="0.0164210650312511"/>
-        <n v="0.0166188395362948"/>
-        <n v="0.0167477947970245"/>
-        <n v="0.0167659088508354"/>
-        <n v="0.0182459229609542"/>
-        <n v="0.0205680443174734"/>
-        <n v="0.0299677386419533"/>
-        <n v="0.040263458514095"/>
+        <n v="0.0124626718123526"/>
+        <n v="0.0124709825464683"/>
+        <n v="0.0125179051917055"/>
+        <n v="0.0125304374284825"/>
+        <n v="0.0125526970280986"/>
+        <n v="0.012553507352753"/>
+        <n v="0.0125593682039823"/>
+        <n v="0.0125619461670006"/>
+        <n v="0.0125839403117134"/>
+        <n v="0.0126006877706183"/>
+        <n v="0.0126134575699191"/>
+        <n v="0.0126195881608499"/>
+        <n v="0.0126226019950381"/>
+        <n v="0.0126598859582523"/>
+        <n v="0.0127112741427428"/>
+        <n v="0.0127119074393845"/>
+        <n v="0.0128308424597175"/>
+        <n v="0.0128473896259296"/>
+        <n v="0.0128531800817593"/>
+        <n v="0.0129181685606768"/>
+        <n v="0.0129613077507679"/>
+        <n v="0.0130195443703591"/>
+        <n v="0.0130994176227148"/>
+        <n v="0.0131886148885506"/>
+        <n v="0.0134529846877591"/>
+        <n v="0.0134692429531631"/>
+        <n v="0.0134712177900632"/>
+        <n v="0.0134735112809735"/>
+        <n v="0.0134995784610357"/>
+        <n v="0.013506162062234"/>
+        <n v="0.0135071830550466"/>
+        <n v="0.0135326311566118"/>
+        <n v="0.0135403040432141"/>
+        <n v="0.013577586437554"/>
+        <n v="0.0135933831360492"/>
+        <n v="0.0136020486090205"/>
+        <n v="0.0136192856959921"/>
+        <n v="0.0136398821003798"/>
+        <n v="0.0136635224431527"/>
+        <n v="0.0136895347200016"/>
+        <n v="0.0136914905091539"/>
+        <n v="0.0137131169687583"/>
+        <n v="0.0137985504603507"/>
+        <n v="0.0138159171622351"/>
+        <n v="0.0139182999004304"/>
+        <n v="0.0139352669511624"/>
+        <n v="0.0141643402888762"/>
+        <n v="0.0144243801639859"/>
+        <n v="0.0144284699817252"/>
+        <n v="0.0144442701130392"/>
+        <n v="0.014447679417254"/>
+        <n v="0.0144944724806178"/>
+        <n v="0.0144967973288582"/>
+        <n v="0.0145086924098168"/>
+        <n v="0.0145150336399124"/>
+        <n v="0.0145155320563741"/>
+        <n v="0.0145309769772272"/>
+        <n v="0.0145415368437708"/>
+        <n v="0.0145438559051414"/>
+        <n v="0.0145491358906348"/>
+        <n v="0.0145700433128921"/>
+        <n v="0.0145827983693263"/>
+        <n v="0.0145834620931173"/>
+        <n v="0.0145924929424003"/>
+        <n v="0.0146138642072471"/>
+        <n v="0.0146182713817412"/>
+        <n v="0.0146285546792296"/>
+        <n v="0.0146555958641398"/>
+        <n v="0.0146663835881702"/>
+        <n v="0.0146769484786268"/>
+        <n v="0.0146773956393"/>
+        <n v="0.0147249158496426"/>
+        <n v="0.014737372536367"/>
+        <n v="0.0147712236902055"/>
+        <n v="0.0150204530639004"/>
+        <n v="0.015054577629523"/>
+        <n v="0.0156678641775377"/>
+        <n v="0.0164513402044849"/>
+        <n v="0.0169496831740034"/>
+        <n v="0.0179188500308673"/>
+        <n v="0.0186199659372583"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -11407,652 +11496,652 @@
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="81">
   <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="68"/>
+    <x v="51"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="54"/>
+    <x v="38"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="64"/>
+    <x v="49"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
     <x v="6"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="38"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="80"/>
-    <x v="80"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="24"/>
-    <x v="19"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="65"/>
-    <x v="66"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="13"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="79"/>
+    <x v="60"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="74"/>
+    <x v="73"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="59"/>
+    <x v="57"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="46"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="58"/>
+    <x v="45"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="43"/>
+    <x v="68"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="47"/>
+    <x v="36"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="67"/>
+    <x v="28"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <x v="26"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
     <x v="59"/>
-    <x v="68"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="44"/>
-    <x v="50"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="12"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="14"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="32"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="25"/>
+    <x v="71"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="29"/>
-    <x v="31"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="49"/>
-    <x v="37"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="46"/>
-    <x v="42"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="25"/>
-    <x v="48"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="48"/>
-    <x v="49"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="50"/>
-    <x v="36"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="60"/>
-    <x v="41"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="74"/>
-    <x v="76"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="20"/>
-    <x v="29"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="79"/>
-    <x v="65"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="70"/>
-    <x v="77"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="62"/>
-    <x v="64"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="68"/>
-    <x v="75"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="40"/>
-    <x v="46"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="7"/>
-    <x v="58"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="53"/>
-    <x v="43"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="31"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="11"/>
-    <x v="21"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="28"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="21"/>
-    <x v="39"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="76"/>
-    <x v="67"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="36"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="33"/>
-    <x v="22"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="73"/>
-    <x v="52"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="35"/>
-    <x v="27"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="55"/>
-    <x v="20"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="51"/>
-    <x v="54"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="47"/>
-    <x v="44"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="22"/>
-    <x v="35"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="17"/>
-    <x v="25"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="58"/>
-    <x v="61"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="4"/>
     <x v="23"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="41"/>
-    <x v="40"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="42"/>
-    <x v="45"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="77"/>
-    <x v="69"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="30"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="26"/>
-    <x v="53"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="18"/>
-    <x v="24"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="57"/>
-    <x v="56"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="72"/>
-    <x v="74"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="43"/>
-    <x v="47"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="16"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="63"/>
-    <x v="70"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="37"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="69"/>
-    <x v="59"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="34"/>
-    <x v="33"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="66"/>
-    <x v="78"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="30"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="28"/>
-    <x v="32"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="71"/>
-    <x v="71"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="67"/>
-    <x v="57"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="15"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="39"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
     <x v="1"/>
     <x v="1"/>
     <x v="78"/>
     <x v="79"/>
   </r>
   <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="75"/>
-    <x v="73"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="50"/>
+    <x v="70"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="33"/>
+    <x v="34"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="13"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="45"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="19"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="62"/>
+    <x v="66"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="22"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="23"/>
+    <x v="50"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="53"/>
     <x v="61"/>
-    <x v="55"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="45"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="66"/>
+    <x v="65"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="41"/>
+    <x v="33"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="38"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="19"/>
-    <x v="34"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
+    <x v="69"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="56"/>
+    <x v="47"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="36"/>
+    <x v="74"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="42"/>
+    <x v="32"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="17"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="31"/>
+    <x v="62"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
     <x v="10"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="23"/>
-    <x v="51"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="56"/>
-    <x v="60"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="64"/>
-    <x v="62"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="54"/>
-    <x v="63"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <x v="52"/>
     <x v="72"/>
   </r>
   <r>
     <x v="2"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="34"/>
+    <x v="64"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="65"/>
+    <x v="37"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="14"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="76"/>
+    <x v="75"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="20"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="39"/>
+    <x v="54"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="49"/>
+    <x v="48"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="61"/>
+    <x v="27"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="28"/>
+    <x v="39"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="55"/>
+    <x v="44"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="77"/>
+    <x v="78"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="57"/>
+    <x v="67"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="12"/>
     <x v="7"/>
   </r>
   <r>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="72"/>
+    <x v="56"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="35"/>
+    <x v="63"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="18"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="37"/>
+    <x v="52"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="70"/>
+    <x v="24"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="44"/>
+    <x v="25"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="75"/>
+    <x v="77"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="24"/>
+    <x v="30"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="51"/>
+    <x v="40"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="32"/>
+    <x v="41"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="46"/>
+    <x v="58"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="73"/>
+    <x v="53"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="21"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="80"/>
+    <x v="76"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="30"/>
+    <x v="35"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="48"/>
+    <x v="55"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="40"/>
+    <x v="43"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="71"/>
+    <x v="80"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="60"/>
+    <x v="31"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="63"/>
+    <x v="26"/>
+  </r>
+  <r>
+    <x v="2"/>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="27"/>
-    <x v="1"/>
+    <x v="42"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="15"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="69"/>
+    <x v="29"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -12122,28 +12211,27 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="1" outlineData="1">
-  <location ref="A6:I12" firstHeaderRow="2" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <location ref="A6:E11" firstHeaderRow="2" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0"/>
     <pivotField axis="axisCol" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0"/>
     <pivotField axis="axisPage" showAll="0"/>
     <pivotField axis="axisPage" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="0"/>
   </rowFields>
   <colFields count="2">
-    <field x="0"/>
+    <field x="1"/>
     <field x="-2"/>
   </colFields>
   <pageFields count="2">
     <pageField fld="3" hier="-1"/>
     <pageField fld="2" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField fld="4" subtotal="average"/>
+  <dataFields count="1">
     <dataField fld="5" subtotal="average"/>
   </dataFields>
 </pivotTableDefinition>
@@ -12271,10 +12359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:I12"/>
+  <dimension ref="A3:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12286,193 +12374,112 @@
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="128" t="s">
-        <v>117</v>
+      <c r="B3" s="138" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="128" t="s">
-        <v>118</v>
+      <c r="B4" s="138" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="57"/>
+      <c r="A6" s="57" t="s">
+        <v>116</v>
+      </c>
       <c r="B6" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="140"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="58"/>
-      <c r="B7" s="16" t="n">
+      <c r="B7" s="141" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16" t="n">
-        <v>200</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>120</v>
+      <c r="C7" s="142" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="142" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="143" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
+      <c r="A8" s="24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" s="59" t="n">
+        <v>0.0125526970280986</v>
+      </c>
+      <c r="C8" s="29" t="n">
+        <v>0.0124626718123526</v>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>0.0127112741427428</v>
+      </c>
+      <c r="E8" s="31" t="n">
+        <v>0.0125755476610647</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" s="59" t="n">
-        <v>0.0273219236613738</v>
-      </c>
-      <c r="C9" s="27" t="n">
-        <v>0.0124849115003355</v>
-      </c>
-      <c r="D9" s="37" t="n">
-        <v>0.0272065054889437</v>
-      </c>
-      <c r="E9" s="37" t="n">
-        <v>0.012576419198419</v>
-      </c>
-      <c r="F9" s="59" t="n">
-        <v>0.0272350196025248</v>
-      </c>
-      <c r="G9" s="27" t="n">
-        <v>0.0125466987406911</v>
-      </c>
-      <c r="H9" s="60" t="n">
-        <v>0.0272544829176141</v>
-      </c>
-      <c r="I9" s="31" t="n">
-        <v>0.0125360098131485</v>
+      <c r="A9" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" s="61" t="n">
+        <v>0.0126134575699191</v>
+      </c>
+      <c r="C9" s="37" t="n">
+        <v>0.0128531800817593</v>
+      </c>
+      <c r="D9" s="35" t="n">
+        <v>0.0127119074393845</v>
+      </c>
+      <c r="E9" s="39" t="n">
+        <v>0.012726181697021</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="32" t="n">
-        <v>100</v>
-      </c>
-      <c r="B10" s="61" t="n">
-        <v>0.0274238627310136</v>
-      </c>
-      <c r="C10" s="35" t="n">
-        <v>0.0125516333272871</v>
-      </c>
-      <c r="D10" s="37" t="n">
-        <v>0.0280065928181823</v>
-      </c>
-      <c r="E10" s="37" t="n">
-        <v>0.0128215332591325</v>
-      </c>
-      <c r="F10" s="61" t="n">
-        <v>0.0272640409606607</v>
-      </c>
-      <c r="G10" s="35" t="n">
-        <v>0.0125226079926572</v>
-      </c>
-      <c r="H10" s="60" t="n">
-        <v>0.0275648321699522</v>
-      </c>
-      <c r="I10" s="39" t="n">
-        <v>0.0126319248596923</v>
+        <v>15</v>
+      </c>
+      <c r="B10" s="62" t="n">
+        <v>0.0130195443703591</v>
+      </c>
+      <c r="C10" s="45" t="n">
+        <v>0.0125619461670006</v>
+      </c>
+      <c r="D10" s="43" t="n">
+        <v>0.0126006877706183</v>
+      </c>
+      <c r="E10" s="47" t="n">
+        <v>0.012727392769326</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="n">
-        <v>200</v>
-      </c>
-      <c r="B11" s="62" t="n">
-        <v>0.0274061332919906</v>
-      </c>
-      <c r="C11" s="43" t="n">
-        <v>0.0127060594733748</v>
-      </c>
-      <c r="D11" s="37" t="n">
-        <v>0.027365722909352</v>
-      </c>
-      <c r="E11" s="37" t="n">
-        <v>0.0125668499049907</v>
-      </c>
-      <c r="F11" s="62" t="n">
-        <v>0.0272377569689874</v>
-      </c>
-      <c r="G11" s="43" t="n">
-        <v>0.0124893482068401</v>
-      </c>
-      <c r="H11" s="60" t="n">
-        <v>0.0273365377234433</v>
-      </c>
-      <c r="I11" s="47" t="n">
-        <v>0.0125874191950685</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63" t="s">
+      <c r="A11" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="64" t="n">
-        <v>0.027383973228126</v>
-      </c>
-      <c r="C12" s="54" t="n">
-        <v>0.0125808681003325</v>
-      </c>
-      <c r="D12" s="64" t="n">
-        <v>0.027526273738826</v>
-      </c>
-      <c r="E12" s="54" t="n">
-        <v>0.0126549341208474</v>
-      </c>
-      <c r="F12" s="64" t="n">
-        <v>0.0272456058440576</v>
-      </c>
-      <c r="G12" s="54" t="n">
-        <v>0.0125195516467294</v>
-      </c>
-      <c r="H12" s="65" t="n">
-        <v>0.0273852842703365</v>
-      </c>
-      <c r="I12" s="56" t="n">
-        <v>0.0125851179559698</v>
+      <c r="B11" s="64" t="n">
+        <v>0.0127285663227923</v>
+      </c>
+      <c r="C11" s="144" t="n">
+        <v>0.0126259326870375</v>
+      </c>
+      <c r="D11" s="54" t="n">
+        <v>0.0126746231175818</v>
+      </c>
+      <c r="E11" s="56" t="n">
+        <v>0.0126763740424705</v>
       </c>
     </row>
   </sheetData>
@@ -35102,10 +35109,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q190"/>
+  <dimension ref="A1:Q273"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K149" activeCellId="0" sqref="K149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A176" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E202" activeCellId="0" sqref="E202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38520,15 +38527,15 @@
       </c>
       <c r="G138" s="0"/>
       <c r="H138" s="103"/>
-      <c r="I138" s="0"/>
+      <c r="I138" s="104" t="s">
+        <v>113</v>
+      </c>
       <c r="J138" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="K138" s="104" t="s">
         <v>32</v>
       </c>
+      <c r="K138" s="105"/>
       <c r="L138" s="105"/>
-      <c r="M138" s="105"/>
+      <c r="M138" s="0"/>
       <c r="N138" s="105"/>
       <c r="O138" s="105"/>
       <c r="P138" s="105"/>
@@ -38555,21 +38562,21 @@
       </c>
       <c r="G139" s="0"/>
       <c r="H139" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="I139" s="0"/>
+        <v>112</v>
+      </c>
+      <c r="I139" s="16" t="n">
+        <v>5</v>
+      </c>
       <c r="J139" s="16" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="K139" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="L139" s="16" t="n">
         <v>200</v>
       </c>
-      <c r="M139" s="108" t="s">
+      <c r="L139" s="108" t="s">
         <v>37</v>
       </c>
+      <c r="M139" s="0"/>
       <c r="N139" s="0"/>
       <c r="O139" s="109"/>
       <c r="P139" s="110"/>
@@ -38598,25 +38605,23 @@
       <c r="H140" s="85" t="n">
         <v>5</v>
       </c>
-      <c r="I140" s="112" t="s">
-        <v>115</v>
+      <c r="I140" s="112" t="n">
+        <v>0.0273219236613738</v>
       </c>
       <c r="J140" s="113" t="n">
-        <v>0.0273219236613738</v>
-      </c>
-      <c r="K140" s="114" t="n">
         <v>0.0272065054889437</v>
       </c>
-      <c r="L140" s="99" t="n">
+      <c r="K140" s="99" t="n">
         <v>0.0272350196025248</v>
       </c>
-      <c r="M140" s="115" t="n">
+      <c r="L140" s="114" t="n">
         <v>0.0272544829176141</v>
       </c>
+      <c r="M140" s="0"/>
       <c r="N140" s="0"/>
       <c r="O140" s="0"/>
-      <c r="P140" s="116"/>
-      <c r="Q140" s="117"/>
+      <c r="P140" s="115"/>
+      <c r="Q140" s="116"/>
     </row>
     <row r="141" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="74" t="n">
@@ -38641,21 +38646,19 @@
       <c r="H141" s="32" t="n">
         <v>100</v>
       </c>
-      <c r="I141" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="J141" s="88" t="n">
+      <c r="I141" s="88" t="n">
         <v>0.0274238627310136</v>
       </c>
-      <c r="K141" s="114" t="n">
+      <c r="J141" s="113" t="n">
         <v>0.0280065928181823</v>
       </c>
-      <c r="L141" s="88" t="n">
+      <c r="K141" s="88" t="n">
         <v>0.0272640409606607</v>
       </c>
-      <c r="M141" s="115" t="n">
+      <c r="L141" s="114" t="n">
         <v>0.0275648321699522</v>
       </c>
+      <c r="M141" s="0"/>
       <c r="N141" s="0"/>
       <c r="O141" s="0"/>
       <c r="P141" s="0"/>
@@ -38684,21 +38687,19 @@
       <c r="H142" s="32" t="n">
         <v>200</v>
       </c>
-      <c r="I142" s="112" t="s">
-        <v>115</v>
-      </c>
-      <c r="J142" s="101" t="n">
+      <c r="I142" s="101" t="n">
         <v>0.0274061332919906</v>
       </c>
-      <c r="K142" s="114" t="n">
+      <c r="J142" s="113" t="n">
         <v>0.027365722909352</v>
       </c>
-      <c r="L142" s="101" t="n">
+      <c r="K142" s="101" t="n">
         <v>0.0272377569689874</v>
       </c>
-      <c r="M142" s="115" t="n">
+      <c r="L142" s="114" t="n">
         <v>0.0273365377234433</v>
       </c>
+      <c r="M142" s="0"/>
       <c r="N142" s="0"/>
       <c r="O142" s="0"/>
       <c r="P142" s="0"/>
@@ -38727,21 +38728,19 @@
       <c r="H143" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="I143" s="112" t="s">
-        <v>115</v>
+      <c r="I143" s="93" t="n">
+        <v>0.027383973228126</v>
       </c>
       <c r="J143" s="93" t="n">
-        <v>0.027383973228126</v>
+        <v>0.027526273738826</v>
       </c>
       <c r="K143" s="93" t="n">
-        <v>0.027526273738826</v>
-      </c>
-      <c r="L143" s="93" t="n">
         <v>0.0272456058440576</v>
       </c>
-      <c r="M143" s="118" t="n">
+      <c r="L143" s="117" t="n">
         <v>0.0273852842703365</v>
       </c>
+      <c r="M143" s="0"/>
       <c r="N143" s="0"/>
       <c r="O143" s="0"/>
       <c r="P143" s="0"/>
@@ -38830,15 +38829,15 @@
       </c>
       <c r="G146" s="0"/>
       <c r="H146" s="103"/>
-      <c r="I146" s="0"/>
+      <c r="I146" s="104" t="s">
+        <v>113</v>
+      </c>
       <c r="J146" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="K146" s="104" t="s">
         <v>32</v>
       </c>
+      <c r="K146" s="105"/>
       <c r="L146" s="105"/>
-      <c r="M146" s="105"/>
+      <c r="M146" s="0"/>
       <c r="N146" s="0"/>
       <c r="O146" s="0"/>
       <c r="P146" s="0"/>
@@ -38865,21 +38864,21 @@
       </c>
       <c r="G147" s="0"/>
       <c r="H147" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="I147" s="0"/>
+        <v>112</v>
+      </c>
+      <c r="I147" s="16" t="n">
+        <v>5</v>
+      </c>
       <c r="J147" s="16" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="K147" s="16" t="n">
-        <v>100</v>
-      </c>
-      <c r="L147" s="16" t="n">
         <v>200</v>
       </c>
-      <c r="M147" s="108" t="s">
+      <c r="L147" s="108" t="s">
         <v>37</v>
       </c>
+      <c r="M147" s="0"/>
       <c r="O147" s="0"/>
       <c r="P147" s="0"/>
       <c r="Q147" s="0"/>
@@ -38907,21 +38906,19 @@
       <c r="H148" s="85" t="n">
         <v>5</v>
       </c>
-      <c r="I148" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="J148" s="119" t="n">
+      <c r="I148" s="118" t="n">
         <v>0.0124849115003355</v>
       </c>
-      <c r="K148" s="114" t="n">
+      <c r="J148" s="113" t="n">
         <v>0.012576419198419</v>
       </c>
+      <c r="K148" s="119" t="n">
+        <v>0.0125466987406911</v>
+      </c>
       <c r="L148" s="120" t="n">
-        <v>0.0125466987406911</v>
-      </c>
-      <c r="M148" s="121" t="n">
         <v>0.0125360098131485</v>
       </c>
+      <c r="M148" s="0"/>
       <c r="N148" s="0"/>
       <c r="O148" s="0"/>
       <c r="P148" s="0"/>
@@ -38949,21 +38946,19 @@
       <c r="H149" s="32" t="n">
         <v>100</v>
       </c>
-      <c r="I149" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="J149" s="122" t="n">
+      <c r="I149" s="121" t="n">
         <v>0.0125516333272871</v>
       </c>
-      <c r="K149" s="114" t="n">
+      <c r="J149" s="113" t="n">
         <v>0.0128215332591325</v>
       </c>
+      <c r="K149" s="121" t="n">
+        <v>0.0125226079926572</v>
+      </c>
       <c r="L149" s="122" t="n">
-        <v>0.0125226079926572</v>
-      </c>
-      <c r="M149" s="123" t="n">
         <v>0.0126319248596923</v>
       </c>
+      <c r="M149" s="0"/>
       <c r="N149" s="0"/>
     </row>
     <row r="150" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38989,21 +38984,19 @@
       <c r="H150" s="32" t="n">
         <v>200</v>
       </c>
-      <c r="I150" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="J150" s="124" t="n">
+      <c r="I150" s="123" t="n">
         <v>0.0127060594733748</v>
       </c>
-      <c r="K150" s="114" t="n">
+      <c r="J150" s="113" t="n">
         <v>0.0125668499049907</v>
       </c>
+      <c r="K150" s="123" t="n">
+        <v>0.0124893482068401</v>
+      </c>
       <c r="L150" s="124" t="n">
-        <v>0.0124893482068401</v>
-      </c>
-      <c r="M150" s="125" t="n">
         <v>0.0125874191950685</v>
       </c>
+      <c r="M150" s="0"/>
       <c r="N150" s="0"/>
     </row>
     <row r="151" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39029,21 +39022,19 @@
       <c r="H151" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="I151" s="109" t="s">
-        <v>116</v>
-      </c>
-      <c r="J151" s="126" t="n">
+      <c r="I151" s="125" t="n">
         <v>0.0125808681003325</v>
       </c>
-      <c r="K151" s="126" t="n">
+      <c r="J151" s="125" t="n">
         <v>0.0126549341208474</v>
       </c>
+      <c r="K151" s="125" t="n">
+        <v>0.0125195516467294</v>
+      </c>
       <c r="L151" s="126" t="n">
-        <v>0.0125195516467294</v>
-      </c>
-      <c r="M151" s="127" t="n">
         <v>0.0125851179559698</v>
       </c>
+      <c r="M151" s="0"/>
       <c r="N151" s="0"/>
     </row>
     <row r="152" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39972,6 +39963,2323 @@
       <c r="G190" s="0"/>
       <c r="M190" s="0"/>
       <c r="N190" s="0"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B191" s="0"/>
+      <c r="C191" s="0"/>
+      <c r="D191" s="0"/>
+      <c r="E191" s="0"/>
+      <c r="F191" s="0"/>
+      <c r="G191" s="0"/>
+      <c r="M191" s="0"/>
+      <c r="N191" s="0"/>
+    </row>
+    <row r="192" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="B192" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="C192" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="D192" s="74" t="s">
+        <v>114</v>
+      </c>
+      <c r="E192" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="F192" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="G192" s="0"/>
+      <c r="M192" s="0"/>
+      <c r="N192" s="0"/>
+    </row>
+    <row r="193" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C193" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D193" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E193" s="0" t="n">
+        <v>0.0278093531209519</v>
+      </c>
+      <c r="F193" s="74" t="n">
+        <v>0.0144944724806178</v>
+      </c>
+      <c r="G193" s="0"/>
+      <c r="L193" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M193" s="0"/>
+      <c r="N193" s="0"/>
+    </row>
+    <row r="194" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D194" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="E194" s="0" t="n">
+        <v>0.0277761435152246</v>
+      </c>
+      <c r="F194" s="74" t="n">
+        <v>0.0136635224431527</v>
+      </c>
+      <c r="G194" s="0"/>
+      <c r="L194" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M194" s="0"/>
+      <c r="N194" s="0"/>
+    </row>
+    <row r="195" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D195" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E195" s="0" t="n">
+        <v>0.0278027096699477</v>
+      </c>
+      <c r="F195" s="74" t="n">
+        <v>0.0144442701130392</v>
+      </c>
+      <c r="G195" s="0"/>
+      <c r="H195" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I195" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="J195" s="84" t="s">
+        <v>116</v>
+      </c>
+      <c r="K195" s="0"/>
+      <c r="L195" s="0"/>
+      <c r="N195" s="0"/>
+    </row>
+    <row r="196" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="D196" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="E196" s="0" t="n">
+        <v>0.0272586871352166</v>
+      </c>
+      <c r="F196" s="74" t="n">
+        <v>0.0124626718123526</v>
+      </c>
+      <c r="G196" s="0"/>
+      <c r="H196" s="85" t="n">
+        <v>400</v>
+      </c>
+      <c r="I196" s="86" t="n">
+        <v>0.0278094296388933</v>
+      </c>
+      <c r="J196" s="87" t="n">
+        <v>0.0145895475922837</v>
+      </c>
+      <c r="K196" s="0"/>
+      <c r="L196" s="0"/>
+      <c r="N196" s="0"/>
+    </row>
+    <row r="197" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C197" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D197" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="E197" s="0" t="n">
+        <v>0.028720556953706</v>
+      </c>
+      <c r="F197" s="74" t="n">
+        <v>0.0145700433128921</v>
+      </c>
+      <c r="G197" s="0"/>
+      <c r="H197" s="90" t="n">
+        <v>500</v>
+      </c>
+      <c r="I197" s="127" t="n">
+        <v>0.0273786504619397</v>
+      </c>
+      <c r="J197" s="128" t="n">
+        <v>0.0130957724060765</v>
+      </c>
+      <c r="K197" s="0"/>
+      <c r="L197" s="0"/>
+      <c r="N197" s="0"/>
+    </row>
+    <row r="198" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B198" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C198" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D198" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E198" s="74" t="n">
+        <v>0.027893601286958</v>
+      </c>
+      <c r="F198" s="74" t="n">
+        <v>0.0147712236902055</v>
+      </c>
+      <c r="G198" s="0"/>
+      <c r="H198" s="32" t="n">
+        <v>600</v>
+      </c>
+      <c r="I198" s="101" t="n">
+        <v>0.0278380981961415</v>
+      </c>
+      <c r="J198" s="102" t="n">
+        <v>0.0140979857561359</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B199" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C199" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D199" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E199" s="74" t="n">
+        <v>0.0277932846262325</v>
+      </c>
+      <c r="F199" s="74" t="n">
+        <v>0.0145415368437708</v>
+      </c>
+      <c r="G199" s="0"/>
+      <c r="H199" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I199" s="93" t="n">
+        <v>0.0276753927656582</v>
+      </c>
+      <c r="J199" s="94" t="n">
+        <v>0.013927768584832</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B200" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C200" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D200" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E200" s="74" t="n">
+        <v>0.0272529773626372</v>
+      </c>
+      <c r="F200" s="74" t="n">
+        <v>0.0129613077507679</v>
+      </c>
+      <c r="G200" s="0"/>
+      <c r="I200" s="95"/>
+      <c r="J200" s="95"/>
+    </row>
+    <row r="201" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B201" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C201" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D201" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E201" s="74" t="n">
+        <v>0.0273247498138547</v>
+      </c>
+      <c r="F201" s="74" t="n">
+        <v>0.0141643402888762</v>
+      </c>
+      <c r="G201" s="0"/>
+      <c r="I201" s="95"/>
+      <c r="J201" s="95"/>
+    </row>
+    <row r="202" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B202" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C202" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D202" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E202" s="74" t="n">
+        <v>0.0277831732658871</v>
+      </c>
+      <c r="F202" s="74" t="n">
+        <v>0.0139352669511624</v>
+      </c>
+      <c r="G202" s="0"/>
+      <c r="H202" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="I202" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="J202" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="M202" s="0"/>
+    </row>
+    <row r="203" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B203" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C203" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D203" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E203" s="74" t="n">
+        <v>0.0277514009752104</v>
+      </c>
+      <c r="F203" s="74" t="n">
+        <v>0.0146663835881702</v>
+      </c>
+      <c r="G203" s="0"/>
+      <c r="H203" s="129" t="n">
+        <v>200</v>
+      </c>
+      <c r="I203" s="112" t="n">
+        <v>0.0276897360017143</v>
+      </c>
+      <c r="J203" s="130" t="n">
+        <v>0.0137611730277449</v>
+      </c>
+      <c r="K203" s="0"/>
+      <c r="L203" s="0"/>
+      <c r="M203" s="0"/>
+    </row>
+    <row r="204" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B204" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C204" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D204" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E204" s="74" t="n">
+        <v>0.0277603267167707</v>
+      </c>
+      <c r="F204" s="74" t="n">
+        <v>0.0136192856959921</v>
+      </c>
+      <c r="G204" s="0"/>
+      <c r="H204" s="131" t="n">
+        <v>300</v>
+      </c>
+      <c r="I204" s="132" t="n">
+        <v>0.0277088995982071</v>
+      </c>
+      <c r="J204" s="133" t="n">
+        <v>0.0143475438655268</v>
+      </c>
+      <c r="K204" s="0"/>
+      <c r="L204" s="0"/>
+      <c r="M204" s="0"/>
+    </row>
+    <row r="205" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B205" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C205" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D205" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E205" s="74" t="n">
+        <v>0.0272165003166818</v>
+      </c>
+      <c r="F205" s="74" t="n">
+        <v>0.0125179051917055</v>
+      </c>
+      <c r="G205" s="0"/>
+      <c r="H205" s="90" t="n">
+        <v>400</v>
+      </c>
+      <c r="I205" s="91" t="n">
+        <v>0.027627542697053</v>
+      </c>
+      <c r="J205" s="92" t="n">
+        <v>0.0136745888612243</v>
+      </c>
+      <c r="K205" s="0"/>
+      <c r="L205" s="0"/>
+      <c r="M205" s="0"/>
+    </row>
+    <row r="206" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B206" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C206" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D206" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E206" s="74" t="n">
+        <v>0.0278078167612897</v>
+      </c>
+      <c r="F206" s="74" t="n">
+        <v>0.0134995784610357</v>
+      </c>
+      <c r="G206" s="0"/>
+      <c r="H206" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I206" s="93" t="n">
+        <v>0.0276753927656582</v>
+      </c>
+      <c r="J206" s="94" t="n">
+        <v>0.013927768584832</v>
+      </c>
+      <c r="K206" s="0"/>
+      <c r="L206" s="0"/>
+      <c r="M206" s="0"/>
+    </row>
+    <row r="207" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B207" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C207" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D207" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E207" s="74" t="n">
+        <v>0.0271518106329575</v>
+      </c>
+      <c r="F207" s="74" t="n">
+        <v>0.0128308424597175</v>
+      </c>
+      <c r="G207" s="0"/>
+      <c r="I207" s="95"/>
+      <c r="J207" s="95"/>
+      <c r="M207" s="0"/>
+    </row>
+    <row r="208" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B208" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C208" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D208" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E208" s="74" t="n">
+        <v>0.0276824073742217</v>
+      </c>
+      <c r="F208" s="74" t="n">
+        <v>0.0145491358906348</v>
+      </c>
+      <c r="G208" s="0"/>
+      <c r="I208" s="95"/>
+      <c r="J208" s="95"/>
+      <c r="M208" s="0"/>
+    </row>
+    <row r="209" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B209" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C209" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D209" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E209" s="74" t="n">
+        <v>0.0276779780809594</v>
+      </c>
+      <c r="F209" s="74" t="n">
+        <v>0.0147249158496426</v>
+      </c>
+      <c r="G209" s="0"/>
+      <c r="H209" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I209" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="J209" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="M209" s="0"/>
+    </row>
+    <row r="210" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B210" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C210" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D210" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E210" s="74" t="n">
+        <v>0.0276915940591702</v>
+      </c>
+      <c r="F210" s="74" t="n">
+        <v>0.0131886148885506</v>
+      </c>
+      <c r="G210" s="0"/>
+      <c r="H210" s="85" t="n">
+        <v>5</v>
+      </c>
+      <c r="I210" s="86" t="n">
+        <v>0.0276950645205097</v>
+      </c>
+      <c r="J210" s="87" t="n">
+        <v>0.0139410199778784</v>
+      </c>
+      <c r="M210" s="0"/>
+    </row>
+    <row r="211" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B211" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C211" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D211" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E211" s="74" t="n">
+        <v>0.0280526200881892</v>
+      </c>
+      <c r="F211" s="74" t="n">
+        <v>0.0179188500308673</v>
+      </c>
+      <c r="G211" s="0"/>
+      <c r="H211" s="90" t="n">
+        <v>10</v>
+      </c>
+      <c r="I211" s="127" t="n">
+        <v>0.0277262747361297</v>
+      </c>
+      <c r="J211" s="128" t="n">
+        <v>0.0137923450444142</v>
+      </c>
+      <c r="M211" s="0"/>
+    </row>
+    <row r="212" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B212" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C212" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D212" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E212" s="74" t="n">
+        <v>0.0272125604602303</v>
+      </c>
+      <c r="F212" s="74" t="n">
+        <v>0.0130195443703591</v>
+      </c>
+      <c r="G212" s="0"/>
+      <c r="H212" s="32" t="n">
+        <v>15</v>
+      </c>
+      <c r="I212" s="101" t="n">
+        <v>0.0276048390403351</v>
+      </c>
+      <c r="J212" s="102" t="n">
+        <v>0.0140499407322035</v>
+      </c>
+      <c r="M212" s="0"/>
+    </row>
+    <row r="213" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B213" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C213" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D213" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E213" s="74" t="n">
+        <v>0.0277700110639005</v>
+      </c>
+      <c r="F213" s="74" t="n">
+        <v>0.0146773956393</v>
+      </c>
+      <c r="G213" s="0"/>
+      <c r="H213" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I213" s="93" t="n">
+        <v>0.0276753927656582</v>
+      </c>
+      <c r="J213" s="94" t="n">
+        <v>0.013927768584832</v>
+      </c>
+      <c r="M213" s="0"/>
+    </row>
+    <row r="214" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B214" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C214" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D214" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E214" s="74" t="n">
+        <v>0.0277024746583089</v>
+      </c>
+      <c r="F214" s="74" t="n">
+        <v>0.0135933831360492</v>
+      </c>
+      <c r="G214" s="0"/>
+      <c r="I214" s="95"/>
+      <c r="J214" s="95"/>
+      <c r="M214" s="0"/>
+    </row>
+    <row r="215" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B215" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C215" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D215" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E215" s="74" t="n">
+        <v>0.0273053628853176</v>
+      </c>
+      <c r="F215" s="74" t="n">
+        <v>0.0125526970280986</v>
+      </c>
+      <c r="G215" s="0"/>
+      <c r="I215" s="95"/>
+      <c r="J215" s="95"/>
+      <c r="M215" s="0"/>
+    </row>
+    <row r="216" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B216" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C216" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D216" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E216" s="74" t="n">
+        <v>0.0277550542727464</v>
+      </c>
+      <c r="F216" s="74" t="n">
+        <v>0.0127112741427428</v>
+      </c>
+      <c r="G216" s="0"/>
+      <c r="H216" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="I216" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="J216" s="97" t="s">
+        <v>116</v>
+      </c>
+      <c r="M216" s="0"/>
+    </row>
+    <row r="217" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B217" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C217" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D217" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E217" s="74" t="n">
+        <v>0.0273701311001188</v>
+      </c>
+      <c r="F217" s="74" t="n">
+        <v>0.0126134575699191</v>
+      </c>
+      <c r="G217" s="0"/>
+      <c r="H217" s="85" t="n">
+        <v>5</v>
+      </c>
+      <c r="I217" s="86" t="n">
+        <v>0.0276577471559041</v>
+      </c>
+      <c r="J217" s="87" t="n">
+        <v>0.0142029345720774</v>
+      </c>
+      <c r="M217" s="0"/>
+    </row>
+    <row r="218" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B218" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C218" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D218" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E218" s="74" t="n">
+        <v>0.0277981416468563</v>
+      </c>
+      <c r="F218" s="74" t="n">
+        <v>0.0146285546792296</v>
+      </c>
+      <c r="G218" s="0"/>
+      <c r="H218" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="I218" s="88" t="n">
+        <v>0.0277317565588921</v>
+      </c>
+      <c r="J218" s="89" t="n">
+        <v>0.0138793923649663</v>
+      </c>
+      <c r="M218" s="0"/>
+    </row>
+    <row r="219" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B219" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C219" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D219" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E219" s="74" t="n">
+        <v>0.027487302185228</v>
+      </c>
+      <c r="F219" s="74" t="n">
+        <v>0.0128531800817593</v>
+      </c>
+      <c r="G219" s="0"/>
+      <c r="H219" s="90" t="n">
+        <v>15</v>
+      </c>
+      <c r="I219" s="91" t="n">
+        <v>0.0276366745821783</v>
+      </c>
+      <c r="J219" s="92" t="n">
+        <v>0.0137009788174524</v>
+      </c>
+      <c r="M219" s="0"/>
+    </row>
+    <row r="220" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B220" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C220" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D220" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E220" s="74" t="n">
+        <v>0.0276663858624463</v>
+      </c>
+      <c r="F220" s="74" t="n">
+        <v>0.014447679417254</v>
+      </c>
+      <c r="G220" s="0"/>
+      <c r="H220" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="I220" s="93" t="n">
+        <v>0.0276753927656582</v>
+      </c>
+      <c r="J220" s="94" t="n">
+        <v>0.013927768584832</v>
+      </c>
+      <c r="M220" s="0"/>
+    </row>
+    <row r="221" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B221" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C221" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D221" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E221" s="74" t="n">
+        <v>0.0272665363842072</v>
+      </c>
+      <c r="F221" s="74" t="n">
+        <v>0.0126006877706183</v>
+      </c>
+      <c r="G221" s="0"/>
+      <c r="H221" s="0"/>
+      <c r="I221" s="0"/>
+      <c r="J221" s="0"/>
+      <c r="M221" s="0"/>
+    </row>
+    <row r="222" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B222" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C222" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D222" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E222" s="74" t="n">
+        <v>0.0277747590940481</v>
+      </c>
+      <c r="F222" s="74" t="n">
+        <v>0.0145827983693263</v>
+      </c>
+      <c r="G222" s="0"/>
+      <c r="M222" s="0"/>
+    </row>
+    <row r="223" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B223" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C223" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D223" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E223" s="74" t="n">
+        <v>0.0278074471434338</v>
+      </c>
+      <c r="F223" s="74" t="n">
+        <v>0.0146182713817412</v>
+      </c>
+      <c r="G223" s="0"/>
+      <c r="H223" s="103"/>
+      <c r="I223" s="104" t="s">
+        <v>113</v>
+      </c>
+      <c r="J223" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="K223" s="105"/>
+      <c r="L223" s="105"/>
+      <c r="M223" s="0"/>
+    </row>
+    <row r="224" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B224" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C224" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D224" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E224" s="74" t="n">
+        <v>0.0277425010147322</v>
+      </c>
+      <c r="F224" s="74" t="n">
+        <v>0.013577586437554</v>
+      </c>
+      <c r="G224" s="0"/>
+      <c r="H224" s="107" t="s">
+        <v>112</v>
+      </c>
+      <c r="I224" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J224" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="K224" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="L224" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="M224" s="0"/>
+    </row>
+    <row r="225" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B225" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C225" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D225" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E225" s="74" t="n">
+        <v>0.0272176386166153</v>
+      </c>
+      <c r="F225" s="74" t="n">
+        <v>0.0129181685606768</v>
+      </c>
+      <c r="G225" s="0"/>
+      <c r="H225" s="85" t="n">
+        <v>5</v>
+      </c>
+      <c r="I225" s="86" t="n">
+        <v>0.0273053628853176</v>
+      </c>
+      <c r="J225" s="134" t="n">
+        <v>0.0272586871352166</v>
+      </c>
+      <c r="K225" s="119" t="n">
+        <v>0.0277550542727464</v>
+      </c>
+      <c r="L225" s="120" t="n">
+        <v>0.0274397014310935</v>
+      </c>
+      <c r="M225" s="0"/>
+    </row>
+    <row r="226" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B226" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C226" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D226" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E226" s="74" t="n">
+        <v>0.027733973046727</v>
+      </c>
+      <c r="F226" s="74" t="n">
+        <v>0.0146769484786268</v>
+      </c>
+      <c r="G226" s="0"/>
+      <c r="H226" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="I226" s="88" t="n">
+        <v>0.0273701311001188</v>
+      </c>
+      <c r="J226" s="113" t="n">
+        <v>0.027487302185228</v>
+      </c>
+      <c r="K226" s="121" t="n">
+        <v>0.0273786645058657</v>
+      </c>
+      <c r="L226" s="122" t="n">
+        <v>0.0274120325970708</v>
+      </c>
+      <c r="M226" s="0"/>
+    </row>
+    <row r="227" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B227" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C227" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D227" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E227" s="74" t="n">
+        <v>0.0277810733875579</v>
+      </c>
+      <c r="F227" s="74" t="n">
+        <v>0.0144243801639859</v>
+      </c>
+      <c r="G227" s="0"/>
+      <c r="H227" s="32" t="n">
+        <v>15</v>
+      </c>
+      <c r="I227" s="91" t="n">
+        <v>0.0272125604602303</v>
+      </c>
+      <c r="J227" s="135" t="n">
+        <v>0.0273051667088274</v>
+      </c>
+      <c r="K227" s="123" t="n">
+        <v>0.0272665363842072</v>
+      </c>
+      <c r="L227" s="124" t="n">
+        <v>0.0272614211844216</v>
+      </c>
+      <c r="M227" s="0"/>
+    </row>
+    <row r="228" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B228" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C228" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D228" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E228" s="74" t="n">
+        <v>0.0272646346878384</v>
+      </c>
+      <c r="F228" s="74" t="n">
+        <v>0.012553507352753</v>
+      </c>
+      <c r="G228" s="0"/>
+      <c r="H228" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="I228" s="93" t="n">
+        <v>0.0272960181485556</v>
+      </c>
+      <c r="J228" s="136" t="n">
+        <v>0.0273503853430907</v>
+      </c>
+      <c r="K228" s="125" t="n">
+        <v>0.0274667517209397</v>
+      </c>
+      <c r="L228" s="126" t="n">
+        <v>0.0273710517375287</v>
+      </c>
+      <c r="M228" s="0"/>
+    </row>
+    <row r="229" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B229" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C229" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D229" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E229" s="74" t="n">
+        <v>0.0277320560480617</v>
+      </c>
+      <c r="F229" s="74" t="n">
+        <v>0.0150204530639004</v>
+      </c>
+      <c r="G229" s="0"/>
+      <c r="H229" s="0"/>
+      <c r="I229" s="0"/>
+      <c r="J229" s="0"/>
+      <c r="K229" s="0"/>
+      <c r="L229" s="0"/>
+      <c r="M229" s="0"/>
+    </row>
+    <row r="230" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B230" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C230" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D230" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E230" s="74" t="n">
+        <v>0.0277505237748832</v>
+      </c>
+      <c r="F230" s="74" t="n">
+        <v>0.0135403040432141</v>
+      </c>
+      <c r="G230" s="0"/>
+      <c r="H230" s="0"/>
+      <c r="I230" s="0"/>
+      <c r="J230" s="0"/>
+      <c r="K230" s="0"/>
+      <c r="L230" s="0"/>
+      <c r="M230" s="0"/>
+    </row>
+    <row r="231" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B231" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C231" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D231" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E231" s="74" t="n">
+        <v>0.027356920053565</v>
+      </c>
+      <c r="F231" s="74" t="n">
+        <v>0.0125839403117134</v>
+      </c>
+      <c r="G231" s="0"/>
+      <c r="H231" s="103"/>
+      <c r="I231" s="104" t="s">
+        <v>113</v>
+      </c>
+      <c r="J231" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="K231" s="105"/>
+      <c r="L231" s="105"/>
+      <c r="M231" s="0"/>
+    </row>
+    <row r="232" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B232" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C232" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D232" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E232" s="74" t="n">
+        <v>0.0276964748558608</v>
+      </c>
+      <c r="F232" s="74" t="n">
+        <v>0.0145834620931173</v>
+      </c>
+      <c r="G232" s="0"/>
+      <c r="H232" s="107" t="s">
+        <v>112</v>
+      </c>
+      <c r="I232" s="16" t="n">
+        <v>5</v>
+      </c>
+      <c r="J232" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="K232" s="16" t="n">
+        <v>15</v>
+      </c>
+      <c r="L232" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="M232" s="0"/>
+    </row>
+    <row r="233" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B233" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C233" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D233" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E233" s="74" t="n">
+        <v>0.027295362988569</v>
+      </c>
+      <c r="F233" s="74" t="n">
+        <v>0.0125593682039823</v>
+      </c>
+      <c r="G233" s="0"/>
+      <c r="H233" s="85" t="n">
+        <v>5</v>
+      </c>
+      <c r="I233" s="86" t="n">
+        <v>0.0125526970280986</v>
+      </c>
+      <c r="J233" s="137" t="n">
+        <v>0.0124626718123526</v>
+      </c>
+      <c r="K233" s="119" t="n">
+        <v>0.0127112741427428</v>
+      </c>
+      <c r="L233" s="120" t="n">
+        <v>0.0125755476610647</v>
+      </c>
+      <c r="M233" s="0"/>
+    </row>
+    <row r="234" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B234" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C234" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D234" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E234" s="74" t="n">
+        <v>0.0273043879412292</v>
+      </c>
+      <c r="F234" s="74" t="n">
+        <v>0.0130994176227148</v>
+      </c>
+      <c r="G234" s="0"/>
+      <c r="H234" s="32" t="n">
+        <v>10</v>
+      </c>
+      <c r="I234" s="88" t="n">
+        <v>0.0126134575699191</v>
+      </c>
+      <c r="J234" s="113" t="n">
+        <v>0.0128531800817593</v>
+      </c>
+      <c r="K234" s="121" t="n">
+        <v>0.0127119074393845</v>
+      </c>
+      <c r="L234" s="122" t="n">
+        <v>0.012726181697021</v>
+      </c>
+      <c r="M234" s="0"/>
+    </row>
+    <row r="235" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B235" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C235" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D235" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E235" s="74" t="n">
+        <v>0.0277726083903836</v>
+      </c>
+      <c r="F235" s="74" t="n">
+        <v>0.014737372536367</v>
+      </c>
+      <c r="G235" s="0"/>
+      <c r="H235" s="32" t="n">
+        <v>15</v>
+      </c>
+      <c r="I235" s="101" t="n">
+        <v>0.0130195443703591</v>
+      </c>
+      <c r="J235" s="135" t="n">
+        <v>0.0125619461670006</v>
+      </c>
+      <c r="K235" s="123" t="n">
+        <v>0.0126006877706183</v>
+      </c>
+      <c r="L235" s="124" t="n">
+        <v>0.012727392769326</v>
+      </c>
+      <c r="M235" s="0"/>
+    </row>
+    <row r="236" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B236" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C236" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D236" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E236" s="74" t="n">
+        <v>0.0277175303354732</v>
+      </c>
+      <c r="F236" s="74" t="n">
+        <v>0.0146138642072471</v>
+      </c>
+      <c r="G236" s="0"/>
+      <c r="H236" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="I236" s="93" t="n">
+        <v>0.0127285663227923</v>
+      </c>
+      <c r="J236" s="136" t="n">
+        <v>0.0126259326870375</v>
+      </c>
+      <c r="K236" s="125" t="n">
+        <v>0.0126746231175818</v>
+      </c>
+      <c r="L236" s="126" t="n">
+        <v>0.0126763740424705</v>
+      </c>
+      <c r="M236" s="0"/>
+    </row>
+    <row r="237" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B237" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C237" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D237" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E237" s="74" t="n">
+        <v>0.0272657333347741</v>
+      </c>
+      <c r="F237" s="74" t="n">
+        <v>0.0126195881608499</v>
+      </c>
+      <c r="G237" s="0"/>
+      <c r="L237" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M237" s="0"/>
+    </row>
+    <row r="238" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B238" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C238" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D238" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E238" s="74" t="n">
+        <v>0.0278050211434735</v>
+      </c>
+      <c r="F238" s="74" t="n">
+        <v>0.0136398821003798</v>
+      </c>
+      <c r="G238" s="0"/>
+      <c r="L238" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M238" s="0"/>
+    </row>
+    <row r="239" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B239" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C239" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D239" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E239" s="74" t="n">
+        <v>0.0273060852930813</v>
+      </c>
+      <c r="F239" s="74" t="n">
+        <v>0.0126598859582523</v>
+      </c>
+      <c r="G239" s="0"/>
+      <c r="L239" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M239" s="0"/>
+    </row>
+    <row r="240" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B240" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C240" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D240" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E240" s="74" t="n">
+        <v>0.0279257951748146</v>
+      </c>
+      <c r="F240" s="74" t="n">
+        <v>0.015054577629523</v>
+      </c>
+      <c r="G240" s="0"/>
+      <c r="L240" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M240" s="0"/>
+    </row>
+    <row r="241" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B241" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C241" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D241" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E241" s="74" t="n">
+        <v>0.0273786645058657</v>
+      </c>
+      <c r="F241" s="74" t="n">
+        <v>0.0127119074393845</v>
+      </c>
+      <c r="G241" s="0"/>
+      <c r="L241" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M241" s="0"/>
+    </row>
+    <row r="242" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B242" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C242" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D242" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E242" s="74" t="n">
+        <v>0.0277366060793134</v>
+      </c>
+      <c r="F242" s="74" t="n">
+        <v>0.0145150336399124</v>
+      </c>
+      <c r="G242" s="0"/>
+      <c r="L242" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M242" s="0"/>
+    </row>
+    <row r="243" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B243" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C243" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D243" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E243" s="74" t="n">
+        <v>0.0277668783301186</v>
+      </c>
+      <c r="F243" s="74" t="n">
+        <v>0.0144284699817252</v>
+      </c>
+      <c r="G243" s="0"/>
+      <c r="L243" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M243" s="0"/>
+    </row>
+    <row r="244" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B244" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C244" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D244" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E244" s="74" t="n">
+        <v>0.0277981288577423</v>
+      </c>
+      <c r="F244" s="74" t="n">
+        <v>0.0134735112809735</v>
+      </c>
+      <c r="G244" s="0"/>
+      <c r="L244" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M244" s="0"/>
+    </row>
+    <row r="245" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B245" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C245" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D245" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E245" s="74" t="n">
+        <v>0.027690100844877</v>
+      </c>
+      <c r="F245" s="74" t="n">
+        <v>0.0136895347200016</v>
+      </c>
+      <c r="G245" s="0"/>
+      <c r="L245" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M245" s="0"/>
+    </row>
+    <row r="246" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B246" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C246" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D246" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E246" s="74" t="n">
+        <v>0.0277773462332775</v>
+      </c>
+      <c r="F246" s="74" t="n">
+        <v>0.0139182999004304</v>
+      </c>
+      <c r="G246" s="0"/>
+      <c r="L246" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M246" s="0"/>
+    </row>
+    <row r="247" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B247" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C247" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D247" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E247" s="74" t="n">
+        <v>0.0279948252467428</v>
+      </c>
+      <c r="F247" s="74" t="n">
+        <v>0.0169496831740034</v>
+      </c>
+      <c r="G247" s="0"/>
+      <c r="L247" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M247" s="0"/>
+    </row>
+    <row r="248" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B248" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C248" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D248" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E248" s="74" t="n">
+        <v>0.0277828978231535</v>
+      </c>
+      <c r="F248" s="74" t="n">
+        <v>0.0146555958641398</v>
+      </c>
+      <c r="G248" s="0"/>
+      <c r="L248" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M248" s="0"/>
+    </row>
+    <row r="249" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B249" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C249" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D249" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E249" s="74" t="n">
+        <v>0.0273051667088274</v>
+      </c>
+      <c r="F249" s="74" t="n">
+        <v>0.0125619461670006</v>
+      </c>
+      <c r="G249" s="0"/>
+      <c r="L249" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M249" s="0"/>
+    </row>
+    <row r="250" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B250" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C250" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D250" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E250" s="74" t="n">
+        <v>0.0278709661161988</v>
+      </c>
+      <c r="F250" s="74" t="n">
+        <v>0.0145309769772272</v>
+      </c>
+      <c r="G250" s="0"/>
+      <c r="L250" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M250" s="0"/>
+    </row>
+    <row r="251" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B251" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C251" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D251" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E251" s="74" t="n">
+        <v>0.0277268761976726</v>
+      </c>
+      <c r="F251" s="74" t="n">
+        <v>0.0145924929424003</v>
+      </c>
+      <c r="G251" s="0"/>
+      <c r="L251" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M251" s="0"/>
+    </row>
+    <row r="252" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B252" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C252" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D252" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E252" s="74" t="n">
+        <v>0.0273683398064657</v>
+      </c>
+      <c r="F252" s="74" t="n">
+        <v>0.0124709825464683</v>
+      </c>
+      <c r="G252" s="0"/>
+      <c r="L252" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M252" s="0"/>
+    </row>
+    <row r="253" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B253" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C253" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D253" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E253" s="74" t="n">
+        <v>0.0277333989059793</v>
+      </c>
+      <c r="F253" s="74" t="n">
+        <v>0.0144967973288582</v>
+      </c>
+      <c r="G253" s="0"/>
+      <c r="L253" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M253" s="0"/>
+    </row>
+    <row r="254" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B254" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C254" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D254" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E254" s="74" t="n">
+        <v>0.0272158467188324</v>
+      </c>
+      <c r="F254" s="74" t="n">
+        <v>0.0126226019950381</v>
+      </c>
+      <c r="G254" s="0"/>
+      <c r="L254" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M254" s="0"/>
+    </row>
+    <row r="255" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B255" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C255" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D255" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E255" s="74" t="n">
+        <v>0.0278248932349117</v>
+      </c>
+      <c r="F255" s="74" t="n">
+        <v>0.0134529846877591</v>
+      </c>
+      <c r="G255" s="0"/>
+      <c r="L255" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M255" s="0"/>
+    </row>
+    <row r="256" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B256" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C256" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D256" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E256" s="74" t="n">
+        <v>0.0277531030510179</v>
+      </c>
+      <c r="F256" s="74" t="n">
+        <v>0.0134692429531631</v>
+      </c>
+      <c r="G256" s="0"/>
+      <c r="L256" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M256" s="0"/>
+    </row>
+    <row r="257" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B257" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C257" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D257" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E257" s="74" t="n">
+        <v>0.0279109589248243</v>
+      </c>
+      <c r="F257" s="74" t="n">
+        <v>0.0164513402044849</v>
+      </c>
+      <c r="G257" s="0"/>
+      <c r="L257" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M257" s="0"/>
+    </row>
+    <row r="258" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B258" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C258" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D258" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E258" s="74" t="n">
+        <v>0.0276757637049803</v>
+      </c>
+      <c r="F258" s="74" t="n">
+        <v>0.0135071830550466</v>
+      </c>
+      <c r="G258" s="0"/>
+      <c r="L258" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M258" s="0"/>
+    </row>
+    <row r="259" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B259" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C259" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D259" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E259" s="74" t="n">
+        <v>0.027770511232103</v>
+      </c>
+      <c r="F259" s="74" t="n">
+        <v>0.0136914905091539</v>
+      </c>
+      <c r="G259" s="0"/>
+      <c r="L259" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M259" s="0"/>
+    </row>
+    <row r="260" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B260" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C260" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D260" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E260" s="74" t="n">
+        <v>0.0277019951349735</v>
+      </c>
+      <c r="F260" s="74" t="n">
+        <v>0.0137131169687583</v>
+      </c>
+      <c r="G260" s="0"/>
+      <c r="L260" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M260" s="0"/>
+    </row>
+    <row r="261" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B261" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C261" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D261" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E261" s="74" t="n">
+        <v>0.0277553616674744</v>
+      </c>
+      <c r="F261" s="74" t="n">
+        <v>0.0145438559051414</v>
+      </c>
+      <c r="G261" s="0"/>
+      <c r="L261" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M261" s="0"/>
+    </row>
+    <row r="262" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B262" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C262" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D262" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E262" s="74" t="n">
+        <v>0.0278794815104737</v>
+      </c>
+      <c r="F262" s="74" t="n">
+        <v>0.0145086924098168</v>
+      </c>
+      <c r="G262" s="0"/>
+      <c r="L262" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M262" s="0"/>
+    </row>
+    <row r="263" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B263" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C263" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D263" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E263" s="74" t="n">
+        <v>0.0273790312592369</v>
+      </c>
+      <c r="F263" s="74" t="n">
+        <v>0.0128473896259296</v>
+      </c>
+      <c r="G263" s="0"/>
+      <c r="L263" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M263" s="0"/>
+    </row>
+    <row r="264" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B264" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C264" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D264" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E264" s="74" t="n">
+        <v>0.0296861445609495</v>
+      </c>
+      <c r="F264" s="74" t="n">
+        <v>0.0156678641775377</v>
+      </c>
+      <c r="G264" s="0"/>
+      <c r="L264" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M264" s="0"/>
+    </row>
+    <row r="265" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B265" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C265" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D265" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E265" s="74" t="n">
+        <v>0.0276937340335798</v>
+      </c>
+      <c r="F265" s="74" t="n">
+        <v>0.0136020486090205</v>
+      </c>
+      <c r="G265" s="0"/>
+      <c r="L265" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M265" s="0"/>
+    </row>
+    <row r="266" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B266" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C266" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D266" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="E266" s="74" t="n">
+        <v>0.0277606145767714</v>
+      </c>
+      <c r="F266" s="74" t="n">
+        <v>0.0145155320563741</v>
+      </c>
+      <c r="G266" s="0"/>
+      <c r="L266" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M266" s="0"/>
+    </row>
+    <row r="267" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B267" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C267" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D267" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E267" s="74" t="n">
+        <v>0.0277371586088751</v>
+      </c>
+      <c r="F267" s="74" t="n">
+        <v>0.0138159171622351</v>
+      </c>
+      <c r="G267" s="0"/>
+      <c r="L267" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M267" s="0"/>
+    </row>
+    <row r="268" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B268" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C268" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D268" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E268" s="74" t="n">
+        <v>0.0278287982505812</v>
+      </c>
+      <c r="F268" s="74" t="n">
+        <v>0.0186199659372583</v>
+      </c>
+      <c r="G268" s="0"/>
+      <c r="L268" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M268" s="0"/>
+    </row>
+    <row r="269" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B269" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C269" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D269" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E269" s="74" t="n">
+        <v>0.0277943996366322</v>
+      </c>
+      <c r="F269" s="74" t="n">
+        <v>0.0135326311566118</v>
+      </c>
+      <c r="G269" s="0"/>
+      <c r="L269" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M269" s="0"/>
+    </row>
+    <row r="270" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B270" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="C270" s="74" t="n">
+        <v>300</v>
+      </c>
+      <c r="D270" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E270" s="74" t="n">
+        <v>0.0278023212572681</v>
+      </c>
+      <c r="F270" s="74" t="n">
+        <v>0.0134712177900632</v>
+      </c>
+      <c r="G270" s="0"/>
+      <c r="L270" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M270" s="0"/>
+    </row>
+    <row r="271" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="74" t="n">
+        <v>15</v>
+      </c>
+      <c r="B271" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="C271" s="74" t="n">
+        <v>400</v>
+      </c>
+      <c r="D271" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E271" s="74" t="n">
+        <v>0.0276900660968758</v>
+      </c>
+      <c r="F271" s="74" t="n">
+        <v>0.0137985504603507</v>
+      </c>
+      <c r="G271" s="0"/>
+      <c r="L271" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M271" s="0"/>
+    </row>
+    <row r="272" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="74" t="n">
+        <v>5</v>
+      </c>
+      <c r="B272" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C272" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D272" s="74" t="n">
+        <v>500</v>
+      </c>
+      <c r="E272" s="74" t="n">
+        <v>0.0273089049360908</v>
+      </c>
+      <c r="F272" s="74" t="n">
+        <v>0.0125304374284825</v>
+      </c>
+      <c r="G272" s="0"/>
+      <c r="L272" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M272" s="0"/>
+    </row>
+    <row r="273" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="B273" s="74" t="n">
+        <v>10</v>
+      </c>
+      <c r="C273" s="74" t="n">
+        <v>200</v>
+      </c>
+      <c r="D273" s="74" t="n">
+        <v>600</v>
+      </c>
+      <c r="E273" s="74" t="n">
+        <v>0.0278153513650753</v>
+      </c>
+      <c r="F273" s="74" t="n">
+        <v>0.013506162062234</v>
+      </c>
+      <c r="G273" s="0"/>
+      <c r="L273" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="M273" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>